<commit_message>
Actualizacion Formato Americano abril
</commit_message>
<xml_diff>
--- a/pipelines/Data Engineering.xlsx
+++ b/pipelines/Data Engineering.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27932"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\saule\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\natus\Documents\Trabajo\PEDRO_PEREZ\Proyecto_Mercado_de_Valores\SP500_INDEX_Analisis\pipelines\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4B1E1AD-75BA-4672-97FF-B3E88ECDD09B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0600BF55-B38B-48F3-8922-83DBF1D47144}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{AF709C27-429E-478E-9AB0-B8CF25FE9941}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{AF709C27-429E-478E-9AB0-B8CF25FE9941}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1499" uniqueCount="635">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1500" uniqueCount="635">
   <si>
     <t>Variable</t>
   </si>
@@ -1866,9 +1866,6 @@
     <t>Formato numerico</t>
   </si>
   <si>
-    <t>Punto</t>
-  </si>
-  <si>
     <t>DD/MM/YY</t>
   </si>
   <si>
@@ -1876,9 +1873,6 @@
   </si>
   <si>
     <t>MM-DD-YY</t>
-  </si>
-  <si>
-    <t>Coma y Punto</t>
   </si>
   <si>
     <t>Percentage balance</t>
@@ -1955,6 +1949,12 @@
   </si>
   <si>
     <t>JOLTS</t>
+  </si>
+  <si>
+    <t>Americano</t>
+  </si>
+  <si>
+    <t>Americano (Coma y Punto)</t>
   </si>
 </sst>
 </file>
@@ -2528,8 +2528,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CB0844A-40A1-4264-8968-9E5B325C5351}">
   <dimension ref="A1:T89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="G78" sqref="G78:G79"/>
+    <sheetView tabSelected="1" topLeftCell="P13" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="T33" sqref="T33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="37.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2666,7 +2666,7 @@
         <v>603</v>
       </c>
       <c r="T2" s="3" t="s">
-        <v>605</v>
+        <v>633</v>
       </c>
     </row>
     <row r="3" spans="1:20" ht="100.8" x14ac:dyDescent="0.3">
@@ -2728,10 +2728,10 @@
         <v>603</v>
       </c>
       <c r="T3" s="3" t="s">
-        <v>605</v>
-      </c>
-    </row>
-    <row r="4" spans="1:20" ht="15" x14ac:dyDescent="0.3">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A4" s="12" t="s">
         <v>12</v>
       </c>
@@ -2781,13 +2781,13 @@
         <v>246</v>
       </c>
       <c r="S4" s="3" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="T4" s="3" t="s">
-        <v>605</v>
-      </c>
-    </row>
-    <row r="5" spans="1:20" ht="15" x14ac:dyDescent="0.3">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A5" s="12" t="s">
         <v>15</v>
       </c>
@@ -2837,10 +2837,10 @@
         <v>246</v>
       </c>
       <c r="S5" s="3" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="T5" s="3" t="s">
-        <v>605</v>
+        <v>633</v>
       </c>
     </row>
     <row r="6" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
@@ -2893,10 +2893,10 @@
         <v>246</v>
       </c>
       <c r="S6" s="3" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="T6" s="3" t="s">
-        <v>605</v>
+        <v>633</v>
       </c>
     </row>
     <row r="7" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
@@ -2949,10 +2949,10 @@
         <v>246</v>
       </c>
       <c r="S7" s="3" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="T7" s="3" t="s">
-        <v>605</v>
+        <v>633</v>
       </c>
     </row>
     <row r="8" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
@@ -3005,13 +3005,13 @@
         <v>246</v>
       </c>
       <c r="S8" s="3" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="T8" s="3" t="s">
-        <v>605</v>
-      </c>
-    </row>
-    <row r="9" spans="1:20" ht="15" x14ac:dyDescent="0.3">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A9" s="12" t="s">
         <v>23</v>
       </c>
@@ -3061,13 +3061,13 @@
         <v>246</v>
       </c>
       <c r="S9" s="3" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="T9" s="3" t="s">
-        <v>605</v>
-      </c>
-    </row>
-    <row r="10" spans="1:20" ht="15" x14ac:dyDescent="0.3">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A10" s="12" t="s">
         <v>25</v>
       </c>
@@ -3117,10 +3117,10 @@
         <v>246</v>
       </c>
       <c r="S10" s="3" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="T10" s="3" t="s">
-        <v>605</v>
+        <v>633</v>
       </c>
     </row>
     <row r="11" spans="1:20" ht="115.2" x14ac:dyDescent="0.3">
@@ -3181,8 +3181,8 @@
       <c r="S11" s="21" t="s">
         <v>603</v>
       </c>
-      <c r="T11" s="21" t="s">
-        <v>605</v>
+      <c r="T11" s="3" t="s">
+        <v>633</v>
       </c>
     </row>
     <row r="12" spans="1:20" ht="100.8" x14ac:dyDescent="0.3">
@@ -3243,8 +3243,8 @@
       <c r="S12" s="21" t="s">
         <v>603</v>
       </c>
-      <c r="T12" s="21" t="s">
-        <v>605</v>
+      <c r="T12" s="3" t="s">
+        <v>633</v>
       </c>
     </row>
     <row r="13" spans="1:20" ht="115.2" x14ac:dyDescent="0.3">
@@ -3305,8 +3305,8 @@
       <c r="S13" s="21" t="s">
         <v>603</v>
       </c>
-      <c r="T13" s="21" t="s">
-        <v>605</v>
+      <c r="T13" s="3" t="s">
+        <v>633</v>
       </c>
     </row>
     <row r="14" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
@@ -3359,13 +3359,13 @@
         <v>246</v>
       </c>
       <c r="S14" s="21" t="s">
-        <v>608</v>
-      </c>
-      <c r="T14" s="21" t="s">
-        <v>605</v>
-      </c>
-    </row>
-    <row r="15" spans="1:20" ht="15" x14ac:dyDescent="0.3">
+        <v>607</v>
+      </c>
+      <c r="T14" s="3" t="s">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A15" s="12" t="s">
         <v>187</v>
       </c>
@@ -3415,10 +3415,10 @@
         <v>246</v>
       </c>
       <c r="S15" s="21" t="s">
-        <v>608</v>
-      </c>
-      <c r="T15" s="21" t="s">
-        <v>605</v>
+        <v>607</v>
+      </c>
+      <c r="T15" s="3" t="s">
+        <v>633</v>
       </c>
     </row>
     <row r="16" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
@@ -3471,10 +3471,10 @@
         <v>246</v>
       </c>
       <c r="S16" s="21" t="s">
-        <v>608</v>
-      </c>
-      <c r="T16" s="21" t="s">
-        <v>605</v>
+        <v>607</v>
+      </c>
+      <c r="T16" s="3" t="s">
+        <v>633</v>
       </c>
     </row>
     <row r="17" spans="1:20" s="41" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -3494,7 +3494,7 @@
         <v>247</v>
       </c>
       <c r="F17" s="35" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
       <c r="G17" s="36"/>
       <c r="H17" s="37"/>
@@ -3527,11 +3527,11 @@
       <c r="S17" s="41" t="s">
         <v>603</v>
       </c>
-      <c r="T17" s="41" t="s">
-        <v>605</v>
-      </c>
-    </row>
-    <row r="18" spans="1:20" ht="15" x14ac:dyDescent="0.3">
+      <c r="T17" s="3" t="s">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A18" s="12" t="s">
         <v>194</v>
       </c>
@@ -3581,13 +3581,13 @@
         <v>246</v>
       </c>
       <c r="S18" s="32" t="s">
-        <v>608</v>
-      </c>
-      <c r="T18" t="s">
-        <v>605</v>
-      </c>
-    </row>
-    <row r="19" spans="1:20" s="30" customFormat="1" ht="15" x14ac:dyDescent="0.3">
+        <v>607</v>
+      </c>
+      <c r="T18" s="3" t="s">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A19" s="23" t="s">
         <v>248</v>
       </c>
@@ -3633,6 +3633,9 @@
       <c r="Q19" s="25" t="s">
         <v>367</v>
       </c>
+      <c r="T19" s="3" t="s">
+        <v>633</v>
+      </c>
     </row>
     <row r="20" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A20" s="12" t="s">
@@ -3681,13 +3684,13 @@
         <v>395</v>
       </c>
       <c r="R20" s="22" t="s">
+        <v>606</v>
+      </c>
+      <c r="S20" s="32" t="s">
         <v>607</v>
       </c>
-      <c r="S20" s="32" t="s">
-        <v>608</v>
-      </c>
-      <c r="T20" t="s">
-        <v>605</v>
+      <c r="T20" s="3" t="s">
+        <v>633</v>
       </c>
     </row>
     <row r="21" spans="1:20" ht="129.6" x14ac:dyDescent="0.3">
@@ -3739,13 +3742,13 @@
         <v>386</v>
       </c>
       <c r="R21" s="31" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="S21" s="32" t="s">
         <v>603</v>
       </c>
-      <c r="T21" s="32" t="s">
-        <v>605</v>
+      <c r="T21" s="3" t="s">
+        <v>633</v>
       </c>
     </row>
     <row r="22" spans="1:20" ht="129.6" x14ac:dyDescent="0.3">
@@ -3797,13 +3800,13 @@
         <v>401</v>
       </c>
       <c r="R22" s="31" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="S22" s="32" t="s">
         <v>603</v>
       </c>
-      <c r="T22" s="32" t="s">
-        <v>605</v>
+      <c r="T22" s="3" t="s">
+        <v>633</v>
       </c>
     </row>
     <row r="23" spans="1:20" ht="15" x14ac:dyDescent="0.3">
@@ -3849,13 +3852,13 @@
         <v>389</v>
       </c>
       <c r="R23" s="31" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="S23" s="32" t="s">
         <v>603</v>
       </c>
-      <c r="T23" s="32" t="s">
-        <v>605</v>
+      <c r="T23" s="3" t="s">
+        <v>633</v>
       </c>
     </row>
     <row r="24" spans="1:20" ht="15" x14ac:dyDescent="0.3">
@@ -3901,13 +3904,13 @@
         <v>398</v>
       </c>
       <c r="R24" s="31" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="S24" s="32" t="s">
         <v>603</v>
       </c>
-      <c r="T24" s="32" t="s">
-        <v>605</v>
+      <c r="T24" s="3" t="s">
+        <v>633</v>
       </c>
     </row>
     <row r="25" spans="1:20" ht="15" x14ac:dyDescent="0.3">
@@ -3953,13 +3956,13 @@
         <v>392</v>
       </c>
       <c r="R25" s="31" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="S25" s="32" t="s">
         <v>603</v>
       </c>
-      <c r="T25" s="32" t="s">
-        <v>605</v>
+      <c r="T25" s="3" t="s">
+        <v>633</v>
       </c>
     </row>
     <row r="26" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
@@ -4009,13 +4012,13 @@
         <v>405</v>
       </c>
       <c r="R26" s="31" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
       <c r="S26" s="32" t="s">
         <v>603</v>
       </c>
-      <c r="T26" s="32" t="s">
-        <v>605</v>
+      <c r="T26" s="3" t="s">
+        <v>633</v>
       </c>
     </row>
     <row r="27" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
@@ -4065,16 +4068,16 @@
         <v>411</v>
       </c>
       <c r="R27" s="31" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
       <c r="S27" s="32" t="s">
         <v>603</v>
       </c>
-      <c r="T27" s="32" t="s">
-        <v>605</v>
-      </c>
-    </row>
-    <row r="28" spans="1:20" ht="15" x14ac:dyDescent="0.3">
+      <c r="T27" s="3" t="s">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="28" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A28" s="12" t="s">
         <v>145</v>
       </c>
@@ -4121,13 +4124,13 @@
         <v>408</v>
       </c>
       <c r="R28" s="31" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
       <c r="S28" s="32" t="s">
         <v>603</v>
       </c>
-      <c r="T28" s="32" t="s">
-        <v>605</v>
+      <c r="T28" s="3" t="s">
+        <v>633</v>
       </c>
     </row>
     <row r="29" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
@@ -4180,13 +4183,13 @@
         <v>246</v>
       </c>
       <c r="S29" s="32" t="s">
-        <v>608</v>
-      </c>
-      <c r="T29" s="32" t="s">
-        <v>605</v>
-      </c>
-    </row>
-    <row r="30" spans="1:20" ht="15" x14ac:dyDescent="0.3">
+        <v>607</v>
+      </c>
+      <c r="T29" s="3" t="s">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="30" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A30" s="12" t="s">
         <v>60</v>
       </c>
@@ -4236,10 +4239,10 @@
         <v>246</v>
       </c>
       <c r="S30" s="32" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="T30" s="32" t="s">
-        <v>609</v>
+        <v>634</v>
       </c>
     </row>
     <row r="31" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
@@ -4292,13 +4295,13 @@
         <v>246</v>
       </c>
       <c r="S31" s="32" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="T31" s="32" t="s">
-        <v>605</v>
-      </c>
-    </row>
-    <row r="32" spans="1:20" ht="15" x14ac:dyDescent="0.3">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="32" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A32" s="12" t="s">
         <v>64</v>
       </c>
@@ -4348,10 +4351,10 @@
         <v>246</v>
       </c>
       <c r="S32" s="32" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="T32" s="32" t="s">
-        <v>605</v>
+        <v>633</v>
       </c>
     </row>
     <row r="33" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
@@ -4404,10 +4407,10 @@
         <v>246</v>
       </c>
       <c r="S33" s="32" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="T33" s="32" t="s">
-        <v>605</v>
+        <v>633</v>
       </c>
     </row>
     <row r="34" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
@@ -4460,13 +4463,13 @@
         <v>246</v>
       </c>
       <c r="S34" s="32" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="T34" s="32" t="s">
-        <v>605</v>
-      </c>
-    </row>
-    <row r="35" spans="1:20" ht="15" x14ac:dyDescent="0.3">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="35" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A35" s="12" t="s">
         <v>267</v>
       </c>
@@ -4513,13 +4516,13 @@
         <v>431</v>
       </c>
       <c r="R35" s="33" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
       <c r="S35" s="32" t="s">
         <v>603</v>
       </c>
       <c r="T35" s="32" t="s">
-        <v>605</v>
+        <v>633</v>
       </c>
     </row>
     <row r="36" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
@@ -4536,7 +4539,7 @@
         <v>225</v>
       </c>
       <c r="E36" s="24" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="F36" s="10" t="s">
         <v>246</v>
@@ -4569,13 +4572,13 @@
         <v>440</v>
       </c>
       <c r="R36" s="33" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
       <c r="S36" s="32" t="s">
         <v>603</v>
       </c>
       <c r="T36" s="32" t="s">
-        <v>605</v>
+        <v>633</v>
       </c>
     </row>
     <row r="37" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
@@ -4625,13 +4628,13 @@
         <v>434</v>
       </c>
       <c r="R37" s="31" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="S37" s="32" t="s">
         <v>603</v>
       </c>
       <c r="T37" s="32" t="s">
-        <v>605</v>
+        <v>633</v>
       </c>
     </row>
     <row r="38" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
@@ -4677,10 +4680,10 @@
         <v>428</v>
       </c>
       <c r="S38" s="32" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="T38" s="32" t="s">
-        <v>605</v>
+        <v>633</v>
       </c>
     </row>
     <row r="39" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
@@ -4726,13 +4729,13 @@
         <v>437</v>
       </c>
       <c r="S39" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="T39" s="32" t="s">
-        <v>605</v>
-      </c>
-    </row>
-    <row r="40" spans="1:20" ht="15" x14ac:dyDescent="0.3">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="40" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A40" s="12" t="s">
         <v>68</v>
       </c>
@@ -4779,16 +4782,16 @@
         <v>489</v>
       </c>
       <c r="R40" s="21" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="S40" s="21" t="s">
         <v>603</v>
       </c>
       <c r="T40" s="32" t="s">
-        <v>605</v>
-      </c>
-    </row>
-    <row r="41" spans="1:20" ht="15" x14ac:dyDescent="0.3">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="41" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A41" s="12" t="s">
         <v>72</v>
       </c>
@@ -4835,16 +4838,16 @@
         <v>483</v>
       </c>
       <c r="R41" s="33" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="S41" s="21" t="s">
         <v>603</v>
       </c>
       <c r="T41" s="32" t="s">
-        <v>605</v>
-      </c>
-    </row>
-    <row r="42" spans="1:20" ht="15" x14ac:dyDescent="0.3">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="42" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A42" s="12" t="s">
         <v>75</v>
       </c>
@@ -4891,13 +4894,13 @@
         <v>504</v>
       </c>
       <c r="R42" s="32" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
       <c r="S42" s="21" t="s">
         <v>603</v>
       </c>
       <c r="T42" s="32" t="s">
-        <v>605</v>
+        <v>633</v>
       </c>
     </row>
     <row r="43" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
@@ -4947,16 +4950,16 @@
         <v>486</v>
       </c>
       <c r="R43" s="33" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
       <c r="S43" s="21" t="s">
         <v>603</v>
       </c>
       <c r="T43" s="32" t="s">
-        <v>605</v>
-      </c>
-    </row>
-    <row r="44" spans="1:20" ht="15" x14ac:dyDescent="0.3">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="44" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A44" s="12" t="s">
         <v>81</v>
       </c>
@@ -5003,13 +5006,13 @@
         <v>507</v>
       </c>
       <c r="R44" s="32" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="S44" s="21" t="s">
         <v>603</v>
       </c>
       <c r="T44" s="32" t="s">
-        <v>605</v>
+        <v>633</v>
       </c>
     </row>
     <row r="45" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
@@ -5062,10 +5065,10 @@
         <v>246</v>
       </c>
       <c r="S45" s="21" t="s">
-        <v>608</v>
-      </c>
-      <c r="T45" t="s">
-        <v>605</v>
+        <v>607</v>
+      </c>
+      <c r="T45" s="32" t="s">
+        <v>633</v>
       </c>
     </row>
     <row r="46" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
@@ -5118,10 +5121,10 @@
         <v>602</v>
       </c>
       <c r="S46" s="21" t="s">
-        <v>621</v>
-      </c>
-      <c r="T46" s="21" t="s">
-        <v>605</v>
+        <v>619</v>
+      </c>
+      <c r="T46" s="32" t="s">
+        <v>633</v>
       </c>
     </row>
     <row r="47" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
@@ -5174,10 +5177,10 @@
         <v>602</v>
       </c>
       <c r="S47" s="21" t="s">
-        <v>621</v>
-      </c>
-      <c r="T47" s="21" t="s">
-        <v>605</v>
+        <v>619</v>
+      </c>
+      <c r="T47" s="32" t="s">
+        <v>633</v>
       </c>
     </row>
     <row r="48" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
@@ -5230,10 +5233,10 @@
         <v>602</v>
       </c>
       <c r="S48" s="21" t="s">
-        <v>621</v>
-      </c>
-      <c r="T48" s="21" t="s">
-        <v>605</v>
+        <v>619</v>
+      </c>
+      <c r="T48" s="32" t="s">
+        <v>633</v>
       </c>
     </row>
     <row r="49" spans="1:20" x14ac:dyDescent="0.3">
@@ -5288,8 +5291,8 @@
       <c r="S49" s="32" t="s">
         <v>603</v>
       </c>
-      <c r="T49" s="21" t="s">
-        <v>605</v>
+      <c r="T49" s="32" t="s">
+        <v>633</v>
       </c>
     </row>
     <row r="50" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
@@ -5342,10 +5345,10 @@
         <v>602</v>
       </c>
       <c r="S50" s="21" t="s">
-        <v>621</v>
-      </c>
-      <c r="T50" s="21" t="s">
-        <v>605</v>
+        <v>619</v>
+      </c>
+      <c r="T50" s="32" t="s">
+        <v>633</v>
       </c>
     </row>
     <row r="51" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
@@ -5400,8 +5403,8 @@
       <c r="S51" s="32" t="s">
         <v>603</v>
       </c>
-      <c r="T51" s="21" t="s">
-        <v>605</v>
+      <c r="T51" s="32" t="s">
+        <v>633</v>
       </c>
     </row>
     <row r="52" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
@@ -5418,7 +5421,7 @@
         <v>225</v>
       </c>
       <c r="E52" s="10" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="F52" s="10" t="s">
         <v>246</v>
@@ -5456,8 +5459,8 @@
       <c r="S52" s="32" t="s">
         <v>603</v>
       </c>
-      <c r="T52" s="21" t="s">
-        <v>605</v>
+      <c r="T52" s="32" t="s">
+        <v>633</v>
       </c>
     </row>
     <row r="53" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
@@ -5512,11 +5515,11 @@
       <c r="S53" s="32" t="s">
         <v>603</v>
       </c>
-      <c r="T53" s="21" t="s">
-        <v>605</v>
-      </c>
-    </row>
-    <row r="54" spans="1:20" ht="15" x14ac:dyDescent="0.3">
+      <c r="T53" s="32" t="s">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="54" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A54" s="12" t="s">
         <v>102</v>
       </c>
@@ -5568,8 +5571,8 @@
       <c r="S54" s="32" t="s">
         <v>603</v>
       </c>
-      <c r="T54" s="21" t="s">
-        <v>605</v>
+      <c r="T54" s="32" t="s">
+        <v>633</v>
       </c>
     </row>
     <row r="55" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
@@ -5624,8 +5627,8 @@
       <c r="S55" s="32" t="s">
         <v>603</v>
       </c>
-      <c r="T55" s="21" t="s">
-        <v>605</v>
+      <c r="T55" s="32" t="s">
+        <v>633</v>
       </c>
     </row>
     <row r="56" spans="1:20" ht="15" x14ac:dyDescent="0.3">
@@ -5680,11 +5683,11 @@
       <c r="S56" s="32" t="s">
         <v>603</v>
       </c>
-      <c r="T56" s="21" t="s">
-        <v>605</v>
-      </c>
-    </row>
-    <row r="57" spans="1:20" ht="30" x14ac:dyDescent="0.3">
+      <c r="T56" s="32" t="s">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="57" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A57" s="12" t="s">
         <v>162</v>
       </c>
@@ -5736,8 +5739,8 @@
       <c r="S57" s="32" t="s">
         <v>603</v>
       </c>
-      <c r="T57" s="21" t="s">
-        <v>605</v>
+      <c r="T57" s="32" t="s">
+        <v>633</v>
       </c>
     </row>
     <row r="58" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
@@ -5790,10 +5793,10 @@
         <v>602</v>
       </c>
       <c r="S58" s="32" t="s">
-        <v>608</v>
-      </c>
-      <c r="T58" s="21" t="s">
-        <v>605</v>
+        <v>607</v>
+      </c>
+      <c r="T58" s="32" t="s">
+        <v>633</v>
       </c>
     </row>
     <row r="59" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
@@ -5848,8 +5851,8 @@
       <c r="S59" s="32" t="s">
         <v>603</v>
       </c>
-      <c r="T59" s="21" t="s">
-        <v>605</v>
+      <c r="T59" s="32" t="s">
+        <v>633</v>
       </c>
     </row>
     <row r="60" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
@@ -5902,13 +5905,13 @@
         <v>602</v>
       </c>
       <c r="S60" s="32" t="s">
-        <v>608</v>
-      </c>
-      <c r="T60" s="21" t="s">
-        <v>605</v>
-      </c>
-    </row>
-    <row r="61" spans="1:20" ht="15" x14ac:dyDescent="0.3">
+        <v>607</v>
+      </c>
+      <c r="T60" s="32" t="s">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="61" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A61" s="12" t="s">
         <v>36</v>
       </c>
@@ -5958,13 +5961,13 @@
         <v>246</v>
       </c>
       <c r="S61" s="32" t="s">
-        <v>608</v>
-      </c>
-      <c r="T61" s="21" t="s">
-        <v>605</v>
-      </c>
-    </row>
-    <row r="62" spans="1:20" ht="15" x14ac:dyDescent="0.3">
+        <v>607</v>
+      </c>
+      <c r="T61" s="32" t="s">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="62" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A62" s="12" t="s">
         <v>39</v>
       </c>
@@ -6014,13 +6017,13 @@
         <v>246</v>
       </c>
       <c r="S62" s="32" t="s">
-        <v>608</v>
-      </c>
-      <c r="T62" s="21" t="s">
-        <v>605</v>
-      </c>
-    </row>
-    <row r="63" spans="1:20" ht="15" x14ac:dyDescent="0.3">
+        <v>607</v>
+      </c>
+      <c r="T62" s="32" t="s">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="63" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A63" s="12" t="s">
         <v>41</v>
       </c>
@@ -6070,13 +6073,13 @@
         <v>246</v>
       </c>
       <c r="S63" s="32" t="s">
-        <v>608</v>
-      </c>
-      <c r="T63" s="21" t="s">
-        <v>605</v>
-      </c>
-    </row>
-    <row r="64" spans="1:20" ht="15" x14ac:dyDescent="0.3">
+        <v>607</v>
+      </c>
+      <c r="T63" s="32" t="s">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="64" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A64" s="12" t="s">
         <v>43</v>
       </c>
@@ -6126,13 +6129,13 @@
         <v>246</v>
       </c>
       <c r="S64" s="32" t="s">
-        <v>608</v>
-      </c>
-      <c r="T64" s="21" t="s">
-        <v>605</v>
-      </c>
-    </row>
-    <row r="65" spans="1:20" ht="15" x14ac:dyDescent="0.3">
+        <v>607</v>
+      </c>
+      <c r="T64" s="32" t="s">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="65" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A65" s="12" t="s">
         <v>45</v>
       </c>
@@ -6182,13 +6185,13 @@
         <v>246</v>
       </c>
       <c r="S65" s="32" t="s">
-        <v>608</v>
-      </c>
-      <c r="T65" s="21" t="s">
-        <v>605</v>
-      </c>
-    </row>
-    <row r="66" spans="1:20" ht="15" x14ac:dyDescent="0.3">
+        <v>607</v>
+      </c>
+      <c r="T65" s="32" t="s">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="66" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A66" s="12" t="s">
         <v>47</v>
       </c>
@@ -6238,13 +6241,13 @@
         <v>246</v>
       </c>
       <c r="S66" s="32" t="s">
-        <v>608</v>
-      </c>
-      <c r="T66" s="21" t="s">
-        <v>605</v>
-      </c>
-    </row>
-    <row r="67" spans="1:20" ht="15" x14ac:dyDescent="0.3">
+        <v>607</v>
+      </c>
+      <c r="T66" s="32" t="s">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="67" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A67" s="12" t="s">
         <v>49</v>
       </c>
@@ -6294,10 +6297,10 @@
         <v>246</v>
       </c>
       <c r="S67" s="32" t="s">
-        <v>608</v>
-      </c>
-      <c r="T67" s="21" t="s">
-        <v>605</v>
+        <v>607</v>
+      </c>
+      <c r="T67" s="32" t="s">
+        <v>633</v>
       </c>
     </row>
     <row r="68" spans="1:20" ht="15" x14ac:dyDescent="0.3">
@@ -6350,10 +6353,10 @@
         <v>246</v>
       </c>
       <c r="S68" s="32" t="s">
-        <v>608</v>
-      </c>
-      <c r="T68" s="21" t="s">
-        <v>605</v>
+        <v>607</v>
+      </c>
+      <c r="T68" s="32" t="s">
+        <v>633</v>
       </c>
     </row>
     <row r="69" spans="1:20" ht="15" x14ac:dyDescent="0.3">
@@ -6406,10 +6409,10 @@
         <v>602</v>
       </c>
       <c r="S69" s="32" t="s">
-        <v>621</v>
-      </c>
-      <c r="T69" s="21" t="s">
-        <v>605</v>
+        <v>619</v>
+      </c>
+      <c r="T69" s="32" t="s">
+        <v>633</v>
       </c>
     </row>
     <row r="70" spans="1:20" ht="15" x14ac:dyDescent="0.3">
@@ -6459,16 +6462,16 @@
         <v>539</v>
       </c>
       <c r="R70" s="31" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
       <c r="S70" s="32" t="s">
-        <v>621</v>
-      </c>
-      <c r="T70" s="21" t="s">
-        <v>605</v>
-      </c>
-    </row>
-    <row r="71" spans="1:20" ht="15" x14ac:dyDescent="0.3">
+        <v>619</v>
+      </c>
+      <c r="T70" s="32" t="s">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="71" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A71" s="12" t="s">
         <v>51</v>
       </c>
@@ -6488,7 +6491,7 @@
         <v>246</v>
       </c>
       <c r="G71" s="13" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
       <c r="H71" s="16"/>
       <c r="I71" s="16"/>
@@ -6515,16 +6518,16 @@
         <v>546</v>
       </c>
       <c r="R71" s="33" t="s">
-        <v>622</v>
+        <v>620</v>
       </c>
       <c r="S71" s="32" t="s">
         <v>603</v>
       </c>
-      <c r="T71" s="21" t="s">
-        <v>605</v>
-      </c>
-    </row>
-    <row r="72" spans="1:20" ht="15" x14ac:dyDescent="0.3">
+      <c r="T71" s="32" t="s">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="72" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A72" s="12" t="s">
         <v>168</v>
       </c>
@@ -6553,7 +6556,7 @@
         <v>169</v>
       </c>
       <c r="L72" s="5" t="s">
-        <v>624</v>
+        <v>622</v>
       </c>
       <c r="M72" s="6" t="s">
         <v>170</v>
@@ -6574,13 +6577,13 @@
         <v>246</v>
       </c>
       <c r="S72" s="32" t="s">
-        <v>629</v>
-      </c>
-      <c r="T72" s="21" t="s">
-        <v>605</v>
-      </c>
-    </row>
-    <row r="73" spans="1:20" ht="15" x14ac:dyDescent="0.3">
+        <v>627</v>
+      </c>
+      <c r="T72" s="32" t="s">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="73" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A73" s="12" t="s">
         <v>171</v>
       </c>
@@ -6609,7 +6612,7 @@
         <v>172</v>
       </c>
       <c r="L73" s="5" t="s">
-        <v>625</v>
+        <v>623</v>
       </c>
       <c r="M73" s="6" t="s">
         <v>170</v>
@@ -6630,13 +6633,13 @@
         <v>246</v>
       </c>
       <c r="S73" s="32" t="s">
-        <v>629</v>
-      </c>
-      <c r="T73" s="21" t="s">
-        <v>605</v>
-      </c>
-    </row>
-    <row r="74" spans="1:20" ht="15" x14ac:dyDescent="0.3">
+        <v>627</v>
+      </c>
+      <c r="T73" s="32" t="s">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="74" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A74" s="12" t="s">
         <v>173</v>
       </c>
@@ -6665,7 +6668,7 @@
         <v>174</v>
       </c>
       <c r="L74" s="5" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
       <c r="M74" s="6" t="s">
         <v>170</v>
@@ -6686,13 +6689,13 @@
         <v>246</v>
       </c>
       <c r="S74" s="32" t="s">
-        <v>629</v>
-      </c>
-      <c r="T74" s="21" t="s">
-        <v>605</v>
-      </c>
-    </row>
-    <row r="75" spans="1:20" ht="15" x14ac:dyDescent="0.3">
+        <v>627</v>
+      </c>
+      <c r="T74" s="32" t="s">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="75" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A75" s="12" t="s">
         <v>175</v>
       </c>
@@ -6742,13 +6745,13 @@
         <v>246</v>
       </c>
       <c r="S75" s="32" t="s">
-        <v>629</v>
-      </c>
-      <c r="T75" s="21" t="s">
-        <v>605</v>
-      </c>
-    </row>
-    <row r="76" spans="1:20" ht="15" x14ac:dyDescent="0.3">
+        <v>627</v>
+      </c>
+      <c r="T75" s="32" t="s">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="76" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A76" s="12" t="s">
         <v>177</v>
       </c>
@@ -6777,7 +6780,7 @@
         <v>178</v>
       </c>
       <c r="L76" s="5" t="s">
-        <v>627</v>
+        <v>625</v>
       </c>
       <c r="M76" s="6" t="s">
         <v>170</v>
@@ -6798,13 +6801,13 @@
         <v>246</v>
       </c>
       <c r="S76" s="32" t="s">
-        <v>629</v>
-      </c>
-      <c r="T76" s="21" t="s">
-        <v>605</v>
-      </c>
-    </row>
-    <row r="77" spans="1:20" ht="15" x14ac:dyDescent="0.3">
+        <v>627</v>
+      </c>
+      <c r="T76" s="32" t="s">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="77" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A77" s="12" t="s">
         <v>179</v>
       </c>
@@ -6833,7 +6836,7 @@
         <v>180</v>
       </c>
       <c r="L77" s="5" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
       <c r="M77" s="6" t="s">
         <v>170</v>
@@ -6854,13 +6857,13 @@
         <v>246</v>
       </c>
       <c r="S77" s="32" t="s">
-        <v>629</v>
-      </c>
-      <c r="T77" s="21" t="s">
-        <v>605</v>
-      </c>
-    </row>
-    <row r="78" spans="1:20" ht="15" x14ac:dyDescent="0.3">
+        <v>627</v>
+      </c>
+      <c r="T77" s="32" t="s">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="78" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A78" s="12" t="s">
         <v>181</v>
       </c>
@@ -6910,13 +6913,13 @@
         <v>246</v>
       </c>
       <c r="S78" s="32" t="s">
-        <v>629</v>
-      </c>
-      <c r="T78" s="21" t="s">
-        <v>605</v>
-      </c>
-    </row>
-    <row r="79" spans="1:20" ht="15" x14ac:dyDescent="0.3">
+        <v>627</v>
+      </c>
+      <c r="T78" s="32" t="s">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="79" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A79" s="12" t="s">
         <v>183</v>
       </c>
@@ -6945,7 +6948,7 @@
         <v>184</v>
       </c>
       <c r="L79" s="5" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
       <c r="M79" s="6" t="s">
         <v>170</v>
@@ -6966,10 +6969,10 @@
         <v>246</v>
       </c>
       <c r="S79" s="32" t="s">
-        <v>629</v>
-      </c>
-      <c r="T79" s="21" t="s">
-        <v>605</v>
+        <v>627</v>
+      </c>
+      <c r="T79" s="32" t="s">
+        <v>633</v>
       </c>
     </row>
     <row r="80" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
@@ -7022,10 +7025,10 @@
         <v>602</v>
       </c>
       <c r="S80" s="21" t="s">
-        <v>608</v>
-      </c>
-      <c r="T80" s="21" t="s">
-        <v>605</v>
+        <v>607</v>
+      </c>
+      <c r="T80" s="32" t="s">
+        <v>633</v>
       </c>
     </row>
     <row r="81" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
@@ -7078,13 +7081,13 @@
         <v>246</v>
       </c>
       <c r="S81" s="32" t="s">
-        <v>629</v>
-      </c>
-      <c r="T81" s="21" t="s">
-        <v>605</v>
-      </c>
-    </row>
-    <row r="82" spans="1:20" ht="30" x14ac:dyDescent="0.3">
+        <v>627</v>
+      </c>
+      <c r="T81" s="32" t="s">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="82" spans="1:20" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A82" s="12" t="s">
         <v>196</v>
       </c>
@@ -7134,13 +7137,13 @@
         <v>246</v>
       </c>
       <c r="S82" s="32" t="s">
-        <v>621</v>
-      </c>
-      <c r="T82" s="21" t="s">
-        <v>605</v>
-      </c>
-    </row>
-    <row r="83" spans="1:20" ht="15" x14ac:dyDescent="0.3">
+        <v>619</v>
+      </c>
+      <c r="T82" s="32" t="s">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="83" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A83" s="12" t="s">
         <v>197</v>
       </c>
@@ -7190,13 +7193,13 @@
         <v>246</v>
       </c>
       <c r="S83" s="32" t="s">
-        <v>621</v>
-      </c>
-      <c r="T83" s="21" t="s">
-        <v>605</v>
-      </c>
-    </row>
-    <row r="84" spans="1:20" ht="15" x14ac:dyDescent="0.3">
+        <v>619</v>
+      </c>
+      <c r="T83" s="32" t="s">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="84" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A84" s="12" t="s">
         <v>108</v>
       </c>
@@ -7216,7 +7219,7 @@
         <v>246</v>
       </c>
       <c r="G84" s="3" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
       <c r="H84" s="16"/>
       <c r="I84" s="16"/>
@@ -7248,11 +7251,11 @@
       <c r="S84" s="32" t="s">
         <v>603</v>
       </c>
-      <c r="T84" s="21" t="s">
-        <v>605</v>
-      </c>
-    </row>
-    <row r="85" spans="1:20" ht="15" x14ac:dyDescent="0.3">
+      <c r="T84" s="32" t="s">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="85" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A85" s="12" t="s">
         <v>112</v>
       </c>
@@ -7272,7 +7275,7 @@
         <v>246</v>
       </c>
       <c r="G85" s="3" t="s">
-        <v>632</v>
+        <v>630</v>
       </c>
       <c r="H85" s="16"/>
       <c r="I85" s="16"/>
@@ -7304,8 +7307,8 @@
       <c r="S85" s="32" t="s">
         <v>603</v>
       </c>
-      <c r="T85" s="21" t="s">
-        <v>605</v>
+      <c r="T85" s="32" t="s">
+        <v>633</v>
       </c>
     </row>
     <row r="86" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
@@ -7328,7 +7331,7 @@
         <v>246</v>
       </c>
       <c r="G86" s="3" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
       <c r="H86" s="16"/>
       <c r="I86" s="16"/>
@@ -7360,11 +7363,11 @@
       <c r="S86" s="32" t="s">
         <v>603</v>
       </c>
-      <c r="T86" s="21" t="s">
-        <v>605</v>
-      </c>
-    </row>
-    <row r="87" spans="1:20" ht="15" x14ac:dyDescent="0.3">
+      <c r="T86" s="32" t="s">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="87" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A87" s="12" t="s">
         <v>118</v>
       </c>
@@ -7384,7 +7387,7 @@
         <v>246</v>
       </c>
       <c r="G87" s="3" t="s">
-        <v>634</v>
+        <v>632</v>
       </c>
       <c r="H87" s="16"/>
       <c r="I87" s="16"/>
@@ -7416,11 +7419,11 @@
       <c r="S87" s="32" t="s">
         <v>603</v>
       </c>
-      <c r="T87" s="21" t="s">
-        <v>605</v>
-      </c>
-    </row>
-    <row r="88" spans="1:20" ht="30" x14ac:dyDescent="0.3">
+      <c r="T87" s="32" t="s">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="88" spans="1:20" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A88" s="12" t="s">
         <v>121</v>
       </c>
@@ -7470,13 +7473,13 @@
         <v>602</v>
       </c>
       <c r="S88" s="32" t="s">
-        <v>608</v>
-      </c>
-      <c r="T88" s="21" t="s">
-        <v>605</v>
-      </c>
-    </row>
-    <row r="89" spans="1:20" ht="30" x14ac:dyDescent="0.3">
+        <v>607</v>
+      </c>
+      <c r="T88" s="32" t="s">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="89" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A89" s="12" t="s">
         <v>123</v>
       </c>
@@ -7526,10 +7529,10 @@
         <v>602</v>
       </c>
       <c r="S89" s="32" t="s">
-        <v>608</v>
-      </c>
-      <c r="T89" s="21" t="s">
-        <v>605</v>
+        <v>607</v>
+      </c>
+      <c r="T89" s="32" t="s">
+        <v>633</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Se agregaron 5 nuevos mercados en Commodities
</commit_message>
<xml_diff>
--- a/pipelines/Data Engineering.xlsx
+++ b/pipelines/Data Engineering.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27932"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\natus\Documents\Trabajo\PEDRO_PEREZ\Proyecto_Mercado_de_Valores\SP500_INDEX_Analisis\pipelines\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\saule\Desktop\Pipeline\Mayo3\SP500_INDEX_Analisis\pipelines\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0600BF55-B38B-48F3-8922-83DBF1D47144}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C56295EA-DBB2-4711-B4E6-40817E32ECCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{AF709C27-429E-478E-9AB0-B8CF25FE9941}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1500" uniqueCount="635">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1596" uniqueCount="670">
   <si>
     <t>Variable</t>
   </si>
@@ -1431,15 +1431,6 @@
     <t>/mnt/c/Users/pedro/OneDrive/Documents/ALGO TRADING/SP500 INDEX/Data/Macro/raw/economics/Fed_Balance_Sheet.csv</t>
   </si>
   <si>
-    <t>Data/Macro/raw/economics/Japan_M2_MoneySupply_YoY.xlsx</t>
-  </si>
-  <si>
-    <t>C:\Users\pedro\OneDrive\Documents\ALGO TRADING\SP500 INDEX\Data\Macro\raw\economics\Japan_M2_MoneySupply_YoY.xlsx</t>
-  </si>
-  <si>
-    <t>/mnt/c/Users/pedro/OneDrive/Documents/ALGO TRADING/SP500 INDEX/Data/Macro/raw/economics/Japan_M2_MoneySupply_YoY.xlsx</t>
-  </si>
-  <si>
     <t>Data/Macro/raw/economics/Mexico_CPI_MoM.xlsx</t>
   </si>
   <si>
@@ -1955,6 +1946,120 @@
   </si>
   <si>
     <t>Americano (Coma y Punto)</t>
+  </si>
+  <si>
+    <t>Data/Macro/raw/economics/Japan_M2_MoneySupply_YoY.csv</t>
+  </si>
+  <si>
+    <t>C:\Users\pedro\OneDrive\Documents\ALGO TRADING\SP500 INDEX\Data\Macro\raw\economics\Japan_M2_MoneySupply_YoY.csv</t>
+  </si>
+  <si>
+    <t>/mnt/c/Users/pedro/OneDrive/Documents/ALGO TRADING/SP500 INDEX/Data/Macro/raw/economics/Japan_M2_MoneySupply_YoY.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.investing.com/commodities/aluminum-historical-data </t>
+  </si>
+  <si>
+    <t>Aluminium_Spot</t>
+  </si>
+  <si>
+    <t>Data/Macro/raw/commodities/Aluminium_Spot.csv</t>
+  </si>
+  <si>
+    <t>C:\Users\pedro\OneDrive\Documents\ALGO TRADING\SP500 INDEX\Data/Macro/raw/commodities/Aluminium_Spot.csv</t>
+  </si>
+  <si>
+    <t>/mnt/c/Users/pedro/OneDrive/Documents/ALGO TRADING/SP500 INDEX/Data/Macro/raw/commodities/Aluminium_Spot.csv</t>
+  </si>
+  <si>
+    <t>Lead_Futures</t>
+  </si>
+  <si>
+    <t>https://www.investing.com/commodities/lead-historical-data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.investing.com/commodities/lead-historical-data </t>
+  </si>
+  <si>
+    <t>Data/Macro/raw/commodities/Lead_Futures.csv</t>
+  </si>
+  <si>
+    <t>C:\Users\pedro\OneDrive\Documents\ALGO TRADING\SP500 INDEX\Data/Macro/raw/commodities/Lead_Futures.csv</t>
+  </si>
+  <si>
+    <t>/mnt/c/Users/pedro/OneDrive/Documents/ALGO TRADING/SP500 INDEX/Data/Macro/raw/commodities/Lead_Futures.csv</t>
+  </si>
+  <si>
+    <t>Palladium_Futures</t>
+  </si>
+  <si>
+    <t>https://www.investing.com/commodities/palladium-historical-data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.investing.com/commodities/palladium-historical-data </t>
+  </si>
+  <si>
+    <t>Data/Macro/raw/commodities/Palladium_Futures.csv</t>
+  </si>
+  <si>
+    <t>C:\Users\pedro\OneDrive\Documents\ALGO TRADING\SP500 INDEX\Data/Macro/raw/commodities/Palladium_Futures.csv</t>
+  </si>
+  <si>
+    <t>/mnt/c/Users/pedro/OneDrive/Documents/ALGO TRADING/SP500 INDEX/Data/Macro/raw/commodities/Palladium_Futures.csv</t>
+  </si>
+  <si>
+    <t>Tin_Futures</t>
+  </si>
+  <si>
+    <t>https://www.investing.com/commodities/tin-historical-data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.investing.com/commodities/tin-historical-data </t>
+  </si>
+  <si>
+    <t>Data/Macro/raw/commodities/Tin_Futures.csv</t>
+  </si>
+  <si>
+    <t>C:\Users\pedro\OneDrive\Documents\ALGO TRADING\SP500 INDEX\Data/Macro/raw/commodities/Tin_Futures.csv</t>
+  </si>
+  <si>
+    <t>/mnt/c/Users/pedro/OneDrive/Documents/ALGO TRADING/SP500 INDEX/Data/Macro/raw/commodities/Tin_Futures.csv</t>
+  </si>
+  <si>
+    <t>Zinc_Futures</t>
+  </si>
+  <si>
+    <t>https://www.investing.com/commodities/zinc-futures-historical-data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.investing.com/commodities/zinc-futures-historical-data </t>
+  </si>
+  <si>
+    <t>Data/Macro/raw/commodities/Zinc_Futures.csv</t>
+  </si>
+  <si>
+    <t>C:\Users\pedro\OneDrive\Documents\ALGO TRADING\SP500 INDEX\Data/Macro/raw/commodities/Zinc_Futures.csv</t>
+  </si>
+  <si>
+    <t>/mnt/c/Users/pedro/OneDrive/Documents/ALGO TRADING/SP500 INDEX/Data/Macro/raw/commodities/Zinc_Futures.csv</t>
+  </si>
+  <si>
+    <t>Nickel_Futures</t>
+  </si>
+  <si>
+    <t>https://www.investing.com/commodities/nickel-historical-data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.investing.com/commodities/nickel-historical-data </t>
+  </si>
+  <si>
+    <t>Data/Macro/raw/commodities/Nickel_Futures.csv</t>
+  </si>
+  <si>
+    <t>C:\Users\pedro\OneDrive\Documents\ALGO TRADING\SP500 INDEX\Data/Macro/raw/commodities/Nickel_Futures.csv</t>
+  </si>
+  <si>
+    <t>/mnt/c/Users/pedro/OneDrive/Documents/ALGO TRADING/SP500 INDEX/Data/Macro/raw/commodities/Nickel_Futures.csv</t>
   </si>
 </sst>
 </file>
@@ -2190,7 +2295,7 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -2526,10 +2631,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CB0844A-40A1-4264-8968-9E5B325C5351}">
-  <dimension ref="A1:T89"/>
+  <dimension ref="A1:T95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P13" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="T33" sqref="T33"/>
+    <sheetView tabSelected="1" topLeftCell="A67" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A96" sqref="A96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="37.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2540,6 +2645,7 @@
     <col min="5" max="5" width="37.5546875" style="11" customWidth="1"/>
     <col min="6" max="11" width="37.5546875" customWidth="1"/>
     <col min="12" max="12" width="68.77734375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="62.77734375" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="68.33203125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="126.88671875" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="130.77734375" bestFit="1" customWidth="1"/>
@@ -2598,13 +2704,13 @@
         <v>326</v>
       </c>
       <c r="R1" s="20" t="s">
-        <v>600</v>
+        <v>597</v>
       </c>
       <c r="S1" s="20" t="s">
+        <v>598</v>
+      </c>
+      <c r="T1" s="20" t="s">
         <v>601</v>
-      </c>
-      <c r="T1" s="20" t="s">
-        <v>604</v>
       </c>
     </row>
     <row r="2" spans="1:20" ht="100.8" x14ac:dyDescent="0.3">
@@ -2660,13 +2766,13 @@
         <v>360</v>
       </c>
       <c r="R2" s="3" t="s">
-        <v>602</v>
+        <v>599</v>
       </c>
       <c r="S2" s="3" t="s">
-        <v>603</v>
+        <v>600</v>
       </c>
       <c r="T2" s="3" t="s">
-        <v>633</v>
+        <v>630</v>
       </c>
     </row>
     <row r="3" spans="1:20" ht="100.8" x14ac:dyDescent="0.3">
@@ -2722,16 +2828,16 @@
         <v>363</v>
       </c>
       <c r="R3" s="3" t="s">
-        <v>602</v>
+        <v>599</v>
       </c>
       <c r="S3" s="3" t="s">
-        <v>603</v>
+        <v>600</v>
       </c>
       <c r="T3" s="3" t="s">
-        <v>633</v>
-      </c>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" ht="15" x14ac:dyDescent="0.3">
       <c r="A4" s="12" t="s">
         <v>12</v>
       </c>
@@ -2781,13 +2887,13 @@
         <v>246</v>
       </c>
       <c r="S4" s="3" t="s">
-        <v>605</v>
+        <v>602</v>
       </c>
       <c r="T4" s="3" t="s">
-        <v>633</v>
-      </c>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" ht="15" x14ac:dyDescent="0.3">
       <c r="A5" s="12" t="s">
         <v>15</v>
       </c>
@@ -2837,10 +2943,10 @@
         <v>246</v>
       </c>
       <c r="S5" s="3" t="s">
-        <v>605</v>
+        <v>602</v>
       </c>
       <c r="T5" s="3" t="s">
-        <v>633</v>
+        <v>630</v>
       </c>
     </row>
     <row r="6" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
@@ -2893,10 +2999,10 @@
         <v>246</v>
       </c>
       <c r="S6" s="3" t="s">
-        <v>605</v>
+        <v>602</v>
       </c>
       <c r="T6" s="3" t="s">
-        <v>633</v>
+        <v>630</v>
       </c>
     </row>
     <row r="7" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
@@ -2949,10 +3055,10 @@
         <v>246</v>
       </c>
       <c r="S7" s="3" t="s">
-        <v>605</v>
+        <v>602</v>
       </c>
       <c r="T7" s="3" t="s">
-        <v>633</v>
+        <v>630</v>
       </c>
     </row>
     <row r="8" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
@@ -3005,13 +3111,13 @@
         <v>246</v>
       </c>
       <c r="S8" s="3" t="s">
-        <v>605</v>
+        <v>602</v>
       </c>
       <c r="T8" s="3" t="s">
-        <v>633</v>
-      </c>
-    </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" ht="15" x14ac:dyDescent="0.3">
       <c r="A9" s="12" t="s">
         <v>23</v>
       </c>
@@ -3061,13 +3167,13 @@
         <v>246</v>
       </c>
       <c r="S9" s="3" t="s">
-        <v>605</v>
+        <v>602</v>
       </c>
       <c r="T9" s="3" t="s">
-        <v>633</v>
-      </c>
-    </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" ht="15" x14ac:dyDescent="0.3">
       <c r="A10" s="12" t="s">
         <v>25</v>
       </c>
@@ -3117,10 +3223,10 @@
         <v>246</v>
       </c>
       <c r="S10" s="3" t="s">
-        <v>605</v>
+        <v>602</v>
       </c>
       <c r="T10" s="3" t="s">
-        <v>633</v>
+        <v>630</v>
       </c>
     </row>
     <row r="11" spans="1:20" ht="115.2" x14ac:dyDescent="0.3">
@@ -3176,13 +3282,13 @@
         <v>339</v>
       </c>
       <c r="R11" s="22" t="s">
-        <v>602</v>
+        <v>599</v>
       </c>
       <c r="S11" s="21" t="s">
-        <v>603</v>
+        <v>600</v>
       </c>
       <c r="T11" s="3" t="s">
-        <v>633</v>
+        <v>630</v>
       </c>
     </row>
     <row r="12" spans="1:20" ht="100.8" x14ac:dyDescent="0.3">
@@ -3238,13 +3344,13 @@
         <v>342</v>
       </c>
       <c r="R12" s="22" t="s">
-        <v>602</v>
+        <v>599</v>
       </c>
       <c r="S12" s="21" t="s">
-        <v>603</v>
+        <v>600</v>
       </c>
       <c r="T12" s="3" t="s">
-        <v>633</v>
+        <v>630</v>
       </c>
     </row>
     <row r="13" spans="1:20" ht="115.2" x14ac:dyDescent="0.3">
@@ -3300,13 +3406,13 @@
         <v>348</v>
       </c>
       <c r="R13" s="22" t="s">
-        <v>602</v>
+        <v>599</v>
       </c>
       <c r="S13" s="21" t="s">
-        <v>603</v>
+        <v>600</v>
       </c>
       <c r="T13" s="3" t="s">
-        <v>633</v>
+        <v>630</v>
       </c>
     </row>
     <row r="14" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
@@ -3359,13 +3465,13 @@
         <v>246</v>
       </c>
       <c r="S14" s="21" t="s">
-        <v>607</v>
+        <v>604</v>
       </c>
       <c r="T14" s="3" t="s">
-        <v>633</v>
-      </c>
-    </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" ht="15" x14ac:dyDescent="0.3">
       <c r="A15" s="12" t="s">
         <v>187</v>
       </c>
@@ -3415,10 +3521,10 @@
         <v>246</v>
       </c>
       <c r="S15" s="21" t="s">
-        <v>607</v>
+        <v>604</v>
       </c>
       <c r="T15" s="3" t="s">
-        <v>633</v>
+        <v>630</v>
       </c>
     </row>
     <row r="16" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
@@ -3471,10 +3577,10 @@
         <v>246</v>
       </c>
       <c r="S16" s="21" t="s">
-        <v>607</v>
+        <v>604</v>
       </c>
       <c r="T16" s="3" t="s">
-        <v>633</v>
+        <v>630</v>
       </c>
     </row>
     <row r="17" spans="1:20" s="41" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -3494,7 +3600,7 @@
         <v>247</v>
       </c>
       <c r="F17" s="35" t="s">
-        <v>618</v>
+        <v>615</v>
       </c>
       <c r="G17" s="36"/>
       <c r="H17" s="37"/>
@@ -3525,13 +3631,13 @@
         <v>246</v>
       </c>
       <c r="S17" s="41" t="s">
-        <v>603</v>
+        <v>600</v>
       </c>
       <c r="T17" s="3" t="s">
-        <v>633</v>
-      </c>
-    </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.3">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" ht="15" x14ac:dyDescent="0.3">
       <c r="A18" s="12" t="s">
         <v>194</v>
       </c>
@@ -3581,13 +3687,13 @@
         <v>246</v>
       </c>
       <c r="S18" s="32" t="s">
-        <v>607</v>
+        <v>604</v>
       </c>
       <c r="T18" s="3" t="s">
-        <v>633</v>
-      </c>
-    </row>
-    <row r="19" spans="1:20" s="30" customFormat="1" x14ac:dyDescent="0.3">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" s="30" customFormat="1" ht="15" x14ac:dyDescent="0.3">
       <c r="A19" s="23" t="s">
         <v>248</v>
       </c>
@@ -3634,7 +3740,7 @@
         <v>367</v>
       </c>
       <c r="T19" s="3" t="s">
-        <v>633</v>
+        <v>630</v>
       </c>
     </row>
     <row r="20" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
@@ -3684,13 +3790,13 @@
         <v>395</v>
       </c>
       <c r="R20" s="22" t="s">
-        <v>606</v>
+        <v>603</v>
       </c>
       <c r="S20" s="32" t="s">
-        <v>607</v>
+        <v>604</v>
       </c>
       <c r="T20" s="3" t="s">
-        <v>633</v>
+        <v>630</v>
       </c>
     </row>
     <row r="21" spans="1:20" ht="129.6" x14ac:dyDescent="0.3">
@@ -3742,13 +3848,13 @@
         <v>386</v>
       </c>
       <c r="R21" s="31" t="s">
-        <v>611</v>
+        <v>608</v>
       </c>
       <c r="S21" s="32" t="s">
-        <v>603</v>
+        <v>600</v>
       </c>
       <c r="T21" s="3" t="s">
-        <v>633</v>
+        <v>630</v>
       </c>
     </row>
     <row r="22" spans="1:20" ht="129.6" x14ac:dyDescent="0.3">
@@ -3800,13 +3906,13 @@
         <v>401</v>
       </c>
       <c r="R22" s="31" t="s">
-        <v>611</v>
+        <v>608</v>
       </c>
       <c r="S22" s="32" t="s">
-        <v>603</v>
+        <v>600</v>
       </c>
       <c r="T22" s="3" t="s">
-        <v>633</v>
+        <v>630</v>
       </c>
     </row>
     <row r="23" spans="1:20" ht="15" x14ac:dyDescent="0.3">
@@ -3852,13 +3958,13 @@
         <v>389</v>
       </c>
       <c r="R23" s="31" t="s">
-        <v>611</v>
+        <v>608</v>
       </c>
       <c r="S23" s="32" t="s">
-        <v>603</v>
+        <v>600</v>
       </c>
       <c r="T23" s="3" t="s">
-        <v>633</v>
+        <v>630</v>
       </c>
     </row>
     <row r="24" spans="1:20" ht="15" x14ac:dyDescent="0.3">
@@ -3904,13 +4010,13 @@
         <v>398</v>
       </c>
       <c r="R24" s="31" t="s">
-        <v>611</v>
+        <v>608</v>
       </c>
       <c r="S24" s="32" t="s">
-        <v>603</v>
+        <v>600</v>
       </c>
       <c r="T24" s="3" t="s">
-        <v>633</v>
+        <v>630</v>
       </c>
     </row>
     <row r="25" spans="1:20" ht="15" x14ac:dyDescent="0.3">
@@ -3956,13 +4062,13 @@
         <v>392</v>
       </c>
       <c r="R25" s="31" t="s">
-        <v>611</v>
+        <v>608</v>
       </c>
       <c r="S25" s="32" t="s">
-        <v>603</v>
+        <v>600</v>
       </c>
       <c r="T25" s="3" t="s">
-        <v>633</v>
+        <v>630</v>
       </c>
     </row>
     <row r="26" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
@@ -4012,13 +4118,13 @@
         <v>405</v>
       </c>
       <c r="R26" s="31" t="s">
-        <v>609</v>
+        <v>606</v>
       </c>
       <c r="S26" s="32" t="s">
-        <v>603</v>
+        <v>600</v>
       </c>
       <c r="T26" s="3" t="s">
-        <v>633</v>
+        <v>630</v>
       </c>
     </row>
     <row r="27" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
@@ -4068,16 +4174,16 @@
         <v>411</v>
       </c>
       <c r="R27" s="31" t="s">
-        <v>609</v>
+        <v>606</v>
       </c>
       <c r="S27" s="32" t="s">
-        <v>603</v>
+        <v>600</v>
       </c>
       <c r="T27" s="3" t="s">
-        <v>633</v>
-      </c>
-    </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.3">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="28" spans="1:20" ht="15" x14ac:dyDescent="0.3">
       <c r="A28" s="12" t="s">
         <v>145</v>
       </c>
@@ -4124,13 +4230,13 @@
         <v>408</v>
       </c>
       <c r="R28" s="31" t="s">
-        <v>610</v>
+        <v>607</v>
       </c>
       <c r="S28" s="32" t="s">
-        <v>603</v>
+        <v>600</v>
       </c>
       <c r="T28" s="3" t="s">
-        <v>633</v>
+        <v>630</v>
       </c>
     </row>
     <row r="29" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
@@ -4183,13 +4289,13 @@
         <v>246</v>
       </c>
       <c r="S29" s="32" t="s">
-        <v>607</v>
+        <v>604</v>
       </c>
       <c r="T29" s="3" t="s">
-        <v>633</v>
-      </c>
-    </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.3">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="30" spans="1:20" ht="15" x14ac:dyDescent="0.3">
       <c r="A30" s="12" t="s">
         <v>60</v>
       </c>
@@ -4239,10 +4345,10 @@
         <v>246</v>
       </c>
       <c r="S30" s="32" t="s">
-        <v>607</v>
+        <v>604</v>
       </c>
       <c r="T30" s="32" t="s">
-        <v>634</v>
+        <v>631</v>
       </c>
     </row>
     <row r="31" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
@@ -4295,13 +4401,13 @@
         <v>246</v>
       </c>
       <c r="S31" s="32" t="s">
-        <v>607</v>
+        <v>604</v>
       </c>
       <c r="T31" s="32" t="s">
-        <v>633</v>
-      </c>
-    </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.3">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="32" spans="1:20" ht="15" x14ac:dyDescent="0.3">
       <c r="A32" s="12" t="s">
         <v>64</v>
       </c>
@@ -4351,10 +4457,10 @@
         <v>246</v>
       </c>
       <c r="S32" s="32" t="s">
-        <v>607</v>
+        <v>604</v>
       </c>
       <c r="T32" s="32" t="s">
-        <v>633</v>
+        <v>630</v>
       </c>
     </row>
     <row r="33" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
@@ -4407,10 +4513,10 @@
         <v>246</v>
       </c>
       <c r="S33" s="32" t="s">
-        <v>607</v>
+        <v>604</v>
       </c>
       <c r="T33" s="32" t="s">
-        <v>633</v>
+        <v>630</v>
       </c>
     </row>
     <row r="34" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
@@ -4463,13 +4569,13 @@
         <v>246</v>
       </c>
       <c r="S34" s="32" t="s">
-        <v>607</v>
+        <v>604</v>
       </c>
       <c r="T34" s="32" t="s">
-        <v>633</v>
-      </c>
-    </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.3">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="35" spans="1:20" ht="15" x14ac:dyDescent="0.3">
       <c r="A35" s="12" t="s">
         <v>267</v>
       </c>
@@ -4516,13 +4622,13 @@
         <v>431</v>
       </c>
       <c r="R35" s="33" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="S35" s="32" t="s">
-        <v>603</v>
+        <v>600</v>
       </c>
       <c r="T35" s="32" t="s">
-        <v>633</v>
+        <v>630</v>
       </c>
     </row>
     <row r="36" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
@@ -4539,7 +4645,7 @@
         <v>225</v>
       </c>
       <c r="E36" s="24" t="s">
-        <v>612</v>
+        <v>609</v>
       </c>
       <c r="F36" s="10" t="s">
         <v>246</v>
@@ -4572,13 +4678,13 @@
         <v>440</v>
       </c>
       <c r="R36" s="33" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="S36" s="32" t="s">
-        <v>603</v>
+        <v>600</v>
       </c>
       <c r="T36" s="32" t="s">
-        <v>633</v>
+        <v>630</v>
       </c>
     </row>
     <row r="37" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
@@ -4628,13 +4734,13 @@
         <v>434</v>
       </c>
       <c r="R37" s="31" t="s">
-        <v>613</v>
+        <v>610</v>
       </c>
       <c r="S37" s="32" t="s">
-        <v>603</v>
+        <v>600</v>
       </c>
       <c r="T37" s="32" t="s">
-        <v>633</v>
+        <v>630</v>
       </c>
     </row>
     <row r="38" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
@@ -4680,10 +4786,10 @@
         <v>428</v>
       </c>
       <c r="S38" s="32" t="s">
-        <v>607</v>
+        <v>604</v>
       </c>
       <c r="T38" s="32" t="s">
-        <v>633</v>
+        <v>630</v>
       </c>
     </row>
     <row r="39" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
@@ -4729,13 +4835,13 @@
         <v>437</v>
       </c>
       <c r="S39" t="s">
-        <v>607</v>
+        <v>604</v>
       </c>
       <c r="T39" s="32" t="s">
-        <v>633</v>
-      </c>
-    </row>
-    <row r="40" spans="1:20" x14ac:dyDescent="0.3">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="40" spans="1:20" ht="15" x14ac:dyDescent="0.3">
       <c r="A40" s="12" t="s">
         <v>68</v>
       </c>
@@ -4773,25 +4879,25 @@
         <v>444</v>
       </c>
       <c r="O40" s="3" t="s">
-        <v>487</v>
+        <v>484</v>
       </c>
       <c r="P40" s="3" t="s">
-        <v>488</v>
+        <v>485</v>
       </c>
       <c r="Q40" s="3" t="s">
-        <v>489</v>
+        <v>486</v>
       </c>
       <c r="R40" s="21" t="s">
-        <v>614</v>
+        <v>611</v>
       </c>
       <c r="S40" s="21" t="s">
-        <v>603</v>
+        <v>600</v>
       </c>
       <c r="T40" s="32" t="s">
-        <v>633</v>
-      </c>
-    </row>
-    <row r="41" spans="1:20" x14ac:dyDescent="0.3">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="41" spans="1:20" ht="15" x14ac:dyDescent="0.3">
       <c r="A41" s="12" t="s">
         <v>72</v>
       </c>
@@ -4829,25 +4935,25 @@
         <v>444</v>
       </c>
       <c r="O41" s="3" t="s">
-        <v>481</v>
+        <v>478</v>
       </c>
       <c r="P41" s="3" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
       <c r="Q41" s="3" t="s">
-        <v>483</v>
+        <v>480</v>
       </c>
       <c r="R41" s="33" t="s">
-        <v>614</v>
+        <v>611</v>
       </c>
       <c r="S41" s="21" t="s">
-        <v>603</v>
+        <v>600</v>
       </c>
       <c r="T41" s="32" t="s">
-        <v>633</v>
-      </c>
-    </row>
-    <row r="42" spans="1:20" x14ac:dyDescent="0.3">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="42" spans="1:20" ht="15" x14ac:dyDescent="0.3">
       <c r="A42" s="12" t="s">
         <v>75</v>
       </c>
@@ -4885,22 +4991,22 @@
         <v>444</v>
       </c>
       <c r="O42" s="3" t="s">
-        <v>502</v>
+        <v>499</v>
       </c>
       <c r="P42" s="3" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
       <c r="Q42" s="3" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="R42" s="32" t="s">
-        <v>615</v>
+        <v>612</v>
       </c>
       <c r="S42" s="21" t="s">
-        <v>603</v>
+        <v>600</v>
       </c>
       <c r="T42" s="32" t="s">
-        <v>633</v>
+        <v>630</v>
       </c>
     </row>
     <row r="43" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
@@ -4941,25 +5047,25 @@
         <v>444</v>
       </c>
       <c r="O43" s="3" t="s">
-        <v>484</v>
+        <v>481</v>
       </c>
       <c r="P43" s="3" t="s">
-        <v>485</v>
+        <v>482</v>
       </c>
       <c r="Q43" s="3" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
       <c r="R43" s="33" t="s">
-        <v>616</v>
+        <v>613</v>
       </c>
       <c r="S43" s="21" t="s">
-        <v>603</v>
+        <v>600</v>
       </c>
       <c r="T43" s="32" t="s">
-        <v>633</v>
-      </c>
-    </row>
-    <row r="44" spans="1:20" x14ac:dyDescent="0.3">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="44" spans="1:20" ht="15" x14ac:dyDescent="0.3">
       <c r="A44" s="12" t="s">
         <v>81</v>
       </c>
@@ -4997,22 +5103,22 @@
         <v>444</v>
       </c>
       <c r="O44" s="3" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
       <c r="P44" s="3" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
       <c r="Q44" s="3" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
       <c r="R44" s="32" t="s">
-        <v>617</v>
+        <v>614</v>
       </c>
       <c r="S44" s="21" t="s">
-        <v>603</v>
+        <v>600</v>
       </c>
       <c r="T44" s="32" t="s">
-        <v>633</v>
+        <v>630</v>
       </c>
     </row>
     <row r="45" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
@@ -5065,10 +5171,10 @@
         <v>246</v>
       </c>
       <c r="S45" s="21" t="s">
-        <v>607</v>
+        <v>604</v>
       </c>
       <c r="T45" s="32" t="s">
-        <v>633</v>
+        <v>630</v>
       </c>
     </row>
     <row r="46" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
@@ -5109,22 +5215,22 @@
         <v>444</v>
       </c>
       <c r="O46" s="3" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="P46" s="3" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="Q46" s="3" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="R46" s="21" t="s">
-        <v>602</v>
+        <v>599</v>
       </c>
       <c r="S46" s="21" t="s">
-        <v>619</v>
+        <v>616</v>
       </c>
       <c r="T46" s="32" t="s">
-        <v>633</v>
+        <v>630</v>
       </c>
     </row>
     <row r="47" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
@@ -5165,22 +5271,22 @@
         <v>444</v>
       </c>
       <c r="O47" s="3" t="s">
-        <v>460</v>
+        <v>632</v>
       </c>
       <c r="P47" s="3" t="s">
-        <v>461</v>
+        <v>633</v>
       </c>
       <c r="Q47" s="3" t="s">
-        <v>462</v>
+        <v>634</v>
       </c>
       <c r="R47" s="21" t="s">
-        <v>602</v>
+        <v>599</v>
       </c>
       <c r="S47" s="21" t="s">
-        <v>619</v>
+        <v>616</v>
       </c>
       <c r="T47" s="32" t="s">
-        <v>633</v>
+        <v>630</v>
       </c>
     </row>
     <row r="48" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
@@ -5230,13 +5336,13 @@
         <v>450</v>
       </c>
       <c r="R48" s="21" t="s">
-        <v>602</v>
+        <v>599</v>
       </c>
       <c r="S48" s="21" t="s">
-        <v>619</v>
+        <v>616</v>
       </c>
       <c r="T48" s="32" t="s">
-        <v>633</v>
+        <v>630</v>
       </c>
     </row>
     <row r="49" spans="1:20" x14ac:dyDescent="0.3">
@@ -5277,22 +5383,22 @@
         <v>444</v>
       </c>
       <c r="O49" s="3" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
       <c r="P49" s="3" t="s">
-        <v>500</v>
+        <v>497</v>
       </c>
       <c r="Q49" s="3" t="s">
-        <v>501</v>
-      </c>
-      <c r="R49" s="42" t="s">
+        <v>498</v>
+      </c>
+      <c r="R49" s="21" t="s">
         <v>246</v>
       </c>
       <c r="S49" s="32" t="s">
-        <v>603</v>
+        <v>600</v>
       </c>
       <c r="T49" s="32" t="s">
-        <v>633</v>
+        <v>630</v>
       </c>
     </row>
     <row r="50" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
@@ -5333,22 +5439,22 @@
         <v>444</v>
       </c>
       <c r="O50" s="3" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="P50" s="3" t="s">
-        <v>464</v>
+        <v>461</v>
       </c>
       <c r="Q50" s="3" t="s">
-        <v>465</v>
+        <v>462</v>
       </c>
       <c r="R50" s="21" t="s">
-        <v>602</v>
+        <v>599</v>
       </c>
       <c r="S50" s="21" t="s">
-        <v>619</v>
+        <v>616</v>
       </c>
       <c r="T50" s="32" t="s">
-        <v>633</v>
+        <v>630</v>
       </c>
     </row>
     <row r="51" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
@@ -5389,22 +5495,22 @@
         <v>444</v>
       </c>
       <c r="O51" s="3" t="s">
-        <v>478</v>
+        <v>475</v>
       </c>
       <c r="P51" s="3" t="s">
-        <v>479</v>
+        <v>476</v>
       </c>
       <c r="Q51" s="3" t="s">
-        <v>480</v>
-      </c>
-      <c r="R51" s="42" t="s">
+        <v>477</v>
+      </c>
+      <c r="R51" s="21" t="s">
         <v>246</v>
       </c>
       <c r="S51" s="32" t="s">
-        <v>603</v>
+        <v>600</v>
       </c>
       <c r="T51" s="32" t="s">
-        <v>633</v>
+        <v>630</v>
       </c>
     </row>
     <row r="52" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
@@ -5421,7 +5527,7 @@
         <v>225</v>
       </c>
       <c r="E52" s="10" t="s">
-        <v>612</v>
+        <v>609</v>
       </c>
       <c r="F52" s="10" t="s">
         <v>246</v>
@@ -5445,22 +5551,22 @@
         <v>444</v>
       </c>
       <c r="O52" s="3" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
       <c r="P52" s="3" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
       <c r="Q52" s="3" t="s">
-        <v>495</v>
-      </c>
-      <c r="R52" s="42" t="s">
+        <v>492</v>
+      </c>
+      <c r="R52" s="21" t="s">
         <v>246</v>
       </c>
       <c r="S52" s="32" t="s">
-        <v>603</v>
+        <v>600</v>
       </c>
       <c r="T52" s="32" t="s">
-        <v>633</v>
+        <v>630</v>
       </c>
     </row>
     <row r="53" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
@@ -5501,25 +5607,25 @@
         <v>444</v>
       </c>
       <c r="O53" s="3" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
       <c r="P53" s="3" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
       <c r="Q53" s="3" t="s">
-        <v>477</v>
-      </c>
-      <c r="R53" s="42" t="s">
+        <v>474</v>
+      </c>
+      <c r="R53" s="21" t="s">
         <v>246</v>
       </c>
       <c r="S53" s="32" t="s">
-        <v>603</v>
+        <v>600</v>
       </c>
       <c r="T53" s="32" t="s">
-        <v>633</v>
-      </c>
-    </row>
-    <row r="54" spans="1:20" x14ac:dyDescent="0.3">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="54" spans="1:20" ht="15" x14ac:dyDescent="0.3">
       <c r="A54" s="12" t="s">
         <v>102</v>
       </c>
@@ -5557,22 +5663,22 @@
         <v>444</v>
       </c>
       <c r="O54" s="3" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
       <c r="P54" s="3" t="s">
-        <v>473</v>
+        <v>470</v>
       </c>
       <c r="Q54" s="3" t="s">
-        <v>474</v>
-      </c>
-      <c r="R54" s="42" t="s">
+        <v>471</v>
+      </c>
+      <c r="R54" s="21" t="s">
         <v>246</v>
       </c>
       <c r="S54" s="32" t="s">
-        <v>603</v>
+        <v>600</v>
       </c>
       <c r="T54" s="32" t="s">
-        <v>633</v>
+        <v>630</v>
       </c>
     </row>
     <row r="55" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
@@ -5613,22 +5719,22 @@
         <v>444</v>
       </c>
       <c r="O55" s="3" t="s">
-        <v>496</v>
+        <v>493</v>
       </c>
       <c r="P55" s="3" t="s">
-        <v>497</v>
+        <v>494</v>
       </c>
       <c r="Q55" s="3" t="s">
-        <v>498</v>
-      </c>
-      <c r="R55" s="42" t="s">
+        <v>495</v>
+      </c>
+      <c r="R55" s="21" t="s">
         <v>246</v>
       </c>
       <c r="S55" s="32" t="s">
-        <v>603</v>
+        <v>600</v>
       </c>
       <c r="T55" s="32" t="s">
-        <v>633</v>
+        <v>630</v>
       </c>
     </row>
     <row r="56" spans="1:20" ht="15" x14ac:dyDescent="0.3">
@@ -5669,22 +5775,22 @@
         <v>444</v>
       </c>
       <c r="O56" s="3" t="s">
-        <v>490</v>
+        <v>487</v>
       </c>
       <c r="P56" s="3" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="Q56" s="3" t="s">
-        <v>492</v>
-      </c>
-      <c r="R56" s="42" t="s">
+        <v>489</v>
+      </c>
+      <c r="R56" s="21" t="s">
         <v>246</v>
       </c>
       <c r="S56" s="32" t="s">
-        <v>603</v>
+        <v>600</v>
       </c>
       <c r="T56" s="32" t="s">
-        <v>633</v>
+        <v>630</v>
       </c>
     </row>
     <row r="57" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
@@ -5733,14 +5839,14 @@
       <c r="Q57" s="3" t="s">
         <v>456</v>
       </c>
-      <c r="R57" s="42" t="s">
+      <c r="R57" s="21" t="s">
         <v>246</v>
       </c>
       <c r="S57" s="32" t="s">
-        <v>603</v>
+        <v>600</v>
       </c>
       <c r="T57" s="32" t="s">
-        <v>633</v>
+        <v>630</v>
       </c>
     </row>
     <row r="58" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
@@ -5790,13 +5896,13 @@
         <v>447</v>
       </c>
       <c r="R58" s="21" t="s">
-        <v>602</v>
+        <v>599</v>
       </c>
       <c r="S58" s="32" t="s">
-        <v>607</v>
+        <v>604</v>
       </c>
       <c r="T58" s="32" t="s">
-        <v>633</v>
+        <v>630</v>
       </c>
     </row>
     <row r="59" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
@@ -5845,14 +5951,14 @@
       <c r="Q59" s="3" t="s">
         <v>459</v>
       </c>
-      <c r="R59" s="42" t="s">
+      <c r="R59" s="21" t="s">
         <v>246</v>
       </c>
       <c r="S59" s="32" t="s">
-        <v>603</v>
+        <v>600</v>
       </c>
       <c r="T59" s="32" t="s">
-        <v>633</v>
+        <v>630</v>
       </c>
     </row>
     <row r="60" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
@@ -5893,25 +5999,25 @@
         <v>444</v>
       </c>
       <c r="O60" s="3" t="s">
-        <v>469</v>
+        <v>466</v>
       </c>
       <c r="P60" s="3" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
       <c r="Q60" s="3" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="R60" s="21" t="s">
-        <v>602</v>
+        <v>599</v>
       </c>
       <c r="S60" s="32" t="s">
-        <v>607</v>
+        <v>604</v>
       </c>
       <c r="T60" s="32" t="s">
-        <v>633</v>
-      </c>
-    </row>
-    <row r="61" spans="1:20" x14ac:dyDescent="0.3">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="61" spans="1:20" ht="15" x14ac:dyDescent="0.3">
       <c r="A61" s="12" t="s">
         <v>36</v>
       </c>
@@ -5946,28 +6052,28 @@
         <v>38</v>
       </c>
       <c r="N61" s="3" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="O61" s="3" t="s">
-        <v>521</v>
+        <v>518</v>
       </c>
       <c r="P61" s="3" t="s">
-        <v>522</v>
+        <v>519</v>
       </c>
       <c r="Q61" s="3" t="s">
-        <v>523</v>
-      </c>
-      <c r="R61" s="42" t="s">
+        <v>520</v>
+      </c>
+      <c r="R61" s="21" t="s">
         <v>246</v>
       </c>
       <c r="S61" s="32" t="s">
-        <v>607</v>
+        <v>604</v>
       </c>
       <c r="T61" s="32" t="s">
-        <v>633</v>
-      </c>
-    </row>
-    <row r="62" spans="1:20" x14ac:dyDescent="0.3">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="62" spans="1:20" ht="15" x14ac:dyDescent="0.3">
       <c r="A62" s="12" t="s">
         <v>39</v>
       </c>
@@ -6002,28 +6108,28 @@
         <v>38</v>
       </c>
       <c r="N62" s="3" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="O62" s="3" t="s">
-        <v>524</v>
+        <v>521</v>
       </c>
       <c r="P62" s="3" t="s">
-        <v>525</v>
+        <v>522</v>
       </c>
       <c r="Q62" s="3" t="s">
-        <v>526</v>
-      </c>
-      <c r="R62" s="42" t="s">
+        <v>523</v>
+      </c>
+      <c r="R62" s="21" t="s">
         <v>246</v>
       </c>
       <c r="S62" s="32" t="s">
-        <v>607</v>
+        <v>604</v>
       </c>
       <c r="T62" s="32" t="s">
-        <v>633</v>
-      </c>
-    </row>
-    <row r="63" spans="1:20" x14ac:dyDescent="0.3">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="63" spans="1:20" ht="15" x14ac:dyDescent="0.3">
       <c r="A63" s="12" t="s">
         <v>41</v>
       </c>
@@ -6058,28 +6164,28 @@
         <v>38</v>
       </c>
       <c r="N63" s="3" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="O63" s="3" t="s">
-        <v>527</v>
+        <v>524</v>
       </c>
       <c r="P63" s="3" t="s">
-        <v>528</v>
+        <v>525</v>
       </c>
       <c r="Q63" s="3" t="s">
-        <v>529</v>
-      </c>
-      <c r="R63" s="42" t="s">
+        <v>526</v>
+      </c>
+      <c r="R63" s="21" t="s">
         <v>246</v>
       </c>
       <c r="S63" s="32" t="s">
-        <v>607</v>
+        <v>604</v>
       </c>
       <c r="T63" s="32" t="s">
-        <v>633</v>
-      </c>
-    </row>
-    <row r="64" spans="1:20" x14ac:dyDescent="0.3">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="64" spans="1:20" ht="15" x14ac:dyDescent="0.3">
       <c r="A64" s="12" t="s">
         <v>43</v>
       </c>
@@ -6114,28 +6220,28 @@
         <v>38</v>
       </c>
       <c r="N64" s="3" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="O64" s="3" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
       <c r="P64" s="3" t="s">
-        <v>516</v>
+        <v>513</v>
       </c>
       <c r="Q64" s="3" t="s">
-        <v>517</v>
-      </c>
-      <c r="R64" s="42" t="s">
+        <v>514</v>
+      </c>
+      <c r="R64" s="21" t="s">
         <v>246</v>
       </c>
       <c r="S64" s="32" t="s">
-        <v>607</v>
+        <v>604</v>
       </c>
       <c r="T64" s="32" t="s">
-        <v>633</v>
-      </c>
-    </row>
-    <row r="65" spans="1:20" x14ac:dyDescent="0.3">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="65" spans="1:20" ht="15" x14ac:dyDescent="0.3">
       <c r="A65" s="12" t="s">
         <v>45</v>
       </c>
@@ -6170,28 +6276,28 @@
         <v>38</v>
       </c>
       <c r="N65" s="3" t="s">
+        <v>505</v>
+      </c>
+      <c r="O65" s="3" t="s">
+        <v>506</v>
+      </c>
+      <c r="P65" s="3" t="s">
+        <v>507</v>
+      </c>
+      <c r="Q65" s="3" t="s">
         <v>508</v>
       </c>
-      <c r="O65" s="3" t="s">
-        <v>509</v>
-      </c>
-      <c r="P65" s="3" t="s">
-        <v>510</v>
-      </c>
-      <c r="Q65" s="3" t="s">
-        <v>511</v>
-      </c>
-      <c r="R65" s="42" t="s">
+      <c r="R65" s="21" t="s">
         <v>246</v>
       </c>
       <c r="S65" s="32" t="s">
-        <v>607</v>
+        <v>604</v>
       </c>
       <c r="T65" s="32" t="s">
-        <v>633</v>
-      </c>
-    </row>
-    <row r="66" spans="1:20" x14ac:dyDescent="0.3">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="66" spans="1:20" ht="15" x14ac:dyDescent="0.3">
       <c r="A66" s="12" t="s">
         <v>47</v>
       </c>
@@ -6226,28 +6332,28 @@
         <v>38</v>
       </c>
       <c r="N66" s="3" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="O66" s="3" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
       <c r="P66" s="3" t="s">
-        <v>513</v>
+        <v>510</v>
       </c>
       <c r="Q66" s="3" t="s">
-        <v>514</v>
-      </c>
-      <c r="R66" s="42" t="s">
+        <v>511</v>
+      </c>
+      <c r="R66" s="21" t="s">
         <v>246</v>
       </c>
       <c r="S66" s="32" t="s">
-        <v>607</v>
+        <v>604</v>
       </c>
       <c r="T66" s="32" t="s">
-        <v>633</v>
-      </c>
-    </row>
-    <row r="67" spans="1:20" x14ac:dyDescent="0.3">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="67" spans="1:20" ht="15" x14ac:dyDescent="0.3">
       <c r="A67" s="12" t="s">
         <v>49</v>
       </c>
@@ -6282,25 +6388,25 @@
         <v>38</v>
       </c>
       <c r="N67" s="3" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="O67" s="3" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
       <c r="P67" s="3" t="s">
-        <v>531</v>
+        <v>528</v>
       </c>
       <c r="Q67" s="3" t="s">
-        <v>532</v>
-      </c>
-      <c r="R67" s="42" t="s">
+        <v>529</v>
+      </c>
+      <c r="R67" s="21" t="s">
         <v>246</v>
       </c>
       <c r="S67" s="32" t="s">
-        <v>607</v>
+        <v>604</v>
       </c>
       <c r="T67" s="32" t="s">
-        <v>633</v>
+        <v>630</v>
       </c>
     </row>
     <row r="68" spans="1:20" ht="15" x14ac:dyDescent="0.3">
@@ -6338,25 +6444,25 @@
         <v>54</v>
       </c>
       <c r="N68" s="3" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="O68" s="3" t="s">
-        <v>518</v>
+        <v>515</v>
       </c>
       <c r="P68" s="3" t="s">
-        <v>519</v>
+        <v>516</v>
       </c>
       <c r="Q68" s="3" t="s">
-        <v>520</v>
-      </c>
-      <c r="R68" s="42" t="s">
+        <v>517</v>
+      </c>
+      <c r="R68" s="21" t="s">
         <v>246</v>
       </c>
       <c r="S68" s="32" t="s">
-        <v>607</v>
+        <v>604</v>
       </c>
       <c r="T68" s="32" t="s">
-        <v>633</v>
+        <v>630</v>
       </c>
     </row>
     <row r="69" spans="1:20" ht="15" x14ac:dyDescent="0.3">
@@ -6394,25 +6500,25 @@
         <v>150</v>
       </c>
       <c r="N69" s="3" t="s">
+        <v>530</v>
+      </c>
+      <c r="O69" s="3" t="s">
+        <v>531</v>
+      </c>
+      <c r="P69" s="3" t="s">
+        <v>532</v>
+      </c>
+      <c r="Q69" s="3" t="s">
         <v>533</v>
       </c>
-      <c r="O69" s="3" t="s">
-        <v>534</v>
-      </c>
-      <c r="P69" s="3" t="s">
-        <v>535</v>
-      </c>
-      <c r="Q69" s="3" t="s">
-        <v>536</v>
-      </c>
       <c r="R69" s="21" t="s">
-        <v>602</v>
+        <v>599</v>
       </c>
       <c r="S69" s="32" t="s">
-        <v>619</v>
+        <v>616</v>
       </c>
       <c r="T69" s="32" t="s">
-        <v>633</v>
+        <v>630</v>
       </c>
     </row>
     <row r="70" spans="1:20" ht="15" x14ac:dyDescent="0.3">
@@ -6450,28 +6556,28 @@
         <v>150</v>
       </c>
       <c r="N70" s="3" t="s">
-        <v>533</v>
+        <v>530</v>
       </c>
       <c r="O70" s="3" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
       <c r="P70" s="3" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
       <c r="Q70" s="3" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
       <c r="R70" s="31" t="s">
-        <v>609</v>
+        <v>606</v>
       </c>
       <c r="S70" s="32" t="s">
-        <v>619</v>
+        <v>616</v>
       </c>
       <c r="T70" s="32" t="s">
-        <v>633</v>
-      </c>
-    </row>
-    <row r="71" spans="1:20" x14ac:dyDescent="0.3">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="71" spans="1:20" ht="15" x14ac:dyDescent="0.3">
       <c r="A71" s="12" t="s">
         <v>51</v>
       </c>
@@ -6491,7 +6597,7 @@
         <v>246</v>
       </c>
       <c r="G71" s="13" t="s">
-        <v>621</v>
+        <v>618</v>
       </c>
       <c r="H71" s="16"/>
       <c r="I71" s="16"/>
@@ -6506,28 +6612,28 @@
         <v>54</v>
       </c>
       <c r="N71" s="3" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
       <c r="O71" s="3" t="s">
-        <v>544</v>
+        <v>541</v>
       </c>
       <c r="P71" s="3" t="s">
-        <v>545</v>
+        <v>542</v>
       </c>
       <c r="Q71" s="3" t="s">
-        <v>546</v>
+        <v>543</v>
       </c>
       <c r="R71" s="33" t="s">
-        <v>620</v>
+        <v>617</v>
       </c>
       <c r="S71" s="32" t="s">
-        <v>603</v>
+        <v>600</v>
       </c>
       <c r="T71" s="32" t="s">
-        <v>633</v>
-      </c>
-    </row>
-    <row r="72" spans="1:20" x14ac:dyDescent="0.3">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="72" spans="1:20" ht="15" x14ac:dyDescent="0.3">
       <c r="A72" s="12" t="s">
         <v>168</v>
       </c>
@@ -6556,34 +6662,34 @@
         <v>169</v>
       </c>
       <c r="L72" s="5" t="s">
-        <v>622</v>
+        <v>619</v>
       </c>
       <c r="M72" s="6" t="s">
         <v>170</v>
       </c>
       <c r="N72" s="3" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
       <c r="O72" s="3" t="s">
-        <v>559</v>
+        <v>556</v>
       </c>
       <c r="P72" s="3" t="s">
-        <v>560</v>
+        <v>557</v>
       </c>
       <c r="Q72" s="3" t="s">
-        <v>561</v>
-      </c>
-      <c r="R72" s="42" t="s">
+        <v>558</v>
+      </c>
+      <c r="R72" s="21" t="s">
         <v>246</v>
       </c>
       <c r="S72" s="32" t="s">
-        <v>627</v>
+        <v>624</v>
       </c>
       <c r="T72" s="32" t="s">
-        <v>633</v>
-      </c>
-    </row>
-    <row r="73" spans="1:20" x14ac:dyDescent="0.3">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="73" spans="1:20" ht="15" x14ac:dyDescent="0.3">
       <c r="A73" s="12" t="s">
         <v>171</v>
       </c>
@@ -6612,34 +6718,34 @@
         <v>172</v>
       </c>
       <c r="L73" s="5" t="s">
-        <v>623</v>
+        <v>620</v>
       </c>
       <c r="M73" s="6" t="s">
         <v>170</v>
       </c>
       <c r="N73" s="3" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
       <c r="O73" s="3" t="s">
-        <v>550</v>
+        <v>547</v>
       </c>
       <c r="P73" s="3" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="Q73" s="3" t="s">
-        <v>552</v>
-      </c>
-      <c r="R73" s="42" t="s">
+        <v>549</v>
+      </c>
+      <c r="R73" s="21" t="s">
         <v>246</v>
       </c>
       <c r="S73" s="32" t="s">
-        <v>627</v>
+        <v>624</v>
       </c>
       <c r="T73" s="32" t="s">
-        <v>633</v>
-      </c>
-    </row>
-    <row r="74" spans="1:20" x14ac:dyDescent="0.3">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="74" spans="1:20" ht="15" x14ac:dyDescent="0.3">
       <c r="A74" s="12" t="s">
         <v>173</v>
       </c>
@@ -6668,34 +6774,34 @@
         <v>174</v>
       </c>
       <c r="L74" s="5" t="s">
-        <v>624</v>
+        <v>621</v>
       </c>
       <c r="M74" s="6" t="s">
         <v>170</v>
       </c>
       <c r="N74" s="3" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
       <c r="O74" s="3" t="s">
-        <v>556</v>
+        <v>553</v>
       </c>
       <c r="P74" s="3" t="s">
-        <v>557</v>
+        <v>554</v>
       </c>
       <c r="Q74" s="3" t="s">
-        <v>558</v>
-      </c>
-      <c r="R74" s="42" t="s">
+        <v>555</v>
+      </c>
+      <c r="R74" s="21" t="s">
         <v>246</v>
       </c>
       <c r="S74" s="32" t="s">
-        <v>627</v>
+        <v>624</v>
       </c>
       <c r="T74" s="32" t="s">
-        <v>633</v>
-      </c>
-    </row>
-    <row r="75" spans="1:20" x14ac:dyDescent="0.3">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="75" spans="1:20" ht="15" x14ac:dyDescent="0.3">
       <c r="A75" s="12" t="s">
         <v>175</v>
       </c>
@@ -6730,28 +6836,28 @@
         <v>170</v>
       </c>
       <c r="N75" s="3" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
       <c r="O75" s="3" t="s">
-        <v>547</v>
+        <v>544</v>
       </c>
       <c r="P75" s="3" t="s">
-        <v>548</v>
+        <v>545</v>
       </c>
       <c r="Q75" s="3" t="s">
-        <v>549</v>
-      </c>
-      <c r="R75" s="42" t="s">
+        <v>546</v>
+      </c>
+      <c r="R75" s="21" t="s">
         <v>246</v>
       </c>
       <c r="S75" s="32" t="s">
-        <v>627</v>
+        <v>624</v>
       </c>
       <c r="T75" s="32" t="s">
-        <v>633</v>
-      </c>
-    </row>
-    <row r="76" spans="1:20" x14ac:dyDescent="0.3">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="76" spans="1:20" ht="15" x14ac:dyDescent="0.3">
       <c r="A76" s="12" t="s">
         <v>177</v>
       </c>
@@ -6780,34 +6886,34 @@
         <v>178</v>
       </c>
       <c r="L76" s="5" t="s">
-        <v>625</v>
+        <v>622</v>
       </c>
       <c r="M76" s="6" t="s">
         <v>170</v>
       </c>
       <c r="N76" s="3" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
       <c r="O76" s="3" t="s">
-        <v>553</v>
+        <v>550</v>
       </c>
       <c r="P76" s="3" t="s">
-        <v>554</v>
+        <v>551</v>
       </c>
       <c r="Q76" s="3" t="s">
-        <v>555</v>
-      </c>
-      <c r="R76" s="42" t="s">
+        <v>552</v>
+      </c>
+      <c r="R76" s="21" t="s">
         <v>246</v>
       </c>
       <c r="S76" s="32" t="s">
-        <v>627</v>
+        <v>624</v>
       </c>
       <c r="T76" s="32" t="s">
-        <v>633</v>
-      </c>
-    </row>
-    <row r="77" spans="1:20" x14ac:dyDescent="0.3">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="77" spans="1:20" ht="15" x14ac:dyDescent="0.3">
       <c r="A77" s="12" t="s">
         <v>179</v>
       </c>
@@ -6836,34 +6942,34 @@
         <v>180</v>
       </c>
       <c r="L77" s="5" t="s">
-        <v>626</v>
+        <v>623</v>
       </c>
       <c r="M77" s="6" t="s">
         <v>170</v>
       </c>
       <c r="N77" s="3" t="s">
+        <v>537</v>
+      </c>
+      <c r="O77" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="P77" s="3" t="s">
+        <v>539</v>
+      </c>
+      <c r="Q77" s="3" t="s">
         <v>540</v>
       </c>
-      <c r="O77" s="3" t="s">
-        <v>541</v>
-      </c>
-      <c r="P77" s="3" t="s">
-        <v>542</v>
-      </c>
-      <c r="Q77" s="3" t="s">
-        <v>543</v>
-      </c>
-      <c r="R77" s="42" t="s">
+      <c r="R77" s="21" t="s">
         <v>246</v>
       </c>
       <c r="S77" s="32" t="s">
-        <v>627</v>
+        <v>624</v>
       </c>
       <c r="T77" s="32" t="s">
-        <v>633</v>
-      </c>
-    </row>
-    <row r="78" spans="1:20" x14ac:dyDescent="0.3">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="78" spans="1:20" ht="15" x14ac:dyDescent="0.3">
       <c r="A78" s="12" t="s">
         <v>181</v>
       </c>
@@ -6898,28 +7004,28 @@
         <v>170</v>
       </c>
       <c r="N78" s="3" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
       <c r="O78" s="3" t="s">
-        <v>562</v>
+        <v>559</v>
       </c>
       <c r="P78" s="3" t="s">
-        <v>563</v>
+        <v>560</v>
       </c>
       <c r="Q78" s="3" t="s">
-        <v>564</v>
-      </c>
-      <c r="R78" s="42" t="s">
+        <v>561</v>
+      </c>
+      <c r="R78" s="21" t="s">
         <v>246</v>
       </c>
       <c r="S78" s="32" t="s">
-        <v>627</v>
+        <v>624</v>
       </c>
       <c r="T78" s="32" t="s">
-        <v>633</v>
-      </c>
-    </row>
-    <row r="79" spans="1:20" x14ac:dyDescent="0.3">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="79" spans="1:20" ht="15" x14ac:dyDescent="0.3">
       <c r="A79" s="12" t="s">
         <v>183</v>
       </c>
@@ -6948,31 +7054,31 @@
         <v>184</v>
       </c>
       <c r="L79" s="5" t="s">
-        <v>628</v>
+        <v>625</v>
       </c>
       <c r="M79" s="6" t="s">
         <v>170</v>
       </c>
       <c r="N79" s="3" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
       <c r="O79" s="3" t="s">
-        <v>565</v>
+        <v>562</v>
       </c>
       <c r="P79" s="3" t="s">
-        <v>566</v>
+        <v>563</v>
       </c>
       <c r="Q79" s="3" t="s">
-        <v>567</v>
-      </c>
-      <c r="R79" s="42" t="s">
+        <v>564</v>
+      </c>
+      <c r="R79" s="21" t="s">
         <v>246</v>
       </c>
       <c r="S79" s="32" t="s">
-        <v>627</v>
+        <v>624</v>
       </c>
       <c r="T79" s="32" t="s">
-        <v>633</v>
+        <v>630</v>
       </c>
     </row>
     <row r="80" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
@@ -7010,25 +7116,25 @@
         <v>155</v>
       </c>
       <c r="N80" s="3" t="s">
-        <v>568</v>
+        <v>565</v>
       </c>
       <c r="O80" s="3" t="s">
-        <v>578</v>
+        <v>575</v>
       </c>
       <c r="P80" s="3" t="s">
-        <v>579</v>
+        <v>576</v>
       </c>
       <c r="Q80" s="3" t="s">
-        <v>580</v>
+        <v>577</v>
       </c>
       <c r="R80" s="21" t="s">
-        <v>602</v>
+        <v>599</v>
       </c>
       <c r="S80" s="21" t="s">
-        <v>607</v>
+        <v>604</v>
       </c>
       <c r="T80" s="32" t="s">
-        <v>633</v>
+        <v>630</v>
       </c>
     </row>
     <row r="81" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
@@ -7066,28 +7172,28 @@
         <v>84</v>
       </c>
       <c r="N81" s="3" t="s">
+        <v>565</v>
+      </c>
+      <c r="O81" s="3" t="s">
+        <v>566</v>
+      </c>
+      <c r="P81" s="3" t="s">
+        <v>567</v>
+      </c>
+      <c r="Q81" s="3" t="s">
         <v>568</v>
       </c>
-      <c r="O81" s="3" t="s">
-        <v>569</v>
-      </c>
-      <c r="P81" s="3" t="s">
-        <v>570</v>
-      </c>
-      <c r="Q81" s="3" t="s">
-        <v>571</v>
-      </c>
-      <c r="R81" s="42" t="s">
+      <c r="R81" s="21" t="s">
         <v>246</v>
       </c>
       <c r="S81" s="32" t="s">
-        <v>627</v>
+        <v>624</v>
       </c>
       <c r="T81" s="32" t="s">
-        <v>633</v>
-      </c>
-    </row>
-    <row r="82" spans="1:20" ht="26.4" x14ac:dyDescent="0.3">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="82" spans="1:20" ht="30" x14ac:dyDescent="0.3">
       <c r="A82" s="12" t="s">
         <v>196</v>
       </c>
@@ -7122,28 +7228,28 @@
         <v>222</v>
       </c>
       <c r="N82" s="3" t="s">
-        <v>568</v>
+        <v>565</v>
       </c>
       <c r="O82" s="3" t="s">
-        <v>575</v>
+        <v>572</v>
       </c>
       <c r="P82" s="3" t="s">
-        <v>576</v>
+        <v>573</v>
       </c>
       <c r="Q82" s="3" t="s">
-        <v>577</v>
-      </c>
-      <c r="R82" s="42" t="s">
+        <v>574</v>
+      </c>
+      <c r="R82" s="21" t="s">
         <v>246</v>
       </c>
       <c r="S82" s="32" t="s">
-        <v>619</v>
+        <v>616</v>
       </c>
       <c r="T82" s="32" t="s">
-        <v>633</v>
-      </c>
-    </row>
-    <row r="83" spans="1:20" x14ac:dyDescent="0.3">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="83" spans="1:20" ht="15" x14ac:dyDescent="0.3">
       <c r="A83" s="12" t="s">
         <v>197</v>
       </c>
@@ -7178,28 +7284,28 @@
         <v>135</v>
       </c>
       <c r="N83" s="3" t="s">
-        <v>568</v>
+        <v>565</v>
       </c>
       <c r="O83" s="3" t="s">
-        <v>572</v>
+        <v>569</v>
       </c>
       <c r="P83" s="3" t="s">
-        <v>573</v>
+        <v>570</v>
       </c>
       <c r="Q83" s="3" t="s">
-        <v>574</v>
-      </c>
-      <c r="R83" s="42" t="s">
+        <v>571</v>
+      </c>
+      <c r="R83" s="21" t="s">
         <v>246</v>
       </c>
       <c r="S83" s="32" t="s">
-        <v>619</v>
+        <v>616</v>
       </c>
       <c r="T83" s="32" t="s">
-        <v>633</v>
-      </c>
-    </row>
-    <row r="84" spans="1:20" x14ac:dyDescent="0.3">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="84" spans="1:20" ht="15" x14ac:dyDescent="0.3">
       <c r="A84" s="12" t="s">
         <v>108</v>
       </c>
@@ -7219,7 +7325,7 @@
         <v>246</v>
       </c>
       <c r="G84" s="3" t="s">
-        <v>629</v>
+        <v>626</v>
       </c>
       <c r="H84" s="16"/>
       <c r="I84" s="16"/>
@@ -7234,28 +7340,28 @@
         <v>111</v>
       </c>
       <c r="N84" s="3" t="s">
-        <v>581</v>
+        <v>578</v>
       </c>
       <c r="O84" s="3" t="s">
-        <v>597</v>
+        <v>594</v>
       </c>
       <c r="P84" s="3" t="s">
-        <v>598</v>
+        <v>595</v>
       </c>
       <c r="Q84" s="3" t="s">
-        <v>599</v>
-      </c>
-      <c r="R84" s="42" t="s">
+        <v>596</v>
+      </c>
+      <c r="R84" s="21" t="s">
         <v>246</v>
       </c>
       <c r="S84" s="32" t="s">
-        <v>603</v>
+        <v>600</v>
       </c>
       <c r="T84" s="32" t="s">
-        <v>633</v>
-      </c>
-    </row>
-    <row r="85" spans="1:20" x14ac:dyDescent="0.3">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="85" spans="1:20" ht="15" x14ac:dyDescent="0.3">
       <c r="A85" s="12" t="s">
         <v>112</v>
       </c>
@@ -7275,7 +7381,7 @@
         <v>246</v>
       </c>
       <c r="G85" s="3" t="s">
-        <v>630</v>
+        <v>627</v>
       </c>
       <c r="H85" s="16"/>
       <c r="I85" s="16"/>
@@ -7290,25 +7396,25 @@
         <v>84</v>
       </c>
       <c r="N85" s="3" t="s">
-        <v>581</v>
+        <v>578</v>
       </c>
       <c r="O85" s="3" t="s">
-        <v>594</v>
+        <v>591</v>
       </c>
       <c r="P85" s="3" t="s">
-        <v>595</v>
+        <v>592</v>
       </c>
       <c r="Q85" s="3" t="s">
-        <v>596</v>
-      </c>
-      <c r="R85" s="42" t="s">
+        <v>593</v>
+      </c>
+      <c r="R85" s="21" t="s">
         <v>246</v>
       </c>
       <c r="S85" s="32" t="s">
-        <v>603</v>
+        <v>600</v>
       </c>
       <c r="T85" s="32" t="s">
-        <v>633</v>
+        <v>630</v>
       </c>
     </row>
     <row r="86" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
@@ -7331,7 +7437,7 @@
         <v>246</v>
       </c>
       <c r="G86" s="3" t="s">
-        <v>631</v>
+        <v>628</v>
       </c>
       <c r="H86" s="16"/>
       <c r="I86" s="16"/>
@@ -7346,28 +7452,28 @@
         <v>84</v>
       </c>
       <c r="N86" s="3" t="s">
-        <v>581</v>
+        <v>578</v>
       </c>
       <c r="O86" s="3" t="s">
-        <v>588</v>
+        <v>585</v>
       </c>
       <c r="P86" s="3" t="s">
-        <v>589</v>
+        <v>586</v>
       </c>
       <c r="Q86" s="3" t="s">
-        <v>590</v>
-      </c>
-      <c r="R86" s="42" t="s">
+        <v>587</v>
+      </c>
+      <c r="R86" s="21" t="s">
         <v>246</v>
       </c>
       <c r="S86" s="32" t="s">
-        <v>603</v>
+        <v>600</v>
       </c>
       <c r="T86" s="32" t="s">
-        <v>633</v>
-      </c>
-    </row>
-    <row r="87" spans="1:20" x14ac:dyDescent="0.3">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="87" spans="1:20" ht="15" x14ac:dyDescent="0.3">
       <c r="A87" s="12" t="s">
         <v>118</v>
       </c>
@@ -7387,7 +7493,7 @@
         <v>246</v>
       </c>
       <c r="G87" s="3" t="s">
-        <v>632</v>
+        <v>629</v>
       </c>
       <c r="H87" s="16"/>
       <c r="I87" s="16"/>
@@ -7402,28 +7508,28 @@
         <v>84</v>
       </c>
       <c r="N87" s="3" t="s">
-        <v>581</v>
+        <v>578</v>
       </c>
       <c r="O87" s="3" t="s">
-        <v>591</v>
+        <v>588</v>
       </c>
       <c r="P87" s="3" t="s">
-        <v>592</v>
+        <v>589</v>
       </c>
       <c r="Q87" s="3" t="s">
-        <v>593</v>
-      </c>
-      <c r="R87" s="42" t="s">
+        <v>590</v>
+      </c>
+      <c r="R87" s="21" t="s">
         <v>246</v>
       </c>
       <c r="S87" s="32" t="s">
-        <v>603</v>
+        <v>600</v>
       </c>
       <c r="T87" s="32" t="s">
-        <v>633</v>
-      </c>
-    </row>
-    <row r="88" spans="1:20" ht="26.4" x14ac:dyDescent="0.3">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="88" spans="1:20" ht="30" x14ac:dyDescent="0.3">
       <c r="A88" s="12" t="s">
         <v>121</v>
       </c>
@@ -7458,28 +7564,28 @@
         <v>209</v>
       </c>
       <c r="N88" s="3" t="s">
+        <v>578</v>
+      </c>
+      <c r="O88" s="3" t="s">
+        <v>579</v>
+      </c>
+      <c r="P88" s="3" t="s">
+        <v>580</v>
+      </c>
+      <c r="Q88" s="3" t="s">
         <v>581</v>
       </c>
-      <c r="O88" s="3" t="s">
-        <v>582</v>
-      </c>
-      <c r="P88" s="3" t="s">
-        <v>583</v>
-      </c>
-      <c r="Q88" s="3" t="s">
-        <v>584</v>
-      </c>
       <c r="R88" s="21" t="s">
-        <v>602</v>
+        <v>599</v>
       </c>
       <c r="S88" s="32" t="s">
-        <v>607</v>
+        <v>604</v>
       </c>
       <c r="T88" s="32" t="s">
-        <v>633</v>
-      </c>
-    </row>
-    <row r="89" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="89" spans="1:20" ht="30" x14ac:dyDescent="0.3">
       <c r="A89" s="12" t="s">
         <v>123</v>
       </c>
@@ -7514,25 +7620,373 @@
         <v>210</v>
       </c>
       <c r="N89" s="3" t="s">
-        <v>581</v>
+        <v>578</v>
       </c>
       <c r="O89" s="3" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="P89" s="3" t="s">
-        <v>586</v>
+        <v>583</v>
       </c>
       <c r="Q89" s="3" t="s">
-        <v>587</v>
+        <v>584</v>
       </c>
       <c r="R89" s="21" t="s">
-        <v>602</v>
+        <v>599</v>
       </c>
       <c r="S89" s="32" t="s">
-        <v>607</v>
+        <v>604</v>
       </c>
       <c r="T89" s="32" t="s">
-        <v>633</v>
+        <v>630</v>
+      </c>
+    </row>
+    <row r="90" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A90" s="10" t="s">
+        <v>636</v>
+      </c>
+      <c r="B90" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="C90" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="D90" s="18" t="s">
+        <v>224</v>
+      </c>
+      <c r="E90" s="10" t="s">
+        <v>245</v>
+      </c>
+      <c r="F90" s="10" t="s">
+        <v>246</v>
+      </c>
+      <c r="G90" s="3" t="s">
+        <v>276</v>
+      </c>
+      <c r="H90" s="15">
+        <v>41640</v>
+      </c>
+      <c r="I90" s="15">
+        <v>45689</v>
+      </c>
+      <c r="J90" s="3"/>
+      <c r="K90" s="3"/>
+      <c r="L90" s="42" t="s">
+        <v>635</v>
+      </c>
+      <c r="M90" s="42" t="s">
+        <v>635</v>
+      </c>
+      <c r="N90" s="3" t="s">
+        <v>412</v>
+      </c>
+      <c r="O90" s="3" t="s">
+        <v>637</v>
+      </c>
+      <c r="P90" s="3" t="s">
+        <v>638</v>
+      </c>
+      <c r="Q90" s="3" t="s">
+        <v>639</v>
+      </c>
+      <c r="R90" s="21" t="s">
+        <v>246</v>
+      </c>
+      <c r="S90" s="21" t="s">
+        <v>604</v>
+      </c>
+      <c r="T90" s="21" t="s">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="91" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A91" s="11" t="s">
+        <v>640</v>
+      </c>
+      <c r="B91" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="C91" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="D91" s="18" t="s">
+        <v>224</v>
+      </c>
+      <c r="E91" s="10" t="s">
+        <v>245</v>
+      </c>
+      <c r="F91" s="10" t="s">
+        <v>246</v>
+      </c>
+      <c r="G91" s="3" t="s">
+        <v>276</v>
+      </c>
+      <c r="H91" s="15">
+        <v>41640</v>
+      </c>
+      <c r="I91" s="15">
+        <v>45689</v>
+      </c>
+      <c r="J91" s="3"/>
+      <c r="K91" s="3"/>
+      <c r="L91" s="42" t="s">
+        <v>642</v>
+      </c>
+      <c r="M91" t="s">
+        <v>641</v>
+      </c>
+      <c r="N91" s="3" t="s">
+        <v>412</v>
+      </c>
+      <c r="O91" s="3" t="s">
+        <v>643</v>
+      </c>
+      <c r="P91" s="3" t="s">
+        <v>644</v>
+      </c>
+      <c r="Q91" s="3" t="s">
+        <v>645</v>
+      </c>
+      <c r="R91" s="21" t="s">
+        <v>246</v>
+      </c>
+      <c r="S91" s="21" t="s">
+        <v>604</v>
+      </c>
+      <c r="T91" s="21" t="s">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="92" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A92" s="11" t="s">
+        <v>646</v>
+      </c>
+      <c r="B92" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="C92" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="D92" s="18" t="s">
+        <v>224</v>
+      </c>
+      <c r="E92" s="10" t="s">
+        <v>245</v>
+      </c>
+      <c r="F92" s="10" t="s">
+        <v>246</v>
+      </c>
+      <c r="G92" s="3" t="s">
+        <v>276</v>
+      </c>
+      <c r="H92" s="15">
+        <v>41640</v>
+      </c>
+      <c r="I92" s="15">
+        <v>45689</v>
+      </c>
+      <c r="J92" s="3"/>
+      <c r="K92" s="3"/>
+      <c r="L92" s="42" t="s">
+        <v>648</v>
+      </c>
+      <c r="M92" t="s">
+        <v>647</v>
+      </c>
+      <c r="N92" s="3" t="s">
+        <v>412</v>
+      </c>
+      <c r="O92" s="3" t="s">
+        <v>649</v>
+      </c>
+      <c r="P92" s="3" t="s">
+        <v>650</v>
+      </c>
+      <c r="Q92" s="3" t="s">
+        <v>651</v>
+      </c>
+      <c r="R92" s="21" t="s">
+        <v>246</v>
+      </c>
+      <c r="S92" s="21" t="s">
+        <v>604</v>
+      </c>
+      <c r="T92" s="21" t="s">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="93" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A93" s="11" t="s">
+        <v>652</v>
+      </c>
+      <c r="B93" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="C93" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="D93" s="18" t="s">
+        <v>224</v>
+      </c>
+      <c r="E93" s="10" t="s">
+        <v>245</v>
+      </c>
+      <c r="F93" s="10" t="s">
+        <v>246</v>
+      </c>
+      <c r="G93" s="3" t="s">
+        <v>276</v>
+      </c>
+      <c r="H93" s="15">
+        <v>41640</v>
+      </c>
+      <c r="I93" s="15">
+        <v>45689</v>
+      </c>
+      <c r="J93" s="3"/>
+      <c r="K93" s="3"/>
+      <c r="L93" s="42" t="s">
+        <v>654</v>
+      </c>
+      <c r="M93" t="s">
+        <v>653</v>
+      </c>
+      <c r="N93" s="3" t="s">
+        <v>412</v>
+      </c>
+      <c r="O93" s="3" t="s">
+        <v>655</v>
+      </c>
+      <c r="P93" s="3" t="s">
+        <v>656</v>
+      </c>
+      <c r="Q93" s="3" t="s">
+        <v>657</v>
+      </c>
+      <c r="R93" s="21" t="s">
+        <v>246</v>
+      </c>
+      <c r="S93" s="21" t="s">
+        <v>604</v>
+      </c>
+      <c r="T93" s="21" t="s">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="94" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A94" s="11" t="s">
+        <v>658</v>
+      </c>
+      <c r="B94" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="C94" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="D94" s="18" t="s">
+        <v>224</v>
+      </c>
+      <c r="E94" s="10" t="s">
+        <v>245</v>
+      </c>
+      <c r="F94" s="10" t="s">
+        <v>246</v>
+      </c>
+      <c r="G94" s="3" t="s">
+        <v>276</v>
+      </c>
+      <c r="H94" s="15">
+        <v>41640</v>
+      </c>
+      <c r="I94" s="15">
+        <v>45689</v>
+      </c>
+      <c r="J94" s="3"/>
+      <c r="K94" s="3"/>
+      <c r="L94" s="42" t="s">
+        <v>660</v>
+      </c>
+      <c r="M94" t="s">
+        <v>659</v>
+      </c>
+      <c r="N94" s="3" t="s">
+        <v>412</v>
+      </c>
+      <c r="O94" s="3" t="s">
+        <v>661</v>
+      </c>
+      <c r="P94" s="3" t="s">
+        <v>662</v>
+      </c>
+      <c r="Q94" s="3" t="s">
+        <v>663</v>
+      </c>
+      <c r="R94" s="21" t="s">
+        <v>246</v>
+      </c>
+      <c r="S94" s="21" t="s">
+        <v>604</v>
+      </c>
+      <c r="T94" s="21" t="s">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="95" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A95" s="11" t="s">
+        <v>664</v>
+      </c>
+      <c r="B95" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="C95" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="D95" s="18" t="s">
+        <v>224</v>
+      </c>
+      <c r="E95" s="10" t="s">
+        <v>245</v>
+      </c>
+      <c r="F95" s="10" t="s">
+        <v>246</v>
+      </c>
+      <c r="G95" s="3" t="s">
+        <v>276</v>
+      </c>
+      <c r="H95" s="15">
+        <v>41640</v>
+      </c>
+      <c r="I95" s="15">
+        <v>45689</v>
+      </c>
+      <c r="J95" s="3"/>
+      <c r="K95" s="3"/>
+      <c r="L95" s="42" t="s">
+        <v>666</v>
+      </c>
+      <c r="M95" t="s">
+        <v>665</v>
+      </c>
+      <c r="N95" s="3" t="s">
+        <v>412</v>
+      </c>
+      <c r="O95" s="3" t="s">
+        <v>667</v>
+      </c>
+      <c r="P95" s="3" t="s">
+        <v>668</v>
+      </c>
+      <c r="Q95" s="3" t="s">
+        <v>669</v>
+      </c>
+      <c r="R95" s="21" t="s">
+        <v>246</v>
+      </c>
+      <c r="S95" s="21" t="s">
+        <v>604</v>
+      </c>
+      <c r="T95" s="21" t="s">
+        <v>630</v>
       </c>
     </row>
   </sheetData>
@@ -7633,8 +8087,15 @@
     <hyperlink ref="L89" r:id="rId93" xr:uid="{E1D67341-068F-460F-8EC6-1E8AB5C9CB74}"/>
     <hyperlink ref="L57" r:id="rId94" xr:uid="{08D74033-9789-4868-8A38-4B01DACE2D96}"/>
     <hyperlink ref="L24" r:id="rId95" xr:uid="{F51C49C1-7ECD-4D04-8C8A-796C03F66464}"/>
+    <hyperlink ref="L90" r:id="rId96" xr:uid="{847A7018-4A2B-4D67-BEAF-62A1C5D42509}"/>
+    <hyperlink ref="M90" r:id="rId97" xr:uid="{ADCF6B15-F291-4078-98D4-9E64E57F7E50}"/>
+    <hyperlink ref="L91" r:id="rId98" xr:uid="{1793FF7C-DB0C-4E11-B329-FD5BC976324A}"/>
+    <hyperlink ref="L92" r:id="rId99" xr:uid="{00E0DD28-054B-4FF7-B70A-5E51FEC9D020}"/>
+    <hyperlink ref="L93" r:id="rId100" xr:uid="{CF992DDA-3871-4DF0-A0A0-273E4A564931}"/>
+    <hyperlink ref="L94" r:id="rId101" xr:uid="{27E0434D-4BA2-4343-80A9-7D55242EE307}"/>
+    <hyperlink ref="L95" r:id="rId102" xr:uid="{77714CE7-D72A-44AE-8092-82C467917C5B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId96"/>
+  <pageSetup orientation="portrait" r:id="rId103"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Se añadieron 26 Nuevos mercados
</commit_message>
<xml_diff>
--- a/pipelines/Data Engineering.xlsx
+++ b/pipelines/Data Engineering.xlsx
@@ -1,34 +1,46 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27932"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\saule\Desktop\Pipeline\Mayo3\SP500_INDEX_Analisis\pipelines\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\natus\Documents\Trabajo\PEDRO_PEREZ\Proyecto_Mercado_de_Valores\SP500_INDEX_Analisis\pipelines\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C56295EA-DBB2-4711-B4E6-40817E32ECCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AB75324-88DA-4BC4-81F4-14E7D7A04927}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{AF709C27-429E-478E-9AB0-B8CF25FE9941}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$Q$89</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1596" uniqueCount="670">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1852" uniqueCount="724">
   <si>
     <t>Variable</t>
   </si>
@@ -1966,9 +1978,6 @@
     <t>Data/Macro/raw/commodities/Aluminium_Spot.csv</t>
   </si>
   <si>
-    <t>C:\Users\pedro\OneDrive\Documents\ALGO TRADING\SP500 INDEX\Data/Macro/raw/commodities/Aluminium_Spot.csv</t>
-  </si>
-  <si>
     <t>/mnt/c/Users/pedro/OneDrive/Documents/ALGO TRADING/SP500 INDEX/Data/Macro/raw/commodities/Aluminium_Spot.csv</t>
   </si>
   <si>
@@ -1984,9 +1993,6 @@
     <t>Data/Macro/raw/commodities/Lead_Futures.csv</t>
   </si>
   <si>
-    <t>C:\Users\pedro\OneDrive\Documents\ALGO TRADING\SP500 INDEX\Data/Macro/raw/commodities/Lead_Futures.csv</t>
-  </si>
-  <si>
     <t>/mnt/c/Users/pedro/OneDrive/Documents/ALGO TRADING/SP500 INDEX/Data/Macro/raw/commodities/Lead_Futures.csv</t>
   </si>
   <si>
@@ -2002,9 +2008,6 @@
     <t>Data/Macro/raw/commodities/Palladium_Futures.csv</t>
   </si>
   <si>
-    <t>C:\Users\pedro\OneDrive\Documents\ALGO TRADING\SP500 INDEX\Data/Macro/raw/commodities/Palladium_Futures.csv</t>
-  </si>
-  <si>
     <t>/mnt/c/Users/pedro/OneDrive/Documents/ALGO TRADING/SP500 INDEX/Data/Macro/raw/commodities/Palladium_Futures.csv</t>
   </si>
   <si>
@@ -2020,9 +2023,6 @@
     <t>Data/Macro/raw/commodities/Tin_Futures.csv</t>
   </si>
   <si>
-    <t>C:\Users\pedro\OneDrive\Documents\ALGO TRADING\SP500 INDEX\Data/Macro/raw/commodities/Tin_Futures.csv</t>
-  </si>
-  <si>
     <t>/mnt/c/Users/pedro/OneDrive/Documents/ALGO TRADING/SP500 INDEX/Data/Macro/raw/commodities/Tin_Futures.csv</t>
   </si>
   <si>
@@ -2038,9 +2038,6 @@
     <t>Data/Macro/raw/commodities/Zinc_Futures.csv</t>
   </si>
   <si>
-    <t>C:\Users\pedro\OneDrive\Documents\ALGO TRADING\SP500 INDEX\Data/Macro/raw/commodities/Zinc_Futures.csv</t>
-  </si>
-  <si>
     <t>/mnt/c/Users/pedro/OneDrive/Documents/ALGO TRADING/SP500 INDEX/Data/Macro/raw/commodities/Zinc_Futures.csv</t>
   </si>
   <si>
@@ -2056,17 +2053,194 @@
     <t>Data/Macro/raw/commodities/Nickel_Futures.csv</t>
   </si>
   <si>
-    <t>C:\Users\pedro\OneDrive\Documents\ALGO TRADING\SP500 INDEX\Data/Macro/raw/commodities/Nickel_Futures.csv</t>
-  </si>
-  <si>
     <t>/mnt/c/Users/pedro/OneDrive/Documents/ALGO TRADING/SP500 INDEX/Data/Macro/raw/commodities/Nickel_Futures.csv</t>
+  </si>
+  <si>
+    <t>Lumber_Futures</t>
+  </si>
+  <si>
+    <t>US_Cocoa_Futures</t>
+  </si>
+  <si>
+    <t>US_Coffee_C_Futures</t>
+  </si>
+  <si>
+    <t>Orange_Juice_Futures</t>
+  </si>
+  <si>
+    <t>US_Sugar</t>
+  </si>
+  <si>
+    <t>US_Corn_Futures</t>
+  </si>
+  <si>
+    <t>US_Wheat_Futures</t>
+  </si>
+  <si>
+    <t>Oats_Futures</t>
+  </si>
+  <si>
+    <t>Rough_Rice_Futures</t>
+  </si>
+  <si>
+    <t>US_Soybean_Meal_Futures</t>
+  </si>
+  <si>
+    <t>US_Soybean_Oil_Futures</t>
+  </si>
+  <si>
+    <t>US_Soybeans_Futures</t>
+  </si>
+  <si>
+    <t>Feeder_Cattle_Futures</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Lean_Hogs_Futures</t>
+  </si>
+  <si>
+    <t>Live_Cattle_Futures</t>
+  </si>
+  <si>
+    <t>Iron_ore_fines_62%_Fe_CFR_Futures</t>
+  </si>
+  <si>
+    <t>US_Cotton_#2_Futures</t>
+  </si>
+  <si>
+    <t>https://www.investing.com/commodities/us-cotton-no.2-historical-data</t>
+  </si>
+  <si>
+    <t>https://www.investing.com/commodities/lumber-historical-data</t>
+  </si>
+  <si>
+    <t>https://www.investing.com/commodities/us-cocoa-historical-data</t>
+  </si>
+  <si>
+    <t>https://www.investing.com/commodities/us-coffee-c-historical-data</t>
+  </si>
+  <si>
+    <t>https://www.investing.com/commodities/orange-juice-historical-data</t>
+  </si>
+  <si>
+    <t>https://www.investing.com/commodities/us-soybean-oil-historical-data</t>
+  </si>
+  <si>
+    <t>https://www.investing.com/commodities/feed-cattle-historical-data</t>
+  </si>
+  <si>
+    <t>www.investing.com/commodities/lean-hogs-historical-data</t>
+  </si>
+  <si>
+    <t>https://www.investing.com/commodities/live-cattle-historical-data</t>
+  </si>
+  <si>
+    <t>https://www.investing.com/commodities/iron-ore-62-cfr-futures-historical-data</t>
+  </si>
+  <si>
+    <t>https://www.investing.com/commodities/us-sugar-no11-historical-data</t>
+  </si>
+  <si>
+    <t>https://www.investing.com/commodities/us-corn-historical-data</t>
+  </si>
+  <si>
+    <t>https://www.investing.com/commodities/us-wheat-historical-data</t>
+  </si>
+  <si>
+    <t>https://www.investing.com/commodities/oats-historical-data</t>
+  </si>
+  <si>
+    <t>https://www.investing.com/commodities/rough-rice-historical-data</t>
+  </si>
+  <si>
+    <t>https://www.investing.com/commodities/us-soybean-meal-historical-data</t>
+  </si>
+  <si>
+    <t>https://www.investing.com/commodities/us-soybeans-historical-data</t>
+  </si>
+  <si>
+    <t>Dow_Jones_Industrial_Average</t>
+  </si>
+  <si>
+    <t>Nasdaq_100_Fi</t>
+  </si>
+  <si>
+    <t>CAC_40</t>
+  </si>
+  <si>
+    <t>https://www.investing.com/indices/us-30-historical-data</t>
+  </si>
+  <si>
+    <t>https://www.investing.com/funds/es0165265002-historical-data</t>
+  </si>
+  <si>
+    <t>https://www.investing.com/indices/france-40-historical-data</t>
+  </si>
+  <si>
+    <t>JPY_EUR</t>
+  </si>
+  <si>
+    <t>BRL_NZD</t>
+  </si>
+  <si>
+    <t>NOK_AUD</t>
+  </si>
+  <si>
+    <t>PHP_ZAR</t>
+  </si>
+  <si>
+    <t>https://www.investing.com/currencies/jpy-eur</t>
+  </si>
+  <si>
+    <t>https://www.investing.com/currencies/usd-gbp-historical-data</t>
+  </si>
+  <si>
+    <t>https://www.investing.com/currencies/brl-nzd-historical-data</t>
+  </si>
+  <si>
+    <t>https://www.investing.com/currencies/nok-aud-historical-data</t>
+  </si>
+  <si>
+    <t>https://www.investing.com/currencies/php-zar-historical-data</t>
+  </si>
+  <si>
+    <t>Prefijo_ruta_raw</t>
+  </si>
+  <si>
+    <t>Data/Macro/raw/</t>
+  </si>
+  <si>
+    <t>C:\Users\pedro\OneDrive\Documents\ALGO TRADING\SP500 INDEX\Data\Macro\raw\</t>
+  </si>
+  <si>
+    <t>C:\Users\pedro\OneDrive\Documents\ALGO TRADING\SP500 INDEX\Data\Macro\raw\commodities\Aluminium_Spot.csv</t>
+  </si>
+  <si>
+    <t>C:\Users\pedro\OneDrive\Documents\ALGO TRADING\SP500 INDEX\Data\Macro\raw\commodities\Palladium_Futures.csv</t>
+  </si>
+  <si>
+    <t>C:\Users\pedro\OneDrive\Documents\ALGO TRADING\SP500 INDEX\Data\Macro\raw\commodities\Lead_Futures.csv</t>
+  </si>
+  <si>
+    <t>C:\Users\pedro\OneDrive\Documents\ALGO TRADING\SP500 INDEX\Data\Macro\raw\commodities\Zinc_Futures.csv</t>
+  </si>
+  <si>
+    <t>C:\Users\pedro\OneDrive\Documents\ALGO TRADING\SP500 INDEX\Data\Macro\raw\commodities\Tin_Futures.csv</t>
+  </si>
+  <si>
+    <t>C:\Users\pedro\OneDrive\Documents\ALGO TRADING\SP500 INDEX\Data\Macro\raw\commodities\Nickel_Futures.csv</t>
+  </si>
+  <si>
+    <t>Prefijo_ruta_windows</t>
+  </si>
+  <si>
+    <t>/mnt/c/Users/pedro/OneDrive/Documents/ALGO TRADING/SP500 INDEX/Data/Macro/raw/</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2146,7 +2320,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -2189,12 +2363,25 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2296,6 +2483,25 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -2631,13 +2837,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CB0844A-40A1-4264-8968-9E5B325C5351}">
-  <dimension ref="A1:T95"/>
+  <dimension ref="A1:T121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A96" sqref="A96"/>
+    <sheetView tabSelected="1" topLeftCell="A94" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C116" sqref="C116:C120"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="37.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="37.5546875" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="2" width="37.5546875" style="11"/>
     <col min="3" max="3" width="37.88671875" style="11" bestFit="1" customWidth="1"/>
@@ -2651,7 +2857,7 @@
     <col min="17" max="17" width="130.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2713,7 +2919,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="2" spans="1:20" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:20" ht="100.8">
       <c r="A2" s="12" t="s">
         <v>5</v>
       </c>
@@ -2775,7 +2981,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="3" spans="1:20" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:20" ht="100.8">
       <c r="A3" s="12" t="s">
         <v>9</v>
       </c>
@@ -2837,7 +3043,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="4" spans="1:20" ht="15" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:20">
       <c r="A4" s="12" t="s">
         <v>12</v>
       </c>
@@ -2893,7 +3099,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="5" spans="1:20" ht="15" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:20">
       <c r="A5" s="12" t="s">
         <v>15</v>
       </c>
@@ -2949,7 +3155,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="6" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:20" ht="28.8">
       <c r="A6" s="12" t="s">
         <v>17</v>
       </c>
@@ -3005,7 +3211,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="7" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:20" ht="28.8">
       <c r="A7" s="12" t="s">
         <v>19</v>
       </c>
@@ -3061,7 +3267,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="8" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:20" ht="28.8">
       <c r="A8" s="12" t="s">
         <v>21</v>
       </c>
@@ -3117,7 +3323,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="9" spans="1:20" ht="15" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:20">
       <c r="A9" s="12" t="s">
         <v>23</v>
       </c>
@@ -3173,7 +3379,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="10" spans="1:20" ht="15" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:20">
       <c r="A10" s="12" t="s">
         <v>25</v>
       </c>
@@ -3229,7 +3435,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="11" spans="1:20" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:20" ht="115.2">
       <c r="A11" s="12" t="s">
         <v>27</v>
       </c>
@@ -3291,7 +3497,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="12" spans="1:20" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:20" ht="100.8">
       <c r="A12" s="12" t="s">
         <v>30</v>
       </c>
@@ -3353,7 +3559,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="13" spans="1:20" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:20" ht="115.2">
       <c r="A13" s="12" t="s">
         <v>33</v>
       </c>
@@ -3415,7 +3621,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="14" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:20" ht="28.8">
       <c r="A14" s="12" t="s">
         <v>185</v>
       </c>
@@ -3471,7 +3677,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="15" spans="1:20" ht="15" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:20">
       <c r="A15" s="12" t="s">
         <v>187</v>
       </c>
@@ -3527,7 +3733,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="16" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:20" ht="28.8">
       <c r="A16" s="12" t="s">
         <v>189</v>
       </c>
@@ -3583,7 +3789,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="17" spans="1:20" s="41" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:20" s="41" customFormat="1" ht="28.8">
       <c r="A17" s="12" t="s">
         <v>191</v>
       </c>
@@ -3637,7 +3843,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="18" spans="1:20" ht="15" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:20">
       <c r="A18" s="12" t="s">
         <v>194</v>
       </c>
@@ -3693,7 +3899,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="19" spans="1:20" s="30" customFormat="1" ht="15" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:20" s="30" customFormat="1">
       <c r="A19" s="23" t="s">
         <v>248</v>
       </c>
@@ -3743,7 +3949,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="20" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:20" ht="28.8">
       <c r="A20" s="12" t="s">
         <v>227</v>
       </c>
@@ -3799,7 +4005,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="21" spans="1:20" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:20" ht="129.6">
       <c r="A21" s="12" t="s">
         <v>256</v>
       </c>
@@ -3857,7 +4063,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="22" spans="1:20" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:20" ht="129.6">
       <c r="A22" s="12" t="s">
         <v>258</v>
       </c>
@@ -3915,7 +4121,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="23" spans="1:20" ht="15" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:20" ht="15">
       <c r="A23" s="12" t="s">
         <v>262</v>
       </c>
@@ -3967,7 +4173,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="24" spans="1:20" ht="15" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:20" ht="15">
       <c r="A24" s="12" t="s">
         <v>264</v>
       </c>
@@ -4019,7 +4225,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="25" spans="1:20" ht="15" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:20" ht="15">
       <c r="A25" s="12" t="s">
         <v>260</v>
       </c>
@@ -4071,7 +4277,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="26" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:20" ht="28.8">
       <c r="A26" s="12" t="s">
         <v>139</v>
       </c>
@@ -4127,7 +4333,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="27" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:20" ht="28.8">
       <c r="A27" s="12" t="s">
         <v>143</v>
       </c>
@@ -4183,7 +4389,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="28" spans="1:20" ht="15" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:20">
       <c r="A28" s="12" t="s">
         <v>145</v>
       </c>
@@ -4239,7 +4445,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="29" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:20" ht="28.8">
       <c r="A29" s="12" t="s">
         <v>57</v>
       </c>
@@ -4295,7 +4501,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="30" spans="1:20" ht="15" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:20">
       <c r="A30" s="12" t="s">
         <v>60</v>
       </c>
@@ -4351,7 +4557,7 @@
         <v>631</v>
       </c>
     </row>
-    <row r="31" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:20" ht="28.8">
       <c r="A31" s="12" t="s">
         <v>62</v>
       </c>
@@ -4407,7 +4613,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="32" spans="1:20" ht="15" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:20">
       <c r="A32" s="12" t="s">
         <v>64</v>
       </c>
@@ -4463,7 +4669,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="33" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:20" ht="28.8">
       <c r="A33" s="12" t="s">
         <v>66</v>
       </c>
@@ -4519,7 +4725,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="34" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:20" ht="28.8">
       <c r="A34" s="12" t="s">
         <v>125</v>
       </c>
@@ -4575,7 +4781,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="35" spans="1:20" ht="15" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:20">
       <c r="A35" s="12" t="s">
         <v>267</v>
       </c>
@@ -4631,7 +4837,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="36" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:20" ht="28.8">
       <c r="A36" s="12" t="s">
         <v>128</v>
       </c>
@@ -4687,7 +4893,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="37" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:20" ht="28.8">
       <c r="A37" s="12" t="s">
         <v>129</v>
       </c>
@@ -4743,7 +4949,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="38" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:20" ht="28.8">
       <c r="A38" s="12" t="s">
         <v>132</v>
       </c>
@@ -4792,7 +4998,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="39" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:20" ht="28.8">
       <c r="A39" s="12" t="s">
         <v>272</v>
       </c>
@@ -4841,7 +5047,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="40" spans="1:20" ht="15" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:20">
       <c r="A40" s="12" t="s">
         <v>68</v>
       </c>
@@ -4897,7 +5103,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="41" spans="1:20" ht="15" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:20">
       <c r="A41" s="12" t="s">
         <v>72</v>
       </c>
@@ -4953,7 +5159,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="42" spans="1:20" ht="15" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:20">
       <c r="A42" s="12" t="s">
         <v>75</v>
       </c>
@@ -5009,7 +5215,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="43" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:20" ht="28.8">
       <c r="A43" s="12" t="s">
         <v>78</v>
       </c>
@@ -5065,7 +5271,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="44" spans="1:20" ht="15" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:20">
       <c r="A44" s="12" t="s">
         <v>81</v>
       </c>
@@ -5121,7 +5327,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="45" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:20" ht="28.8">
       <c r="A45" s="12" t="s">
         <v>85</v>
       </c>
@@ -5177,7 +5383,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="46" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:20" ht="28.8">
       <c r="A46" s="12" t="s">
         <v>250</v>
       </c>
@@ -5233,7 +5439,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="47" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:20" ht="28.8">
       <c r="A47" s="12" t="s">
         <v>251</v>
       </c>
@@ -5289,7 +5495,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="48" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:20" ht="28.8">
       <c r="A48" s="12" t="s">
         <v>252</v>
       </c>
@@ -5345,7 +5551,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="49" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:20">
       <c r="A49" s="12" t="s">
         <v>253</v>
       </c>
@@ -5401,7 +5607,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="50" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:20" ht="28.8">
       <c r="A50" s="12" t="s">
         <v>254</v>
       </c>
@@ -5457,7 +5663,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="51" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:20" ht="28.8">
       <c r="A51" s="12" t="s">
         <v>94</v>
       </c>
@@ -5513,7 +5719,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="52" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:20" ht="28.8">
       <c r="A52" s="12" t="s">
         <v>97</v>
       </c>
@@ -5569,7 +5775,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="53" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:20" ht="28.8">
       <c r="A53" s="12" t="s">
         <v>99</v>
       </c>
@@ -5625,7 +5831,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="54" spans="1:20" ht="15" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:20">
       <c r="A54" s="12" t="s">
         <v>102</v>
       </c>
@@ -5681,7 +5887,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="55" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:20" ht="28.8">
       <c r="A55" s="12" t="s">
         <v>105</v>
       </c>
@@ -5737,7 +5943,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="56" spans="1:20" ht="15" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:20" ht="15">
       <c r="A56" s="12" t="s">
         <v>159</v>
       </c>
@@ -5793,7 +5999,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="57" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:20" ht="28.8">
       <c r="A57" s="12" t="s">
         <v>162</v>
       </c>
@@ -5849,7 +6055,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="58" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:20" ht="28.8">
       <c r="A58" s="12" t="s">
         <v>163</v>
       </c>
@@ -5905,7 +6111,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="59" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:20" ht="28.8">
       <c r="A59" s="12" t="s">
         <v>165</v>
       </c>
@@ -5961,7 +6167,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="60" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:20" ht="28.8">
       <c r="A60" s="12" t="s">
         <v>255</v>
       </c>
@@ -6017,7 +6223,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="61" spans="1:20" ht="15" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:20">
       <c r="A61" s="12" t="s">
         <v>36</v>
       </c>
@@ -6073,7 +6279,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="62" spans="1:20" ht="15" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:20">
       <c r="A62" s="12" t="s">
         <v>39</v>
       </c>
@@ -6129,7 +6335,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="63" spans="1:20" ht="15" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:20">
       <c r="A63" s="12" t="s">
         <v>41</v>
       </c>
@@ -6185,7 +6391,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="64" spans="1:20" ht="15" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:20">
       <c r="A64" s="12" t="s">
         <v>43</v>
       </c>
@@ -6241,7 +6447,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="65" spans="1:20" ht="15" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:20">
       <c r="A65" s="12" t="s">
         <v>45</v>
       </c>
@@ -6297,7 +6503,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="66" spans="1:20" ht="15" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:20">
       <c r="A66" s="12" t="s">
         <v>47</v>
       </c>
@@ -6353,7 +6559,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="67" spans="1:20" ht="15" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:20">
       <c r="A67" s="12" t="s">
         <v>49</v>
       </c>
@@ -6409,7 +6615,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="68" spans="1:20" ht="15" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:20" ht="15">
       <c r="A68" s="12" t="s">
         <v>55</v>
       </c>
@@ -6465,7 +6671,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="69" spans="1:20" ht="15" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:20" ht="15">
       <c r="A69" s="12" t="s">
         <v>148</v>
       </c>
@@ -6521,7 +6727,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="70" spans="1:20" ht="15" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:20" ht="15">
       <c r="A70" s="12" t="s">
         <v>151</v>
       </c>
@@ -6577,7 +6783,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="71" spans="1:20" ht="15" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:20">
       <c r="A71" s="12" t="s">
         <v>51</v>
       </c>
@@ -6633,7 +6839,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="72" spans="1:20" ht="15" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:20">
       <c r="A72" s="12" t="s">
         <v>168</v>
       </c>
@@ -6689,7 +6895,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="73" spans="1:20" ht="15" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:20">
       <c r="A73" s="12" t="s">
         <v>171</v>
       </c>
@@ -6745,7 +6951,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="74" spans="1:20" ht="15" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:20">
       <c r="A74" s="12" t="s">
         <v>173</v>
       </c>
@@ -6801,7 +7007,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="75" spans="1:20" ht="15" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:20">
       <c r="A75" s="12" t="s">
         <v>175</v>
       </c>
@@ -6857,7 +7063,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="76" spans="1:20" ht="15" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:20">
       <c r="A76" s="12" t="s">
         <v>177</v>
       </c>
@@ -6913,7 +7119,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="77" spans="1:20" ht="15" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:20">
       <c r="A77" s="12" t="s">
         <v>179</v>
       </c>
@@ -6969,7 +7175,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="78" spans="1:20" ht="15" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:20">
       <c r="A78" s="12" t="s">
         <v>181</v>
       </c>
@@ -7025,7 +7231,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="79" spans="1:20" ht="15" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:20">
       <c r="A79" s="12" t="s">
         <v>183</v>
       </c>
@@ -7081,7 +7287,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="80" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:20" ht="28.8">
       <c r="A80" s="12" t="s">
         <v>153</v>
       </c>
@@ -7137,7 +7343,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="81" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:20" ht="28.8">
       <c r="A81" s="12" t="s">
         <v>156</v>
       </c>
@@ -7193,7 +7399,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="82" spans="1:20" ht="30" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:20" ht="30">
       <c r="A82" s="12" t="s">
         <v>196</v>
       </c>
@@ -7249,7 +7455,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="83" spans="1:20" ht="15" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:20">
       <c r="A83" s="12" t="s">
         <v>197</v>
       </c>
@@ -7305,7 +7511,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="84" spans="1:20" ht="15" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:20" ht="15">
       <c r="A84" s="12" t="s">
         <v>108</v>
       </c>
@@ -7361,7 +7567,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="85" spans="1:20" ht="15" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:20">
       <c r="A85" s="12" t="s">
         <v>112</v>
       </c>
@@ -7417,7 +7623,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="86" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:20" ht="28.8">
       <c r="A86" s="12" t="s">
         <v>115</v>
       </c>
@@ -7473,7 +7679,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="87" spans="1:20" ht="15" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:20">
       <c r="A87" s="12" t="s">
         <v>118</v>
       </c>
@@ -7529,7 +7735,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="88" spans="1:20" ht="30" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:20" ht="30">
       <c r="A88" s="12" t="s">
         <v>121</v>
       </c>
@@ -7585,7 +7791,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="89" spans="1:20" ht="30" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:20" ht="30">
       <c r="A89" s="12" t="s">
         <v>123</v>
       </c>
@@ -7641,7 +7847,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="90" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:20">
       <c r="A90" s="10" t="s">
         <v>636</v>
       </c>
@@ -7671,7 +7877,7 @@
       </c>
       <c r="J90" s="3"/>
       <c r="K90" s="3"/>
-      <c r="L90" s="42" t="s">
+      <c r="L90" s="17" t="s">
         <v>635</v>
       </c>
       <c r="M90" s="42" t="s">
@@ -7684,10 +7890,10 @@
         <v>637</v>
       </c>
       <c r="P90" s="3" t="s">
+        <v>716</v>
+      </c>
+      <c r="Q90" s="3" t="s">
         <v>638</v>
-      </c>
-      <c r="Q90" s="3" t="s">
-        <v>639</v>
       </c>
       <c r="R90" s="21" t="s">
         <v>246</v>
@@ -7699,9 +7905,9 @@
         <v>630</v>
       </c>
     </row>
-    <row r="91" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A91" s="11" t="s">
-        <v>640</v>
+    <row r="91" spans="1:20">
+      <c r="A91" s="10" t="s">
+        <v>639</v>
       </c>
       <c r="B91" s="9" t="s">
         <v>230</v>
@@ -7729,23 +7935,23 @@
       </c>
       <c r="J91" s="3"/>
       <c r="K91" s="3"/>
-      <c r="L91" s="42" t="s">
-        <v>642</v>
+      <c r="L91" s="17" t="s">
+        <v>641</v>
       </c>
       <c r="M91" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="N91" s="3" t="s">
         <v>412</v>
       </c>
       <c r="O91" s="3" t="s">
+        <v>642</v>
+      </c>
+      <c r="P91" s="3" t="s">
+        <v>718</v>
+      </c>
+      <c r="Q91" s="3" t="s">
         <v>643</v>
-      </c>
-      <c r="P91" s="3" t="s">
-        <v>644</v>
-      </c>
-      <c r="Q91" s="3" t="s">
-        <v>645</v>
       </c>
       <c r="R91" s="21" t="s">
         <v>246</v>
@@ -7757,9 +7963,9 @@
         <v>630</v>
       </c>
     </row>
-    <row r="92" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A92" s="11" t="s">
-        <v>646</v>
+    <row r="92" spans="1:20">
+      <c r="A92" s="10" t="s">
+        <v>644</v>
       </c>
       <c r="B92" s="9" t="s">
         <v>230</v>
@@ -7787,23 +7993,23 @@
       </c>
       <c r="J92" s="3"/>
       <c r="K92" s="3"/>
-      <c r="L92" s="42" t="s">
-        <v>648</v>
+      <c r="L92" s="17" t="s">
+        <v>646</v>
       </c>
       <c r="M92" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="N92" s="3" t="s">
         <v>412</v>
       </c>
       <c r="O92" s="3" t="s">
-        <v>649</v>
+        <v>647</v>
       </c>
       <c r="P92" s="3" t="s">
-        <v>650</v>
+        <v>717</v>
       </c>
       <c r="Q92" s="3" t="s">
-        <v>651</v>
+        <v>648</v>
       </c>
       <c r="R92" s="21" t="s">
         <v>246</v>
@@ -7815,9 +8021,9 @@
         <v>630</v>
       </c>
     </row>
-    <row r="93" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A93" s="11" t="s">
-        <v>652</v>
+    <row r="93" spans="1:20">
+      <c r="A93" s="10" t="s">
+        <v>649</v>
       </c>
       <c r="B93" s="9" t="s">
         <v>230</v>
@@ -7845,23 +8051,23 @@
       </c>
       <c r="J93" s="3"/>
       <c r="K93" s="3"/>
-      <c r="L93" s="42" t="s">
-        <v>654</v>
+      <c r="L93" s="17" t="s">
+        <v>651</v>
       </c>
       <c r="M93" t="s">
-        <v>653</v>
+        <v>650</v>
       </c>
       <c r="N93" s="3" t="s">
         <v>412</v>
       </c>
       <c r="O93" s="3" t="s">
-        <v>655</v>
+        <v>652</v>
       </c>
       <c r="P93" s="3" t="s">
-        <v>656</v>
+        <v>720</v>
       </c>
       <c r="Q93" s="3" t="s">
-        <v>657</v>
+        <v>653</v>
       </c>
       <c r="R93" s="21" t="s">
         <v>246</v>
@@ -7873,9 +8079,9 @@
         <v>630</v>
       </c>
     </row>
-    <row r="94" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A94" s="11" t="s">
-        <v>658</v>
+    <row r="94" spans="1:20">
+      <c r="A94" s="10" t="s">
+        <v>654</v>
       </c>
       <c r="B94" s="9" t="s">
         <v>230</v>
@@ -7903,23 +8109,23 @@
       </c>
       <c r="J94" s="3"/>
       <c r="K94" s="3"/>
-      <c r="L94" s="42" t="s">
-        <v>660</v>
+      <c r="L94" s="17" t="s">
+        <v>656</v>
       </c>
       <c r="M94" t="s">
-        <v>659</v>
+        <v>655</v>
       </c>
       <c r="N94" s="3" t="s">
         <v>412</v>
       </c>
       <c r="O94" s="3" t="s">
-        <v>661</v>
+        <v>657</v>
       </c>
       <c r="P94" s="3" t="s">
-        <v>662</v>
+        <v>719</v>
       </c>
       <c r="Q94" s="3" t="s">
-        <v>663</v>
+        <v>658</v>
       </c>
       <c r="R94" s="21" t="s">
         <v>246</v>
@@ -7931,9 +8137,9 @@
         <v>630</v>
       </c>
     </row>
-    <row r="95" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A95" s="11" t="s">
-        <v>664</v>
+    <row r="95" spans="1:20">
+      <c r="A95" s="10" t="s">
+        <v>659</v>
       </c>
       <c r="B95" s="9" t="s">
         <v>230</v>
@@ -7961,23 +8167,23 @@
       </c>
       <c r="J95" s="3"/>
       <c r="K95" s="3"/>
-      <c r="L95" s="42" t="s">
-        <v>666</v>
+      <c r="L95" s="17" t="s">
+        <v>661</v>
       </c>
       <c r="M95" t="s">
-        <v>665</v>
-      </c>
-      <c r="N95" s="3" t="s">
+        <v>660</v>
+      </c>
+      <c r="N95" s="48" t="s">
         <v>412</v>
       </c>
-      <c r="O95" s="3" t="s">
-        <v>667</v>
-      </c>
-      <c r="P95" s="3" t="s">
-        <v>668</v>
-      </c>
-      <c r="Q95" s="3" t="s">
-        <v>669</v>
+      <c r="O95" s="48" t="s">
+        <v>662</v>
+      </c>
+      <c r="P95" s="48" t="s">
+        <v>721</v>
+      </c>
+      <c r="Q95" s="48" t="s">
+        <v>663</v>
       </c>
       <c r="R95" s="21" t="s">
         <v>246</v>
@@ -7988,6 +8194,1459 @@
       <c r="T95" s="21" t="s">
         <v>630</v>
       </c>
+    </row>
+    <row r="96" spans="1:20">
+      <c r="A96" s="10" t="s">
+        <v>680</v>
+      </c>
+      <c r="B96" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="C96" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="D96" s="18" t="s">
+        <v>224</v>
+      </c>
+      <c r="E96" s="10" t="s">
+        <v>245</v>
+      </c>
+      <c r="F96" s="10" t="s">
+        <v>246</v>
+      </c>
+      <c r="G96" s="3" t="s">
+        <v>276</v>
+      </c>
+      <c r="H96" s="43">
+        <v>41640</v>
+      </c>
+      <c r="I96" s="44">
+        <v>45792</v>
+      </c>
+      <c r="J96" s="3"/>
+      <c r="K96" s="3"/>
+      <c r="L96" s="17" t="s">
+        <v>681</v>
+      </c>
+      <c r="M96" s="3"/>
+      <c r="N96" s="3" t="str">
+        <f>Hoja2!$A$2&amp;""&amp;B96</f>
+        <v>Data/Macro/raw/commodities</v>
+      </c>
+      <c r="O96" s="3" t="str">
+        <f>N96&amp;"/"&amp;A96&amp;".csv"</f>
+        <v>Data/Macro/raw/commodities/US_Cotton_#2_Futures.csv</v>
+      </c>
+      <c r="P96" s="3" t="str">
+        <f>Hoja2!$B$2&amp;B96&amp;"\"&amp;A96&amp;".csv"</f>
+        <v>C:\Users\pedro\OneDrive\Documents\ALGO TRADING\SP500 INDEX\Data\Macro\raw\commodities\US_Cotton_#2_Futures.csv</v>
+      </c>
+      <c r="Q96" s="3" t="str">
+        <f>Hoja2!$C$2&amp;B96&amp;"/"&amp;A96&amp;".csv"</f>
+        <v>/mnt/c/Users/pedro/OneDrive/Documents/ALGO TRADING/SP500 INDEX/Data/Macro/raw/commodities/US_Cotton_#2_Futures.csv</v>
+      </c>
+      <c r="R96" s="3"/>
+      <c r="S96" s="3" t="s">
+        <v>604</v>
+      </c>
+      <c r="T96" s="3" t="s">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="97" spans="1:20">
+      <c r="A97" s="10" t="s">
+        <v>664</v>
+      </c>
+      <c r="B97" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="C97" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="D97" s="18" t="s">
+        <v>224</v>
+      </c>
+      <c r="E97" s="10" t="s">
+        <v>245</v>
+      </c>
+      <c r="F97" s="10" t="s">
+        <v>246</v>
+      </c>
+      <c r="G97" s="3" t="s">
+        <v>276</v>
+      </c>
+      <c r="H97" s="15">
+        <v>41640</v>
+      </c>
+      <c r="I97" s="44">
+        <v>45792</v>
+      </c>
+      <c r="J97" s="3"/>
+      <c r="K97" s="3"/>
+      <c r="L97" s="17" t="s">
+        <v>682</v>
+      </c>
+      <c r="M97" s="3"/>
+      <c r="N97" s="3" t="str">
+        <f>Hoja2!$A$2&amp;""&amp;B97</f>
+        <v>Data/Macro/raw/commodities</v>
+      </c>
+      <c r="O97" s="3" t="str">
+        <f t="shared" ref="O97:O120" si="0">N97&amp;"/"&amp;A97&amp;".csv"</f>
+        <v>Data/Macro/raw/commodities/Lumber_Futures.csv</v>
+      </c>
+      <c r="P97" s="3" t="str">
+        <f>Hoja2!$B$2&amp;B97&amp;"\"&amp;A97&amp;".csv"</f>
+        <v>C:\Users\pedro\OneDrive\Documents\ALGO TRADING\SP500 INDEX\Data\Macro\raw\commodities\Lumber_Futures.csv</v>
+      </c>
+      <c r="Q97" s="3" t="str">
+        <f>Hoja2!$C$2&amp;B97&amp;"/"&amp;A97&amp;".csv"</f>
+        <v>/mnt/c/Users/pedro/OneDrive/Documents/ALGO TRADING/SP500 INDEX/Data/Macro/raw/commodities/Lumber_Futures.csv</v>
+      </c>
+      <c r="R97" s="3"/>
+      <c r="S97" s="3" t="s">
+        <v>604</v>
+      </c>
+      <c r="T97" s="3" t="s">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="98" spans="1:20">
+      <c r="A98" s="10" t="s">
+        <v>665</v>
+      </c>
+      <c r="B98" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="C98" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="D98" s="18" t="s">
+        <v>224</v>
+      </c>
+      <c r="E98" s="10" t="s">
+        <v>245</v>
+      </c>
+      <c r="F98" s="10" t="s">
+        <v>246</v>
+      </c>
+      <c r="G98" s="3" t="s">
+        <v>276</v>
+      </c>
+      <c r="H98" s="15">
+        <v>41640</v>
+      </c>
+      <c r="I98" s="44">
+        <v>45792</v>
+      </c>
+      <c r="J98" s="3"/>
+      <c r="K98" s="3"/>
+      <c r="L98" s="17" t="s">
+        <v>683</v>
+      </c>
+      <c r="M98" s="3"/>
+      <c r="N98" s="3" t="str">
+        <f>Hoja2!$A$2&amp;""&amp;B98</f>
+        <v>Data/Macro/raw/commodities</v>
+      </c>
+      <c r="O98" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>Data/Macro/raw/commodities/US_Cocoa_Futures.csv</v>
+      </c>
+      <c r="P98" s="3" t="str">
+        <f>Hoja2!$B$2&amp;B98&amp;"\"&amp;A98&amp;".csv"</f>
+        <v>C:\Users\pedro\OneDrive\Documents\ALGO TRADING\SP500 INDEX\Data\Macro\raw\commodities\US_Cocoa_Futures.csv</v>
+      </c>
+      <c r="Q98" s="3" t="str">
+        <f>Hoja2!$C$2&amp;B98&amp;"/"&amp;A98&amp;".csv"</f>
+        <v>/mnt/c/Users/pedro/OneDrive/Documents/ALGO TRADING/SP500 INDEX/Data/Macro/raw/commodities/US_Cocoa_Futures.csv</v>
+      </c>
+      <c r="R98" s="3"/>
+      <c r="S98" s="3" t="s">
+        <v>604</v>
+      </c>
+      <c r="T98" s="3" t="s">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="99" spans="1:20">
+      <c r="A99" s="10" t="s">
+        <v>666</v>
+      </c>
+      <c r="B99" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="C99" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="D99" s="18" t="s">
+        <v>224</v>
+      </c>
+      <c r="E99" s="10" t="s">
+        <v>245</v>
+      </c>
+      <c r="F99" s="10" t="s">
+        <v>246</v>
+      </c>
+      <c r="G99" s="3" t="s">
+        <v>276</v>
+      </c>
+      <c r="H99" s="15">
+        <v>41640</v>
+      </c>
+      <c r="I99" s="44">
+        <v>45792</v>
+      </c>
+      <c r="J99" s="3"/>
+      <c r="K99" s="3"/>
+      <c r="L99" s="17" t="s">
+        <v>684</v>
+      </c>
+      <c r="M99" s="3"/>
+      <c r="N99" s="3" t="str">
+        <f>Hoja2!$A$2&amp;""&amp;B99</f>
+        <v>Data/Macro/raw/commodities</v>
+      </c>
+      <c r="O99" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>Data/Macro/raw/commodities/US_Coffee_C_Futures.csv</v>
+      </c>
+      <c r="P99" s="3" t="str">
+        <f>Hoja2!$B$2&amp;B99&amp;"\"&amp;A99&amp;".csv"</f>
+        <v>C:\Users\pedro\OneDrive\Documents\ALGO TRADING\SP500 INDEX\Data\Macro\raw\commodities\US_Coffee_C_Futures.csv</v>
+      </c>
+      <c r="Q99" s="3" t="str">
+        <f>Hoja2!$C$2&amp;B99&amp;"/"&amp;A99&amp;".csv"</f>
+        <v>/mnt/c/Users/pedro/OneDrive/Documents/ALGO TRADING/SP500 INDEX/Data/Macro/raw/commodities/US_Coffee_C_Futures.csv</v>
+      </c>
+      <c r="R99" s="3"/>
+      <c r="S99" s="3" t="s">
+        <v>604</v>
+      </c>
+      <c r="T99" s="3" t="s">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="100" spans="1:20">
+      <c r="A100" s="10" t="s">
+        <v>667</v>
+      </c>
+      <c r="B100" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="C100" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="D100" s="18" t="s">
+        <v>224</v>
+      </c>
+      <c r="E100" s="10" t="s">
+        <v>245</v>
+      </c>
+      <c r="F100" s="10" t="s">
+        <v>246</v>
+      </c>
+      <c r="G100" s="3" t="s">
+        <v>276</v>
+      </c>
+      <c r="H100" s="15">
+        <v>41640</v>
+      </c>
+      <c r="I100" s="44">
+        <v>45792</v>
+      </c>
+      <c r="J100" s="3"/>
+      <c r="K100" s="3"/>
+      <c r="L100" s="17" t="s">
+        <v>685</v>
+      </c>
+      <c r="M100" s="3"/>
+      <c r="N100" s="3" t="str">
+        <f>Hoja2!$A$2&amp;""&amp;B100</f>
+        <v>Data/Macro/raw/commodities</v>
+      </c>
+      <c r="O100" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>Data/Macro/raw/commodities/Orange_Juice_Futures.csv</v>
+      </c>
+      <c r="P100" s="3" t="str">
+        <f>Hoja2!$B$2&amp;B100&amp;"\"&amp;A100&amp;".csv"</f>
+        <v>C:\Users\pedro\OneDrive\Documents\ALGO TRADING\SP500 INDEX\Data\Macro\raw\commodities\Orange_Juice_Futures.csv</v>
+      </c>
+      <c r="Q100" s="3" t="str">
+        <f>Hoja2!$C$2&amp;B100&amp;"/"&amp;A100&amp;".csv"</f>
+        <v>/mnt/c/Users/pedro/OneDrive/Documents/ALGO TRADING/SP500 INDEX/Data/Macro/raw/commodities/Orange_Juice_Futures.csv</v>
+      </c>
+      <c r="R100" s="3"/>
+      <c r="S100" s="3" t="s">
+        <v>604</v>
+      </c>
+      <c r="T100" s="3" t="s">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="101" spans="1:20">
+      <c r="A101" s="10" t="s">
+        <v>668</v>
+      </c>
+      <c r="B101" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="C101" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="D101" s="18" t="s">
+        <v>224</v>
+      </c>
+      <c r="E101" s="10" t="s">
+        <v>245</v>
+      </c>
+      <c r="F101" s="10" t="s">
+        <v>246</v>
+      </c>
+      <c r="G101" s="3" t="s">
+        <v>276</v>
+      </c>
+      <c r="H101" s="15">
+        <v>41640</v>
+      </c>
+      <c r="I101" s="44">
+        <v>45792</v>
+      </c>
+      <c r="J101" s="3"/>
+      <c r="K101" s="3"/>
+      <c r="L101" s="3" t="s">
+        <v>691</v>
+      </c>
+      <c r="M101" s="3"/>
+      <c r="N101" s="3" t="str">
+        <f>Hoja2!$A$2&amp;""&amp;B101</f>
+        <v>Data/Macro/raw/commodities</v>
+      </c>
+      <c r="O101" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>Data/Macro/raw/commodities/US_Sugar.csv</v>
+      </c>
+      <c r="P101" s="3" t="str">
+        <f>Hoja2!$B$2&amp;B101&amp;"\"&amp;A101&amp;".csv"</f>
+        <v>C:\Users\pedro\OneDrive\Documents\ALGO TRADING\SP500 INDEX\Data\Macro\raw\commodities\US_Sugar.csv</v>
+      </c>
+      <c r="Q101" s="3" t="str">
+        <f>Hoja2!$C$2&amp;B101&amp;"/"&amp;A101&amp;".csv"</f>
+        <v>/mnt/c/Users/pedro/OneDrive/Documents/ALGO TRADING/SP500 INDEX/Data/Macro/raw/commodities/US_Sugar.csv</v>
+      </c>
+      <c r="R101" s="3"/>
+      <c r="S101" s="3" t="s">
+        <v>604</v>
+      </c>
+      <c r="T101" s="3" t="s">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="102" spans="1:20">
+      <c r="A102" s="10" t="s">
+        <v>669</v>
+      </c>
+      <c r="B102" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="C102" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="D102" s="18" t="s">
+        <v>224</v>
+      </c>
+      <c r="E102" s="10" t="s">
+        <v>245</v>
+      </c>
+      <c r="F102" s="10" t="s">
+        <v>246</v>
+      </c>
+      <c r="G102" s="3" t="s">
+        <v>276</v>
+      </c>
+      <c r="H102" s="15">
+        <v>41640</v>
+      </c>
+      <c r="I102" s="44">
+        <v>45792</v>
+      </c>
+      <c r="J102" s="3"/>
+      <c r="K102" s="3"/>
+      <c r="L102" s="3" t="s">
+        <v>692</v>
+      </c>
+      <c r="M102" s="3"/>
+      <c r="N102" s="3" t="str">
+        <f>Hoja2!$A$2&amp;""&amp;B102</f>
+        <v>Data/Macro/raw/commodities</v>
+      </c>
+      <c r="O102" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>Data/Macro/raw/commodities/US_Corn_Futures.csv</v>
+      </c>
+      <c r="P102" s="3" t="str">
+        <f>Hoja2!$B$2&amp;B102&amp;"\"&amp;A102&amp;".csv"</f>
+        <v>C:\Users\pedro\OneDrive\Documents\ALGO TRADING\SP500 INDEX\Data\Macro\raw\commodities\US_Corn_Futures.csv</v>
+      </c>
+      <c r="Q102" s="3" t="str">
+        <f>Hoja2!$C$2&amp;B102&amp;"/"&amp;A102&amp;".csv"</f>
+        <v>/mnt/c/Users/pedro/OneDrive/Documents/ALGO TRADING/SP500 INDEX/Data/Macro/raw/commodities/US_Corn_Futures.csv</v>
+      </c>
+      <c r="R102" s="3"/>
+      <c r="S102" s="3" t="s">
+        <v>604</v>
+      </c>
+      <c r="T102" s="3" t="s">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="103" spans="1:20">
+      <c r="A103" s="10" t="s">
+        <v>670</v>
+      </c>
+      <c r="B103" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="C103" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="D103" s="18" t="s">
+        <v>224</v>
+      </c>
+      <c r="E103" s="10" t="s">
+        <v>245</v>
+      </c>
+      <c r="F103" s="10" t="s">
+        <v>246</v>
+      </c>
+      <c r="G103" s="3" t="s">
+        <v>276</v>
+      </c>
+      <c r="H103" s="43">
+        <v>41640</v>
+      </c>
+      <c r="I103" s="44">
+        <v>45792</v>
+      </c>
+      <c r="J103" s="3"/>
+      <c r="K103" s="3"/>
+      <c r="L103" s="3" t="s">
+        <v>693</v>
+      </c>
+      <c r="M103" s="3"/>
+      <c r="N103" s="3" t="str">
+        <f>Hoja2!$A$2&amp;""&amp;B103</f>
+        <v>Data/Macro/raw/commodities</v>
+      </c>
+      <c r="O103" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>Data/Macro/raw/commodities/US_Wheat_Futures.csv</v>
+      </c>
+      <c r="P103" s="3" t="str">
+        <f>Hoja2!$B$2&amp;B103&amp;"\"&amp;A103&amp;".csv"</f>
+        <v>C:\Users\pedro\OneDrive\Documents\ALGO TRADING\SP500 INDEX\Data\Macro\raw\commodities\US_Wheat_Futures.csv</v>
+      </c>
+      <c r="Q103" s="3" t="str">
+        <f>Hoja2!$C$2&amp;B103&amp;"/"&amp;A103&amp;".csv"</f>
+        <v>/mnt/c/Users/pedro/OneDrive/Documents/ALGO TRADING/SP500 INDEX/Data/Macro/raw/commodities/US_Wheat_Futures.csv</v>
+      </c>
+      <c r="R103" s="3"/>
+      <c r="S103" s="3" t="s">
+        <v>604</v>
+      </c>
+      <c r="T103" s="3" t="s">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="104" spans="1:20">
+      <c r="A104" s="10" t="s">
+        <v>671</v>
+      </c>
+      <c r="B104" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="C104" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="D104" s="18" t="s">
+        <v>224</v>
+      </c>
+      <c r="E104" s="10" t="s">
+        <v>245</v>
+      </c>
+      <c r="F104" s="10" t="s">
+        <v>246</v>
+      </c>
+      <c r="G104" s="3" t="s">
+        <v>276</v>
+      </c>
+      <c r="H104" s="15">
+        <v>41640</v>
+      </c>
+      <c r="I104" s="44">
+        <v>45792</v>
+      </c>
+      <c r="J104" s="3"/>
+      <c r="K104" s="3"/>
+      <c r="L104" s="3" t="s">
+        <v>694</v>
+      </c>
+      <c r="M104" s="3"/>
+      <c r="N104" s="3" t="str">
+        <f>Hoja2!$A$2&amp;""&amp;B104</f>
+        <v>Data/Macro/raw/commodities</v>
+      </c>
+      <c r="O104" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>Data/Macro/raw/commodities/Oats_Futures.csv</v>
+      </c>
+      <c r="P104" s="3" t="str">
+        <f>Hoja2!$B$2&amp;B104&amp;"\"&amp;A104&amp;".csv"</f>
+        <v>C:\Users\pedro\OneDrive\Documents\ALGO TRADING\SP500 INDEX\Data\Macro\raw\commodities\Oats_Futures.csv</v>
+      </c>
+      <c r="Q104" s="3" t="str">
+        <f>Hoja2!$C$2&amp;B104&amp;"/"&amp;A104&amp;".csv"</f>
+        <v>/mnt/c/Users/pedro/OneDrive/Documents/ALGO TRADING/SP500 INDEX/Data/Macro/raw/commodities/Oats_Futures.csv</v>
+      </c>
+      <c r="R104" s="3"/>
+      <c r="S104" s="3" t="s">
+        <v>604</v>
+      </c>
+      <c r="T104" s="3" t="s">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="105" spans="1:20">
+      <c r="A105" s="10" t="s">
+        <v>672</v>
+      </c>
+      <c r="B105" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="C105" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="D105" s="18" t="s">
+        <v>224</v>
+      </c>
+      <c r="E105" s="10" t="s">
+        <v>245</v>
+      </c>
+      <c r="F105" s="10" t="s">
+        <v>246</v>
+      </c>
+      <c r="G105" s="3" t="s">
+        <v>276</v>
+      </c>
+      <c r="H105" s="15">
+        <v>41640</v>
+      </c>
+      <c r="I105" s="44">
+        <v>45792</v>
+      </c>
+      <c r="J105" s="3"/>
+      <c r="K105" s="3"/>
+      <c r="L105" s="17" t="s">
+        <v>695</v>
+      </c>
+      <c r="M105" s="3"/>
+      <c r="N105" s="3" t="str">
+        <f>Hoja2!$A$2&amp;""&amp;B105</f>
+        <v>Data/Macro/raw/commodities</v>
+      </c>
+      <c r="O105" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>Data/Macro/raw/commodities/Rough_Rice_Futures.csv</v>
+      </c>
+      <c r="P105" s="3" t="str">
+        <f>Hoja2!$B$2&amp;B105&amp;"\"&amp;A105&amp;".csv"</f>
+        <v>C:\Users\pedro\OneDrive\Documents\ALGO TRADING\SP500 INDEX\Data\Macro\raw\commodities\Rough_Rice_Futures.csv</v>
+      </c>
+      <c r="Q105" s="3" t="str">
+        <f>Hoja2!$C$2&amp;B105&amp;"/"&amp;A105&amp;".csv"</f>
+        <v>/mnt/c/Users/pedro/OneDrive/Documents/ALGO TRADING/SP500 INDEX/Data/Macro/raw/commodities/Rough_Rice_Futures.csv</v>
+      </c>
+      <c r="R105" s="3"/>
+      <c r="S105" s="3" t="s">
+        <v>604</v>
+      </c>
+      <c r="T105" s="3" t="s">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="106" spans="1:20">
+      <c r="A106" s="10" t="s">
+        <v>673</v>
+      </c>
+      <c r="B106" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="C106" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="D106" s="18" t="s">
+        <v>224</v>
+      </c>
+      <c r="E106" s="10" t="s">
+        <v>245</v>
+      </c>
+      <c r="F106" s="10" t="s">
+        <v>246</v>
+      </c>
+      <c r="G106" s="3" t="s">
+        <v>276</v>
+      </c>
+      <c r="H106" s="15">
+        <v>41640</v>
+      </c>
+      <c r="I106" s="44">
+        <v>45792</v>
+      </c>
+      <c r="J106" s="3"/>
+      <c r="K106" s="3"/>
+      <c r="L106" s="3" t="s">
+        <v>696</v>
+      </c>
+      <c r="M106" s="3"/>
+      <c r="N106" s="3" t="str">
+        <f>Hoja2!$A$2&amp;""&amp;B106</f>
+        <v>Data/Macro/raw/commodities</v>
+      </c>
+      <c r="O106" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>Data/Macro/raw/commodities/US_Soybean_Meal_Futures.csv</v>
+      </c>
+      <c r="P106" s="3" t="str">
+        <f>Hoja2!$B$2&amp;B106&amp;"\"&amp;A106&amp;".csv"</f>
+        <v>C:\Users\pedro\OneDrive\Documents\ALGO TRADING\SP500 INDEX\Data\Macro\raw\commodities\US_Soybean_Meal_Futures.csv</v>
+      </c>
+      <c r="Q106" s="3" t="str">
+        <f>Hoja2!$C$2&amp;B106&amp;"/"&amp;A106&amp;".csv"</f>
+        <v>/mnt/c/Users/pedro/OneDrive/Documents/ALGO TRADING/SP500 INDEX/Data/Macro/raw/commodities/US_Soybean_Meal_Futures.csv</v>
+      </c>
+      <c r="R106" s="3"/>
+      <c r="S106" s="3" t="s">
+        <v>604</v>
+      </c>
+      <c r="T106" s="3" t="s">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="107" spans="1:20">
+      <c r="A107" s="10" t="s">
+        <v>674</v>
+      </c>
+      <c r="B107" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="C107" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="D107" s="18" t="s">
+        <v>224</v>
+      </c>
+      <c r="E107" s="10" t="s">
+        <v>245</v>
+      </c>
+      <c r="F107" s="10" t="s">
+        <v>246</v>
+      </c>
+      <c r="G107" s="3" t="s">
+        <v>276</v>
+      </c>
+      <c r="H107" s="15">
+        <v>41640</v>
+      </c>
+      <c r="I107" s="44">
+        <v>45793</v>
+      </c>
+      <c r="J107" s="3"/>
+      <c r="K107" s="3"/>
+      <c r="L107" s="17" t="s">
+        <v>686</v>
+      </c>
+      <c r="M107" s="3"/>
+      <c r="N107" s="3" t="str">
+        <f>Hoja2!$A$2&amp;""&amp;B107</f>
+        <v>Data/Macro/raw/commodities</v>
+      </c>
+      <c r="O107" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>Data/Macro/raw/commodities/US_Soybean_Oil_Futures.csv</v>
+      </c>
+      <c r="P107" s="3" t="str">
+        <f>Hoja2!$B$2&amp;B107&amp;"\"&amp;A107&amp;".csv"</f>
+        <v>C:\Users\pedro\OneDrive\Documents\ALGO TRADING\SP500 INDEX\Data\Macro\raw\commodities\US_Soybean_Oil_Futures.csv</v>
+      </c>
+      <c r="Q107" s="3" t="str">
+        <f>Hoja2!$C$2&amp;B107&amp;"/"&amp;A107&amp;".csv"</f>
+        <v>/mnt/c/Users/pedro/OneDrive/Documents/ALGO TRADING/SP500 INDEX/Data/Macro/raw/commodities/US_Soybean_Oil_Futures.csv</v>
+      </c>
+      <c r="R107" s="3"/>
+      <c r="S107" s="3" t="s">
+        <v>604</v>
+      </c>
+      <c r="T107" s="3" t="s">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="108" spans="1:20">
+      <c r="A108" s="10" t="s">
+        <v>675</v>
+      </c>
+      <c r="B108" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="C108" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="D108" s="18" t="s">
+        <v>224</v>
+      </c>
+      <c r="E108" s="10" t="s">
+        <v>245</v>
+      </c>
+      <c r="F108" s="10" t="s">
+        <v>246</v>
+      </c>
+      <c r="G108" s="3" t="s">
+        <v>276</v>
+      </c>
+      <c r="H108" s="15">
+        <v>41640</v>
+      </c>
+      <c r="I108" s="44">
+        <v>45793</v>
+      </c>
+      <c r="J108" s="3"/>
+      <c r="K108" s="3"/>
+      <c r="L108" s="3" t="s">
+        <v>697</v>
+      </c>
+      <c r="M108" s="3"/>
+      <c r="N108" s="3" t="str">
+        <f>Hoja2!$A$2&amp;""&amp;B108</f>
+        <v>Data/Macro/raw/commodities</v>
+      </c>
+      <c r="O108" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>Data/Macro/raw/commodities/US_Soybeans_Futures.csv</v>
+      </c>
+      <c r="P108" s="3" t="str">
+        <f>Hoja2!$B$2&amp;B108&amp;"\"&amp;A108&amp;".csv"</f>
+        <v>C:\Users\pedro\OneDrive\Documents\ALGO TRADING\SP500 INDEX\Data\Macro\raw\commodities\US_Soybeans_Futures.csv</v>
+      </c>
+      <c r="Q108" s="3" t="str">
+        <f>Hoja2!$C$2&amp;B108&amp;"/"&amp;A108&amp;".csv"</f>
+        <v>/mnt/c/Users/pedro/OneDrive/Documents/ALGO TRADING/SP500 INDEX/Data/Macro/raw/commodities/US_Soybeans_Futures.csv</v>
+      </c>
+      <c r="R108" s="3"/>
+      <c r="S108" s="3" t="s">
+        <v>604</v>
+      </c>
+      <c r="T108" s="3" t="s">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="109" spans="1:20">
+      <c r="A109" s="10" t="s">
+        <v>676</v>
+      </c>
+      <c r="B109" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="C109" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="D109" s="18" t="s">
+        <v>224</v>
+      </c>
+      <c r="E109" s="10" t="s">
+        <v>245</v>
+      </c>
+      <c r="F109" s="10" t="s">
+        <v>246</v>
+      </c>
+      <c r="G109" s="3" t="s">
+        <v>276</v>
+      </c>
+      <c r="H109" s="15">
+        <v>41640</v>
+      </c>
+      <c r="I109" s="44">
+        <v>45793</v>
+      </c>
+      <c r="J109" s="3"/>
+      <c r="K109" s="3"/>
+      <c r="L109" s="17" t="s">
+        <v>687</v>
+      </c>
+      <c r="M109" s="3"/>
+      <c r="N109" s="3" t="str">
+        <f>Hoja2!$A$2&amp;""&amp;B109</f>
+        <v>Data/Macro/raw/commodities</v>
+      </c>
+      <c r="O109" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>Data/Macro/raw/commodities/Feeder_Cattle_Futures.csv</v>
+      </c>
+      <c r="P109" s="3" t="str">
+        <f>Hoja2!$B$2&amp;B109&amp;"\"&amp;A109&amp;".csv"</f>
+        <v>C:\Users\pedro\OneDrive\Documents\ALGO TRADING\SP500 INDEX\Data\Macro\raw\commodities\Feeder_Cattle_Futures.csv</v>
+      </c>
+      <c r="Q109" s="3" t="str">
+        <f>Hoja2!$C$2&amp;B109&amp;"/"&amp;A109&amp;".csv"</f>
+        <v>/mnt/c/Users/pedro/OneDrive/Documents/ALGO TRADING/SP500 INDEX/Data/Macro/raw/commodities/Feeder_Cattle_Futures.csv</v>
+      </c>
+      <c r="R109" s="3"/>
+      <c r="S109" s="3" t="s">
+        <v>604</v>
+      </c>
+      <c r="T109" s="3" t="s">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="110" spans="1:20">
+      <c r="A110" s="10" t="s">
+        <v>677</v>
+      </c>
+      <c r="B110" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="C110" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="D110" s="18" t="s">
+        <v>224</v>
+      </c>
+      <c r="E110" s="10" t="s">
+        <v>245</v>
+      </c>
+      <c r="F110" s="10" t="s">
+        <v>246</v>
+      </c>
+      <c r="G110" s="3" t="s">
+        <v>276</v>
+      </c>
+      <c r="H110" s="43">
+        <v>41640</v>
+      </c>
+      <c r="I110" s="44">
+        <v>45793</v>
+      </c>
+      <c r="J110" s="3"/>
+      <c r="K110" s="3"/>
+      <c r="L110" s="17" t="s">
+        <v>688</v>
+      </c>
+      <c r="M110" s="3"/>
+      <c r="N110" s="3" t="str">
+        <f>Hoja2!$A$2&amp;""&amp;B110</f>
+        <v>Data/Macro/raw/commodities</v>
+      </c>
+      <c r="O110" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>Data/Macro/raw/commodities/ Lean_Hogs_Futures.csv</v>
+      </c>
+      <c r="P110" s="3" t="str">
+        <f>Hoja2!$B$2&amp;B110&amp;"\"&amp;A110&amp;".csv"</f>
+        <v>C:\Users\pedro\OneDrive\Documents\ALGO TRADING\SP500 INDEX\Data\Macro\raw\commodities\ Lean_Hogs_Futures.csv</v>
+      </c>
+      <c r="Q110" s="3" t="str">
+        <f>Hoja2!$C$2&amp;B110&amp;"/"&amp;A110&amp;".csv"</f>
+        <v>/mnt/c/Users/pedro/OneDrive/Documents/ALGO TRADING/SP500 INDEX/Data/Macro/raw/commodities/ Lean_Hogs_Futures.csv</v>
+      </c>
+      <c r="R110" s="3"/>
+      <c r="S110" s="3" t="s">
+        <v>604</v>
+      </c>
+      <c r="T110" s="3" t="s">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="111" spans="1:20">
+      <c r="A111" s="10" t="s">
+        <v>678</v>
+      </c>
+      <c r="B111" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="C111" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="D111" s="18" t="s">
+        <v>224</v>
+      </c>
+      <c r="E111" s="10" t="s">
+        <v>245</v>
+      </c>
+      <c r="F111" s="10" t="s">
+        <v>246</v>
+      </c>
+      <c r="G111" s="3" t="s">
+        <v>276</v>
+      </c>
+      <c r="H111" s="15">
+        <v>41640</v>
+      </c>
+      <c r="I111" s="44">
+        <v>45793</v>
+      </c>
+      <c r="J111" s="3"/>
+      <c r="K111" s="3"/>
+      <c r="L111" s="17" t="s">
+        <v>689</v>
+      </c>
+      <c r="M111" s="3"/>
+      <c r="N111" s="3" t="str">
+        <f>Hoja2!$A$2&amp;""&amp;B111</f>
+        <v>Data/Macro/raw/commodities</v>
+      </c>
+      <c r="O111" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>Data/Macro/raw/commodities/Live_Cattle_Futures.csv</v>
+      </c>
+      <c r="P111" s="3" t="str">
+        <f>Hoja2!$B$2&amp;B111&amp;"\"&amp;A111&amp;".csv"</f>
+        <v>C:\Users\pedro\OneDrive\Documents\ALGO TRADING\SP500 INDEX\Data\Macro\raw\commodities\Live_Cattle_Futures.csv</v>
+      </c>
+      <c r="Q111" s="3" t="str">
+        <f>Hoja2!$C$2&amp;B111&amp;"/"&amp;A111&amp;".csv"</f>
+        <v>/mnt/c/Users/pedro/OneDrive/Documents/ALGO TRADING/SP500 INDEX/Data/Macro/raw/commodities/Live_Cattle_Futures.csv</v>
+      </c>
+      <c r="R111" s="3"/>
+      <c r="S111" s="3" t="s">
+        <v>604</v>
+      </c>
+      <c r="T111" s="3" t="s">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="112" spans="1:20">
+      <c r="A112" s="45" t="s">
+        <v>679</v>
+      </c>
+      <c r="B112" s="46" t="s">
+        <v>230</v>
+      </c>
+      <c r="C112" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="D112" s="47" t="s">
+        <v>224</v>
+      </c>
+      <c r="E112" s="45" t="s">
+        <v>245</v>
+      </c>
+      <c r="F112" s="45" t="s">
+        <v>246</v>
+      </c>
+      <c r="G112" s="48" t="s">
+        <v>276</v>
+      </c>
+      <c r="H112" s="49">
+        <v>41640</v>
+      </c>
+      <c r="I112" s="44">
+        <v>45793</v>
+      </c>
+      <c r="J112" s="48"/>
+      <c r="K112" s="48"/>
+      <c r="L112" s="17" t="s">
+        <v>690</v>
+      </c>
+      <c r="M112" s="3"/>
+      <c r="N112" s="3" t="str">
+        <f>Hoja2!$A$2&amp;""&amp;B112</f>
+        <v>Data/Macro/raw/commodities</v>
+      </c>
+      <c r="O112" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>Data/Macro/raw/commodities/Iron_ore_fines_62%_Fe_CFR_Futures.csv</v>
+      </c>
+      <c r="P112" s="3" t="str">
+        <f>Hoja2!$B$2&amp;B112&amp;"\"&amp;A112&amp;".csv"</f>
+        <v>C:\Users\pedro\OneDrive\Documents\ALGO TRADING\SP500 INDEX\Data\Macro\raw\commodities\Iron_ore_fines_62%_Fe_CFR_Futures.csv</v>
+      </c>
+      <c r="Q112" s="3" t="str">
+        <f>Hoja2!$C$2&amp;B112&amp;"/"&amp;A112&amp;".csv"</f>
+        <v>/mnt/c/Users/pedro/OneDrive/Documents/ALGO TRADING/SP500 INDEX/Data/Macro/raw/commodities/Iron_ore_fines_62%_Fe_CFR_Futures.csv</v>
+      </c>
+      <c r="R112" s="3"/>
+      <c r="S112" s="3" t="s">
+        <v>604</v>
+      </c>
+      <c r="T112" s="3" t="s">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="113" spans="1:20">
+      <c r="A113" s="10" t="s">
+        <v>698</v>
+      </c>
+      <c r="B113" s="9" t="s">
+        <v>231</v>
+      </c>
+      <c r="C113" s="10" t="s">
+        <v>170</v>
+      </c>
+      <c r="D113" s="18" t="s">
+        <v>224</v>
+      </c>
+      <c r="E113" s="45" t="s">
+        <v>245</v>
+      </c>
+      <c r="F113" s="45" t="s">
+        <v>246</v>
+      </c>
+      <c r="G113" s="48" t="s">
+        <v>276</v>
+      </c>
+      <c r="H113" s="43">
+        <v>41640</v>
+      </c>
+      <c r="I113" s="44">
+        <v>45793</v>
+      </c>
+      <c r="J113" s="3"/>
+      <c r="K113" s="3"/>
+      <c r="L113" s="3" t="s">
+        <v>701</v>
+      </c>
+      <c r="M113" s="3"/>
+      <c r="N113" s="3" t="str">
+        <f>Hoja2!$A$2&amp;""&amp;B113</f>
+        <v>Data/Macro/raw/index_pricing</v>
+      </c>
+      <c r="O113" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>Data/Macro/raw/index_pricing/Dow_Jones_Industrial_Average.csv</v>
+      </c>
+      <c r="P113" s="3" t="str">
+        <f>Hoja2!$B$2&amp;B113&amp;"\"&amp;A113&amp;".csv"</f>
+        <v>C:\Users\pedro\OneDrive\Documents\ALGO TRADING\SP500 INDEX\Data\Macro\raw\index_pricing\Dow_Jones_Industrial_Average.csv</v>
+      </c>
+      <c r="Q113" s="3" t="str">
+        <f>Hoja2!$C$2&amp;B113&amp;"/"&amp;A113&amp;".csv"</f>
+        <v>/mnt/c/Users/pedro/OneDrive/Documents/ALGO TRADING/SP500 INDEX/Data/Macro/raw/index_pricing/Dow_Jones_Industrial_Average.csv</v>
+      </c>
+      <c r="R113" s="3"/>
+      <c r="S113" s="3" t="s">
+        <v>604</v>
+      </c>
+      <c r="T113" s="3" t="s">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="114" spans="1:20">
+      <c r="A114" s="10" t="s">
+        <v>699</v>
+      </c>
+      <c r="B114" s="9" t="s">
+        <v>231</v>
+      </c>
+      <c r="C114" s="10" t="s">
+        <v>170</v>
+      </c>
+      <c r="D114" s="18" t="s">
+        <v>224</v>
+      </c>
+      <c r="E114" s="45" t="s">
+        <v>245</v>
+      </c>
+      <c r="F114" s="45" t="s">
+        <v>246</v>
+      </c>
+      <c r="G114" s="48" t="s">
+        <v>276</v>
+      </c>
+      <c r="H114" s="15">
+        <v>41640</v>
+      </c>
+      <c r="I114" s="44">
+        <v>45793</v>
+      </c>
+      <c r="J114" s="3"/>
+      <c r="K114" s="3"/>
+      <c r="L114" s="3" t="s">
+        <v>702</v>
+      </c>
+      <c r="M114" s="3"/>
+      <c r="N114" s="3" t="str">
+        <f>Hoja2!$A$2&amp;""&amp;B114</f>
+        <v>Data/Macro/raw/index_pricing</v>
+      </c>
+      <c r="O114" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>Data/Macro/raw/index_pricing/Nasdaq_100_Fi.csv</v>
+      </c>
+      <c r="P114" s="3" t="str">
+        <f>Hoja2!$B$2&amp;B114&amp;"\"&amp;A114&amp;".csv"</f>
+        <v>C:\Users\pedro\OneDrive\Documents\ALGO TRADING\SP500 INDEX\Data\Macro\raw\index_pricing\Nasdaq_100_Fi.csv</v>
+      </c>
+      <c r="Q114" s="3" t="str">
+        <f>Hoja2!$C$2&amp;B114&amp;"/"&amp;A114&amp;".csv"</f>
+        <v>/mnt/c/Users/pedro/OneDrive/Documents/ALGO TRADING/SP500 INDEX/Data/Macro/raw/index_pricing/Nasdaq_100_Fi.csv</v>
+      </c>
+      <c r="R114" s="3"/>
+      <c r="S114" s="3" t="s">
+        <v>604</v>
+      </c>
+      <c r="T114" s="3" t="s">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="115" spans="1:20">
+      <c r="A115" s="10" t="s">
+        <v>700</v>
+      </c>
+      <c r="B115" s="9" t="s">
+        <v>231</v>
+      </c>
+      <c r="C115" s="10" t="s">
+        <v>170</v>
+      </c>
+      <c r="D115" s="18" t="s">
+        <v>224</v>
+      </c>
+      <c r="E115" s="45" t="s">
+        <v>245</v>
+      </c>
+      <c r="F115" s="45" t="s">
+        <v>246</v>
+      </c>
+      <c r="G115" s="48" t="s">
+        <v>276</v>
+      </c>
+      <c r="H115" s="49">
+        <v>41640</v>
+      </c>
+      <c r="I115" s="44">
+        <v>45793</v>
+      </c>
+      <c r="J115" s="3"/>
+      <c r="K115" s="3"/>
+      <c r="L115" s="3" t="s">
+        <v>703</v>
+      </c>
+      <c r="M115" s="3"/>
+      <c r="N115" s="3" t="str">
+        <f>Hoja2!$A$2&amp;""&amp;B115</f>
+        <v>Data/Macro/raw/index_pricing</v>
+      </c>
+      <c r="O115" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>Data/Macro/raw/index_pricing/CAC_40.csv</v>
+      </c>
+      <c r="P115" s="3" t="str">
+        <f>Hoja2!$B$2&amp;B115&amp;"\"&amp;A115&amp;".csv"</f>
+        <v>C:\Users\pedro\OneDrive\Documents\ALGO TRADING\SP500 INDEX\Data\Macro\raw\index_pricing\CAC_40.csv</v>
+      </c>
+      <c r="Q115" s="3" t="str">
+        <f>Hoja2!$C$2&amp;B115&amp;"/"&amp;A115&amp;".csv"</f>
+        <v>/mnt/c/Users/pedro/OneDrive/Documents/ALGO TRADING/SP500 INDEX/Data/Macro/raw/index_pricing/CAC_40.csv</v>
+      </c>
+      <c r="R115" s="3"/>
+      <c r="S115" s="3" t="s">
+        <v>604</v>
+      </c>
+      <c r="T115" s="3" t="s">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="116" spans="1:20">
+      <c r="A116" s="10" t="s">
+        <v>704</v>
+      </c>
+      <c r="B116" s="10" t="s">
+        <v>229</v>
+      </c>
+      <c r="C116" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="D116" s="18" t="s">
+        <v>224</v>
+      </c>
+      <c r="E116" s="45" t="s">
+        <v>245</v>
+      </c>
+      <c r="F116" s="45" t="s">
+        <v>246</v>
+      </c>
+      <c r="G116" s="48" t="s">
+        <v>276</v>
+      </c>
+      <c r="H116" s="43">
+        <v>41640</v>
+      </c>
+      <c r="I116" s="44">
+        <v>45793</v>
+      </c>
+      <c r="J116" s="3"/>
+      <c r="K116" s="3"/>
+      <c r="L116" s="3" t="s">
+        <v>708</v>
+      </c>
+      <c r="M116" s="3"/>
+      <c r="N116" s="3" t="str">
+        <f>Hoja2!$A$2&amp;""&amp;B116</f>
+        <v>Data/Macro/raw/exchange_rate</v>
+      </c>
+      <c r="O116" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>Data/Macro/raw/exchange_rate/JPY_EUR.csv</v>
+      </c>
+      <c r="P116" s="3" t="str">
+        <f>Hoja2!$B$2&amp;B116&amp;"\"&amp;A116&amp;".csv"</f>
+        <v>C:\Users\pedro\OneDrive\Documents\ALGO TRADING\SP500 INDEX\Data\Macro\raw\exchange_rate\JPY_EUR.csv</v>
+      </c>
+      <c r="Q116" s="3" t="str">
+        <f>Hoja2!$C$2&amp;B116&amp;"/"&amp;A116&amp;".csv"</f>
+        <v>/mnt/c/Users/pedro/OneDrive/Documents/ALGO TRADING/SP500 INDEX/Data/Macro/raw/exchange_rate/JPY_EUR.csv</v>
+      </c>
+      <c r="R116" s="3"/>
+      <c r="S116" s="3" t="s">
+        <v>604</v>
+      </c>
+      <c r="T116" s="3" t="s">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="117" spans="1:20">
+      <c r="A117" s="10" t="s">
+        <v>704</v>
+      </c>
+      <c r="B117" s="10" t="s">
+        <v>229</v>
+      </c>
+      <c r="C117" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="D117" s="18" t="s">
+        <v>224</v>
+      </c>
+      <c r="E117" s="45" t="s">
+        <v>245</v>
+      </c>
+      <c r="F117" s="45" t="s">
+        <v>246</v>
+      </c>
+      <c r="G117" s="48" t="s">
+        <v>276</v>
+      </c>
+      <c r="H117" s="15">
+        <v>41640</v>
+      </c>
+      <c r="I117" s="44">
+        <v>45793</v>
+      </c>
+      <c r="J117" s="3"/>
+      <c r="K117" s="3"/>
+      <c r="L117" s="3" t="s">
+        <v>709</v>
+      </c>
+      <c r="M117" s="3"/>
+      <c r="N117" s="3" t="str">
+        <f>Hoja2!$A$2&amp;""&amp;B117</f>
+        <v>Data/Macro/raw/exchange_rate</v>
+      </c>
+      <c r="O117" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>Data/Macro/raw/exchange_rate/JPY_EUR.csv</v>
+      </c>
+      <c r="P117" s="3" t="str">
+        <f>Hoja2!$B$2&amp;B117&amp;"\"&amp;A117&amp;".csv"</f>
+        <v>C:\Users\pedro\OneDrive\Documents\ALGO TRADING\SP500 INDEX\Data\Macro\raw\exchange_rate\JPY_EUR.csv</v>
+      </c>
+      <c r="Q117" s="3" t="str">
+        <f>Hoja2!$C$2&amp;B117&amp;"/"&amp;A117&amp;".csv"</f>
+        <v>/mnt/c/Users/pedro/OneDrive/Documents/ALGO TRADING/SP500 INDEX/Data/Macro/raw/exchange_rate/JPY_EUR.csv</v>
+      </c>
+      <c r="R117" s="3"/>
+      <c r="S117" s="3" t="s">
+        <v>604</v>
+      </c>
+      <c r="T117" s="3" t="s">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="118" spans="1:20">
+      <c r="A118" s="10" t="s">
+        <v>705</v>
+      </c>
+      <c r="B118" s="10" t="s">
+        <v>229</v>
+      </c>
+      <c r="C118" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="D118" s="18" t="s">
+        <v>224</v>
+      </c>
+      <c r="E118" s="45" t="s">
+        <v>245</v>
+      </c>
+      <c r="F118" s="45" t="s">
+        <v>246</v>
+      </c>
+      <c r="G118" s="48" t="s">
+        <v>276</v>
+      </c>
+      <c r="H118" s="49">
+        <v>41640</v>
+      </c>
+      <c r="I118" s="44">
+        <v>45793</v>
+      </c>
+      <c r="J118" s="3"/>
+      <c r="K118" s="3"/>
+      <c r="L118" s="3" t="s">
+        <v>710</v>
+      </c>
+      <c r="M118" s="3"/>
+      <c r="N118" s="3" t="str">
+        <f>Hoja2!$A$2&amp;""&amp;B118</f>
+        <v>Data/Macro/raw/exchange_rate</v>
+      </c>
+      <c r="O118" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>Data/Macro/raw/exchange_rate/BRL_NZD.csv</v>
+      </c>
+      <c r="P118" s="3" t="str">
+        <f>Hoja2!$B$2&amp;B118&amp;"\"&amp;A118&amp;".csv"</f>
+        <v>C:\Users\pedro\OneDrive\Documents\ALGO TRADING\SP500 INDEX\Data\Macro\raw\exchange_rate\BRL_NZD.csv</v>
+      </c>
+      <c r="Q118" s="3" t="str">
+        <f>Hoja2!$C$2&amp;B118&amp;"/"&amp;A118&amp;".csv"</f>
+        <v>/mnt/c/Users/pedro/OneDrive/Documents/ALGO TRADING/SP500 INDEX/Data/Macro/raw/exchange_rate/BRL_NZD.csv</v>
+      </c>
+      <c r="R118" s="3"/>
+      <c r="S118" s="3" t="s">
+        <v>604</v>
+      </c>
+      <c r="T118" s="3" t="s">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="119" spans="1:20">
+      <c r="A119" s="10" t="s">
+        <v>706</v>
+      </c>
+      <c r="B119" s="10" t="s">
+        <v>229</v>
+      </c>
+      <c r="C119" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="D119" s="18" t="s">
+        <v>224</v>
+      </c>
+      <c r="E119" s="45" t="s">
+        <v>245</v>
+      </c>
+      <c r="F119" s="45" t="s">
+        <v>246</v>
+      </c>
+      <c r="G119" s="48" t="s">
+        <v>276</v>
+      </c>
+      <c r="H119" s="43">
+        <v>41640</v>
+      </c>
+      <c r="I119" s="44">
+        <v>45793</v>
+      </c>
+      <c r="J119" s="3"/>
+      <c r="K119" s="3"/>
+      <c r="L119" s="3" t="s">
+        <v>711</v>
+      </c>
+      <c r="M119" s="3"/>
+      <c r="N119" s="3" t="str">
+        <f>Hoja2!$A$2&amp;""&amp;B119</f>
+        <v>Data/Macro/raw/exchange_rate</v>
+      </c>
+      <c r="O119" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>Data/Macro/raw/exchange_rate/NOK_AUD.csv</v>
+      </c>
+      <c r="P119" s="3" t="str">
+        <f>Hoja2!$B$2&amp;B119&amp;"\"&amp;A119&amp;".csv"</f>
+        <v>C:\Users\pedro\OneDrive\Documents\ALGO TRADING\SP500 INDEX\Data\Macro\raw\exchange_rate\NOK_AUD.csv</v>
+      </c>
+      <c r="Q119" s="3" t="str">
+        <f>Hoja2!$C$2&amp;B119&amp;"/"&amp;A119&amp;".csv"</f>
+        <v>/mnt/c/Users/pedro/OneDrive/Documents/ALGO TRADING/SP500 INDEX/Data/Macro/raw/exchange_rate/NOK_AUD.csv</v>
+      </c>
+      <c r="R119" s="3"/>
+      <c r="S119" s="3" t="s">
+        <v>604</v>
+      </c>
+      <c r="T119" s="3" t="s">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="120" spans="1:20">
+      <c r="A120" s="10" t="s">
+        <v>707</v>
+      </c>
+      <c r="B120" s="10" t="s">
+        <v>229</v>
+      </c>
+      <c r="C120" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="D120" s="18" t="s">
+        <v>224</v>
+      </c>
+      <c r="E120" s="10" t="s">
+        <v>245</v>
+      </c>
+      <c r="F120" s="10" t="s">
+        <v>246</v>
+      </c>
+      <c r="G120" s="48" t="s">
+        <v>276</v>
+      </c>
+      <c r="H120" s="15">
+        <v>41640</v>
+      </c>
+      <c r="I120" s="44">
+        <v>45793</v>
+      </c>
+      <c r="J120" s="3"/>
+      <c r="K120" s="3"/>
+      <c r="L120" s="3" t="s">
+        <v>712</v>
+      </c>
+      <c r="M120" s="3"/>
+      <c r="N120" s="3" t="str">
+        <f>Hoja2!$A$2&amp;""&amp;B120</f>
+        <v>Data/Macro/raw/exchange_rate</v>
+      </c>
+      <c r="O120" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>Data/Macro/raw/exchange_rate/PHP_ZAR.csv</v>
+      </c>
+      <c r="P120" s="3" t="str">
+        <f>Hoja2!$B$2&amp;B120&amp;"\"&amp;A120&amp;".csv"</f>
+        <v>C:\Users\pedro\OneDrive\Documents\ALGO TRADING\SP500 INDEX\Data\Macro\raw\exchange_rate\PHP_ZAR.csv</v>
+      </c>
+      <c r="Q120" s="3" t="str">
+        <f>Hoja2!$C$2&amp;B120&amp;"/"&amp;A120&amp;".csv"</f>
+        <v>/mnt/c/Users/pedro/OneDrive/Documents/ALGO TRADING/SP500 INDEX/Data/Macro/raw/exchange_rate/PHP_ZAR.csv</v>
+      </c>
+      <c r="R120" s="3"/>
+      <c r="S120" s="3" t="s">
+        <v>604</v>
+      </c>
+      <c r="T120" s="3" t="s">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="121" spans="1:20">
+      <c r="G121" s="48"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:Q89" xr:uid="{9CB0844A-40A1-4264-8968-9E5B325C5351}"/>
@@ -8094,8 +9753,61 @@
     <hyperlink ref="L93" r:id="rId100" xr:uid="{CF992DDA-3871-4DF0-A0A0-273E4A564931}"/>
     <hyperlink ref="L94" r:id="rId101" xr:uid="{27E0434D-4BA2-4343-80A9-7D55242EE307}"/>
     <hyperlink ref="L95" r:id="rId102" xr:uid="{77714CE7-D72A-44AE-8092-82C467917C5B}"/>
+    <hyperlink ref="L96" r:id="rId103" xr:uid="{05E99B5D-8CBF-42E4-97A4-BD3FF8CAA775}"/>
+    <hyperlink ref="L97" r:id="rId104" xr:uid="{4E95364D-2CA2-4360-AA5E-F1906FF07962}"/>
+    <hyperlink ref="L98" r:id="rId105" xr:uid="{D47AC000-2E34-483E-B88B-86274DC4BFDB}"/>
+    <hyperlink ref="L99" r:id="rId106" xr:uid="{ED11F257-5B86-46A0-9E4F-616EAF0CFA7B}"/>
+    <hyperlink ref="L100" r:id="rId107" xr:uid="{4DCAEA53-9B3F-4CAA-B339-27C4B11D3201}"/>
+    <hyperlink ref="L107" r:id="rId108" xr:uid="{C33A7208-5892-46D5-BAA9-74A740BF4B86}"/>
+    <hyperlink ref="L109" r:id="rId109" xr:uid="{A42BABC0-7931-44F4-A571-76FFA565542E}"/>
+    <hyperlink ref="L110" r:id="rId110" xr:uid="{36D12388-8C9E-4008-819B-EEDD81EBBCBB}"/>
+    <hyperlink ref="L111" r:id="rId111" xr:uid="{CF2A9C23-89FC-43E8-83B3-B1A4E6438DC2}"/>
+    <hyperlink ref="L112" r:id="rId112" xr:uid="{30B578EC-DD56-4CAD-87FF-5762F6B9CB48}"/>
+    <hyperlink ref="L105" r:id="rId113" xr:uid="{8996123D-7FE6-4193-85A3-4B90B98038F0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId103"/>
+  <pageSetup orientation="portrait" r:id="rId114"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36E36D80-2C8E-4B39-8FE3-62C2B2225939}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="21.6640625" customWidth="1"/>
+    <col min="2" max="2" width="71.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="121" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>713</v>
+      </c>
+      <c r="B1" t="s">
+        <v>722</v>
+      </c>
+      <c r="C1" t="s">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>714</v>
+      </c>
+      <c r="B2" t="s">
+        <v>715</v>
+      </c>
+      <c r="C2" t="s">
+        <v>723</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Se actualiza Data Enginnering
</commit_message>
<xml_diff>
--- a/pipelines/Data Engineering.xlsx
+++ b/pipelines/Data Engineering.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\natus\Documents\Trabajo\PEDRO_PEREZ\Proyecto_Mercado_de_Valores\SP500_INDEX_Analisis\pipelines\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AB75324-88DA-4BC4-81F4-14E7D7A04927}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0279DC5A-8787-410A-90F1-6476F399F56B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{AF709C27-429E-478E-9AB0-B8CF25FE9941}"/>
   </bookViews>
@@ -2839,7 +2839,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CB0844A-40A1-4264-8968-9E5B325C5351}">
   <dimension ref="A1:T121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A94" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A97" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="C116" sqref="C116:C120"/>
     </sheetView>
   </sheetViews>
@@ -4121,7 +4121,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="23" spans="1:20" ht="15">
+    <row r="23" spans="1:20">
       <c r="A23" s="12" t="s">
         <v>262</v>
       </c>
@@ -4173,7 +4173,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="24" spans="1:20" ht="15">
+    <row r="24" spans="1:20">
       <c r="A24" s="12" t="s">
         <v>264</v>
       </c>
@@ -4225,7 +4225,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="25" spans="1:20" ht="15">
+    <row r="25" spans="1:20">
       <c r="A25" s="12" t="s">
         <v>260</v>
       </c>
@@ -5943,7 +5943,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="56" spans="1:20" ht="15">
+    <row r="56" spans="1:20">
       <c r="A56" s="12" t="s">
         <v>159</v>
       </c>
@@ -6615,7 +6615,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="68" spans="1:20" ht="15">
+    <row r="68" spans="1:20">
       <c r="A68" s="12" t="s">
         <v>55</v>
       </c>
@@ -6671,7 +6671,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="69" spans="1:20" ht="15">
+    <row r="69" spans="1:20">
       <c r="A69" s="12" t="s">
         <v>148</v>
       </c>
@@ -6727,7 +6727,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="70" spans="1:20" ht="15">
+    <row r="70" spans="1:20">
       <c r="A70" s="12" t="s">
         <v>151</v>
       </c>
@@ -7399,7 +7399,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="82" spans="1:20" ht="30">
+    <row r="82" spans="1:20" ht="26.4">
       <c r="A82" s="12" t="s">
         <v>196</v>
       </c>
@@ -7511,7 +7511,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="84" spans="1:20" ht="15">
+    <row r="84" spans="1:20">
       <c r="A84" s="12" t="s">
         <v>108</v>
       </c>
@@ -7735,7 +7735,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="88" spans="1:20" ht="30">
+    <row r="88" spans="1:20" ht="26.4">
       <c r="A88" s="12" t="s">
         <v>121</v>
       </c>
@@ -7791,7 +7791,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="89" spans="1:20" ht="30">
+    <row r="89" spans="1:20" ht="28.8">
       <c r="A89" s="12" t="s">
         <v>123</v>
       </c>

</xml_diff>

<commit_message>
Se actualiza Data Enginnering y Mercado (brent)
</commit_message>
<xml_diff>
--- a/pipelines/Data Engineering.xlsx
+++ b/pipelines/Data Engineering.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\natus\Documents\Trabajo\PEDRO_PEREZ\Proyecto_Mercado_de_Valores\SP500_INDEX_Analisis\pipelines\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0279DC5A-8787-410A-90F1-6476F399F56B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78B45F88-42EC-4A63-BE4F-26D9B6D9BE85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{AF709C27-429E-478E-9AB0-B8CF25FE9941}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1852" uniqueCount="724">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1862" uniqueCount="726">
   <si>
     <t>Variable</t>
   </si>
@@ -2234,6 +2234,12 @@
   </si>
   <si>
     <t>/mnt/c/Users/pedro/OneDrive/Documents/ALGO TRADING/SP500 INDEX/Data/Macro/raw/</t>
+  </si>
+  <si>
+    <t>Brent_Oil_Futures</t>
+  </si>
+  <si>
+    <t>https://www.investing.com/commodities/brent-oil-historical-data</t>
   </si>
 </sst>
 </file>
@@ -2837,10 +2843,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CB0844A-40A1-4264-8968-9E5B325C5351}">
-  <dimension ref="A1:T121"/>
+  <dimension ref="A1:T122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A97" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C116" sqref="C116:C120"/>
+    <sheetView tabSelected="1" topLeftCell="A92" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="T112" sqref="T112:T113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="37.5546875" defaultRowHeight="14.4"/>
@@ -8292,7 +8298,7 @@
         <v>Data/Macro/raw/commodities</v>
       </c>
       <c r="O97" s="3" t="str">
-        <f t="shared" ref="O97:O120" si="0">N97&amp;"/"&amp;A97&amp;".csv"</f>
+        <f t="shared" ref="O97:O121" si="0">N97&amp;"/"&amp;A97&amp;".csv"</f>
         <v>Data/Macro/raw/commodities/Lumber_Futures.csv</v>
       </c>
       <c r="P97" s="3" t="str">
@@ -9182,16 +9188,16 @@
       </c>
     </row>
     <row r="113" spans="1:20">
-      <c r="A113" s="10" t="s">
-        <v>698</v>
-      </c>
-      <c r="B113" s="9" t="s">
-        <v>231</v>
-      </c>
-      <c r="C113" s="10" t="s">
-        <v>170</v>
-      </c>
-      <c r="D113" s="18" t="s">
+      <c r="A113" s="45" t="s">
+        <v>724</v>
+      </c>
+      <c r="B113" s="46" t="s">
+        <v>230</v>
+      </c>
+      <c r="C113" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="D113" s="47" t="s">
         <v>224</v>
       </c>
       <c r="E113" s="45" t="s">
@@ -9203,33 +9209,33 @@
       <c r="G113" s="48" t="s">
         <v>276</v>
       </c>
-      <c r="H113" s="43">
+      <c r="H113" s="15">
         <v>41640</v>
       </c>
       <c r="I113" s="44">
-        <v>45793</v>
-      </c>
-      <c r="J113" s="3"/>
-      <c r="K113" s="3"/>
-      <c r="L113" s="3" t="s">
-        <v>701</v>
+        <v>45796</v>
+      </c>
+      <c r="J113" s="48"/>
+      <c r="K113" s="48"/>
+      <c r="L113" s="17" t="s">
+        <v>725</v>
       </c>
       <c r="M113" s="3"/>
       <c r="N113" s="3" t="str">
         <f>Hoja2!$A$2&amp;""&amp;B113</f>
-        <v>Data/Macro/raw/index_pricing</v>
+        <v>Data/Macro/raw/commodities</v>
       </c>
       <c r="O113" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>Data/Macro/raw/index_pricing/Dow_Jones_Industrial_Average.csv</v>
+        <v>Data/Macro/raw/commodities/Brent_Oil_Futures.csv</v>
       </c>
       <c r="P113" s="3" t="str">
         <f>Hoja2!$B$2&amp;B113&amp;"\"&amp;A113&amp;".csv"</f>
-        <v>C:\Users\pedro\OneDrive\Documents\ALGO TRADING\SP500 INDEX\Data\Macro\raw\index_pricing\Dow_Jones_Industrial_Average.csv</v>
+        <v>C:\Users\pedro\OneDrive\Documents\ALGO TRADING\SP500 INDEX\Data\Macro\raw\commodities\Brent_Oil_Futures.csv</v>
       </c>
       <c r="Q113" s="3" t="str">
         <f>Hoja2!$C$2&amp;B113&amp;"/"&amp;A113&amp;".csv"</f>
-        <v>/mnt/c/Users/pedro/OneDrive/Documents/ALGO TRADING/SP500 INDEX/Data/Macro/raw/index_pricing/Dow_Jones_Industrial_Average.csv</v>
+        <v>/mnt/c/Users/pedro/OneDrive/Documents/ALGO TRADING/SP500 INDEX/Data/Macro/raw/commodities/Brent_Oil_Futures.csv</v>
       </c>
       <c r="R113" s="3"/>
       <c r="S113" s="3" t="s">
@@ -9241,7 +9247,7 @@
     </row>
     <row r="114" spans="1:20">
       <c r="A114" s="10" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="B114" s="9" t="s">
         <v>231</v>
@@ -9261,7 +9267,7 @@
       <c r="G114" s="48" t="s">
         <v>276</v>
       </c>
-      <c r="H114" s="15">
+      <c r="H114" s="43">
         <v>41640</v>
       </c>
       <c r="I114" s="44">
@@ -9270,7 +9276,7 @@
       <c r="J114" s="3"/>
       <c r="K114" s="3"/>
       <c r="L114" s="3" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="M114" s="3"/>
       <c r="N114" s="3" t="str">
@@ -9279,15 +9285,15 @@
       </c>
       <c r="O114" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>Data/Macro/raw/index_pricing/Nasdaq_100_Fi.csv</v>
+        <v>Data/Macro/raw/index_pricing/Dow_Jones_Industrial_Average.csv</v>
       </c>
       <c r="P114" s="3" t="str">
         <f>Hoja2!$B$2&amp;B114&amp;"\"&amp;A114&amp;".csv"</f>
-        <v>C:\Users\pedro\OneDrive\Documents\ALGO TRADING\SP500 INDEX\Data\Macro\raw\index_pricing\Nasdaq_100_Fi.csv</v>
+        <v>C:\Users\pedro\OneDrive\Documents\ALGO TRADING\SP500 INDEX\Data\Macro\raw\index_pricing\Dow_Jones_Industrial_Average.csv</v>
       </c>
       <c r="Q114" s="3" t="str">
         <f>Hoja2!$C$2&amp;B114&amp;"/"&amp;A114&amp;".csv"</f>
-        <v>/mnt/c/Users/pedro/OneDrive/Documents/ALGO TRADING/SP500 INDEX/Data/Macro/raw/index_pricing/Nasdaq_100_Fi.csv</v>
+        <v>/mnt/c/Users/pedro/OneDrive/Documents/ALGO TRADING/SP500 INDEX/Data/Macro/raw/index_pricing/Dow_Jones_Industrial_Average.csv</v>
       </c>
       <c r="R114" s="3"/>
       <c r="S114" s="3" t="s">
@@ -9299,7 +9305,7 @@
     </row>
     <row r="115" spans="1:20">
       <c r="A115" s="10" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="B115" s="9" t="s">
         <v>231</v>
@@ -9319,7 +9325,7 @@
       <c r="G115" s="48" t="s">
         <v>276</v>
       </c>
-      <c r="H115" s="49">
+      <c r="H115" s="15">
         <v>41640</v>
       </c>
       <c r="I115" s="44">
@@ -9328,7 +9334,7 @@
       <c r="J115" s="3"/>
       <c r="K115" s="3"/>
       <c r="L115" s="3" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="M115" s="3"/>
       <c r="N115" s="3" t="str">
@@ -9337,15 +9343,15 @@
       </c>
       <c r="O115" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>Data/Macro/raw/index_pricing/CAC_40.csv</v>
+        <v>Data/Macro/raw/index_pricing/Nasdaq_100_Fi.csv</v>
       </c>
       <c r="P115" s="3" t="str">
         <f>Hoja2!$B$2&amp;B115&amp;"\"&amp;A115&amp;".csv"</f>
-        <v>C:\Users\pedro\OneDrive\Documents\ALGO TRADING\SP500 INDEX\Data\Macro\raw\index_pricing\CAC_40.csv</v>
+        <v>C:\Users\pedro\OneDrive\Documents\ALGO TRADING\SP500 INDEX\Data\Macro\raw\index_pricing\Nasdaq_100_Fi.csv</v>
       </c>
       <c r="Q115" s="3" t="str">
         <f>Hoja2!$C$2&amp;B115&amp;"/"&amp;A115&amp;".csv"</f>
-        <v>/mnt/c/Users/pedro/OneDrive/Documents/ALGO TRADING/SP500 INDEX/Data/Macro/raw/index_pricing/CAC_40.csv</v>
+        <v>/mnt/c/Users/pedro/OneDrive/Documents/ALGO TRADING/SP500 INDEX/Data/Macro/raw/index_pricing/Nasdaq_100_Fi.csv</v>
       </c>
       <c r="R115" s="3"/>
       <c r="S115" s="3" t="s">
@@ -9357,13 +9363,13 @@
     </row>
     <row r="116" spans="1:20">
       <c r="A116" s="10" t="s">
-        <v>704</v>
-      </c>
-      <c r="B116" s="10" t="s">
-        <v>229</v>
+        <v>700</v>
+      </c>
+      <c r="B116" s="9" t="s">
+        <v>231</v>
       </c>
       <c r="C116" s="10" t="s">
-        <v>54</v>
+        <v>170</v>
       </c>
       <c r="D116" s="18" t="s">
         <v>224</v>
@@ -9377,7 +9383,7 @@
       <c r="G116" s="48" t="s">
         <v>276</v>
       </c>
-      <c r="H116" s="43">
+      <c r="H116" s="49">
         <v>41640</v>
       </c>
       <c r="I116" s="44">
@@ -9386,24 +9392,24 @@
       <c r="J116" s="3"/>
       <c r="K116" s="3"/>
       <c r="L116" s="3" t="s">
-        <v>708</v>
+        <v>703</v>
       </c>
       <c r="M116" s="3"/>
       <c r="N116" s="3" t="str">
         <f>Hoja2!$A$2&amp;""&amp;B116</f>
-        <v>Data/Macro/raw/exchange_rate</v>
+        <v>Data/Macro/raw/index_pricing</v>
       </c>
       <c r="O116" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>Data/Macro/raw/exchange_rate/JPY_EUR.csv</v>
+        <v>Data/Macro/raw/index_pricing/CAC_40.csv</v>
       </c>
       <c r="P116" s="3" t="str">
         <f>Hoja2!$B$2&amp;B116&amp;"\"&amp;A116&amp;".csv"</f>
-        <v>C:\Users\pedro\OneDrive\Documents\ALGO TRADING\SP500 INDEX\Data\Macro\raw\exchange_rate\JPY_EUR.csv</v>
+        <v>C:\Users\pedro\OneDrive\Documents\ALGO TRADING\SP500 INDEX\Data\Macro\raw\index_pricing\CAC_40.csv</v>
       </c>
       <c r="Q116" s="3" t="str">
         <f>Hoja2!$C$2&amp;B116&amp;"/"&amp;A116&amp;".csv"</f>
-        <v>/mnt/c/Users/pedro/OneDrive/Documents/ALGO TRADING/SP500 INDEX/Data/Macro/raw/exchange_rate/JPY_EUR.csv</v>
+        <v>/mnt/c/Users/pedro/OneDrive/Documents/ALGO TRADING/SP500 INDEX/Data/Macro/raw/index_pricing/CAC_40.csv</v>
       </c>
       <c r="R116" s="3"/>
       <c r="S116" s="3" t="s">
@@ -9435,7 +9441,7 @@
       <c r="G117" s="48" t="s">
         <v>276</v>
       </c>
-      <c r="H117" s="15">
+      <c r="H117" s="43">
         <v>41640</v>
       </c>
       <c r="I117" s="44">
@@ -9444,7 +9450,7 @@
       <c r="J117" s="3"/>
       <c r="K117" s="3"/>
       <c r="L117" s="3" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="M117" s="3"/>
       <c r="N117" s="3" t="str">
@@ -9473,7 +9479,7 @@
     </row>
     <row r="118" spans="1:20">
       <c r="A118" s="10" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="B118" s="10" t="s">
         <v>229</v>
@@ -9493,7 +9499,7 @@
       <c r="G118" s="48" t="s">
         <v>276</v>
       </c>
-      <c r="H118" s="49">
+      <c r="H118" s="15">
         <v>41640</v>
       </c>
       <c r="I118" s="44">
@@ -9502,7 +9508,7 @@
       <c r="J118" s="3"/>
       <c r="K118" s="3"/>
       <c r="L118" s="3" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="M118" s="3"/>
       <c r="N118" s="3" t="str">
@@ -9511,15 +9517,15 @@
       </c>
       <c r="O118" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>Data/Macro/raw/exchange_rate/BRL_NZD.csv</v>
+        <v>Data/Macro/raw/exchange_rate/JPY_EUR.csv</v>
       </c>
       <c r="P118" s="3" t="str">
         <f>Hoja2!$B$2&amp;B118&amp;"\"&amp;A118&amp;".csv"</f>
-        <v>C:\Users\pedro\OneDrive\Documents\ALGO TRADING\SP500 INDEX\Data\Macro\raw\exchange_rate\BRL_NZD.csv</v>
+        <v>C:\Users\pedro\OneDrive\Documents\ALGO TRADING\SP500 INDEX\Data\Macro\raw\exchange_rate\JPY_EUR.csv</v>
       </c>
       <c r="Q118" s="3" t="str">
         <f>Hoja2!$C$2&amp;B118&amp;"/"&amp;A118&amp;".csv"</f>
-        <v>/mnt/c/Users/pedro/OneDrive/Documents/ALGO TRADING/SP500 INDEX/Data/Macro/raw/exchange_rate/BRL_NZD.csv</v>
+        <v>/mnt/c/Users/pedro/OneDrive/Documents/ALGO TRADING/SP500 INDEX/Data/Macro/raw/exchange_rate/JPY_EUR.csv</v>
       </c>
       <c r="R118" s="3"/>
       <c r="S118" s="3" t="s">
@@ -9531,7 +9537,7 @@
     </row>
     <row r="119" spans="1:20">
       <c r="A119" s="10" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="B119" s="10" t="s">
         <v>229</v>
@@ -9551,7 +9557,7 @@
       <c r="G119" s="48" t="s">
         <v>276</v>
       </c>
-      <c r="H119" s="43">
+      <c r="H119" s="49">
         <v>41640</v>
       </c>
       <c r="I119" s="44">
@@ -9560,7 +9566,7 @@
       <c r="J119" s="3"/>
       <c r="K119" s="3"/>
       <c r="L119" s="3" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="M119" s="3"/>
       <c r="N119" s="3" t="str">
@@ -9569,15 +9575,15 @@
       </c>
       <c r="O119" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>Data/Macro/raw/exchange_rate/NOK_AUD.csv</v>
+        <v>Data/Macro/raw/exchange_rate/BRL_NZD.csv</v>
       </c>
       <c r="P119" s="3" t="str">
         <f>Hoja2!$B$2&amp;B119&amp;"\"&amp;A119&amp;".csv"</f>
-        <v>C:\Users\pedro\OneDrive\Documents\ALGO TRADING\SP500 INDEX\Data\Macro\raw\exchange_rate\NOK_AUD.csv</v>
+        <v>C:\Users\pedro\OneDrive\Documents\ALGO TRADING\SP500 INDEX\Data\Macro\raw\exchange_rate\BRL_NZD.csv</v>
       </c>
       <c r="Q119" s="3" t="str">
         <f>Hoja2!$C$2&amp;B119&amp;"/"&amp;A119&amp;".csv"</f>
-        <v>/mnt/c/Users/pedro/OneDrive/Documents/ALGO TRADING/SP500 INDEX/Data/Macro/raw/exchange_rate/NOK_AUD.csv</v>
+        <v>/mnt/c/Users/pedro/OneDrive/Documents/ALGO TRADING/SP500 INDEX/Data/Macro/raw/exchange_rate/BRL_NZD.csv</v>
       </c>
       <c r="R119" s="3"/>
       <c r="S119" s="3" t="s">
@@ -9589,7 +9595,7 @@
     </row>
     <row r="120" spans="1:20">
       <c r="A120" s="10" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="B120" s="10" t="s">
         <v>229</v>
@@ -9600,16 +9606,16 @@
       <c r="D120" s="18" t="s">
         <v>224</v>
       </c>
-      <c r="E120" s="10" t="s">
+      <c r="E120" s="45" t="s">
         <v>245</v>
       </c>
-      <c r="F120" s="10" t="s">
+      <c r="F120" s="45" t="s">
         <v>246</v>
       </c>
       <c r="G120" s="48" t="s">
         <v>276</v>
       </c>
-      <c r="H120" s="15">
+      <c r="H120" s="43">
         <v>41640</v>
       </c>
       <c r="I120" s="44">
@@ -9618,7 +9624,7 @@
       <c r="J120" s="3"/>
       <c r="K120" s="3"/>
       <c r="L120" s="3" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="M120" s="3"/>
       <c r="N120" s="3" t="str">
@@ -9627,15 +9633,15 @@
       </c>
       <c r="O120" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>Data/Macro/raw/exchange_rate/PHP_ZAR.csv</v>
+        <v>Data/Macro/raw/exchange_rate/NOK_AUD.csv</v>
       </c>
       <c r="P120" s="3" t="str">
         <f>Hoja2!$B$2&amp;B120&amp;"\"&amp;A120&amp;".csv"</f>
-        <v>C:\Users\pedro\OneDrive\Documents\ALGO TRADING\SP500 INDEX\Data\Macro\raw\exchange_rate\PHP_ZAR.csv</v>
+        <v>C:\Users\pedro\OneDrive\Documents\ALGO TRADING\SP500 INDEX\Data\Macro\raw\exchange_rate\NOK_AUD.csv</v>
       </c>
       <c r="Q120" s="3" t="str">
         <f>Hoja2!$C$2&amp;B120&amp;"/"&amp;A120&amp;".csv"</f>
-        <v>/mnt/c/Users/pedro/OneDrive/Documents/ALGO TRADING/SP500 INDEX/Data/Macro/raw/exchange_rate/PHP_ZAR.csv</v>
+        <v>/mnt/c/Users/pedro/OneDrive/Documents/ALGO TRADING/SP500 INDEX/Data/Macro/raw/exchange_rate/NOK_AUD.csv</v>
       </c>
       <c r="R120" s="3"/>
       <c r="S120" s="3" t="s">
@@ -9646,7 +9652,65 @@
       </c>
     </row>
     <row r="121" spans="1:20">
-      <c r="G121" s="48"/>
+      <c r="A121" s="10" t="s">
+        <v>707</v>
+      </c>
+      <c r="B121" s="10" t="s">
+        <v>229</v>
+      </c>
+      <c r="C121" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="D121" s="18" t="s">
+        <v>224</v>
+      </c>
+      <c r="E121" s="10" t="s">
+        <v>245</v>
+      </c>
+      <c r="F121" s="10" t="s">
+        <v>246</v>
+      </c>
+      <c r="G121" s="48" t="s">
+        <v>276</v>
+      </c>
+      <c r="H121" s="15">
+        <v>41640</v>
+      </c>
+      <c r="I121" s="44">
+        <v>45793</v>
+      </c>
+      <c r="J121" s="3"/>
+      <c r="K121" s="3"/>
+      <c r="L121" s="3" t="s">
+        <v>712</v>
+      </c>
+      <c r="M121" s="3"/>
+      <c r="N121" s="3" t="str">
+        <f>Hoja2!$A$2&amp;""&amp;B121</f>
+        <v>Data/Macro/raw/exchange_rate</v>
+      </c>
+      <c r="O121" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>Data/Macro/raw/exchange_rate/PHP_ZAR.csv</v>
+      </c>
+      <c r="P121" s="3" t="str">
+        <f>Hoja2!$B$2&amp;B121&amp;"\"&amp;A121&amp;".csv"</f>
+        <v>C:\Users\pedro\OneDrive\Documents\ALGO TRADING\SP500 INDEX\Data\Macro\raw\exchange_rate\PHP_ZAR.csv</v>
+      </c>
+      <c r="Q121" s="3" t="str">
+        <f>Hoja2!$C$2&amp;B121&amp;"/"&amp;A121&amp;".csv"</f>
+        <v>/mnt/c/Users/pedro/OneDrive/Documents/ALGO TRADING/SP500 INDEX/Data/Macro/raw/exchange_rate/PHP_ZAR.csv</v>
+      </c>
+      <c r="R121" s="3"/>
+      <c r="S121" s="3" t="s">
+        <v>604</v>
+      </c>
+      <c r="T121" s="3" t="s">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="122" spans="1:20">
+      <c r="G122" s="48"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:Q89" xr:uid="{9CB0844A-40A1-4264-8968-9E5B325C5351}"/>
@@ -9764,9 +9828,10 @@
     <hyperlink ref="L111" r:id="rId111" xr:uid="{CF2A9C23-89FC-43E8-83B3-B1A4E6438DC2}"/>
     <hyperlink ref="L112" r:id="rId112" xr:uid="{30B578EC-DD56-4CAD-87FF-5762F6B9CB48}"/>
     <hyperlink ref="L105" r:id="rId113" xr:uid="{8996123D-7FE6-4193-85A3-4B90B98038F0}"/>
+    <hyperlink ref="L113" r:id="rId114" xr:uid="{07203FF3-AFB1-4C54-8E01-B1FE16CF9927}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId114"/>
+  <pageSetup orientation="portrait" r:id="rId115"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Se agrego en el step_0, para que pase el archivo del DANE de exportaciones.
En el step_1 se hizo forward filling para llenar los datos faltantes del DANE
</commit_message>
<xml_diff>
--- a/pipelines/Data Engineering.xlsx
+++ b/pipelines/Data Engineering.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\saule\Desktop\Pipeline\UltimoHadid.exe\SP500_INDEX_Analisis\pipelines\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\saule\Desktop\Pipeline\UltimoHadidMayo\SP500_INDEX_Analisis\pipelines\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C36091D3-B5F8-4CE2-8345-533E2F4CE15E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E65B6CE2-42BA-41F3-B7EB-083B1106699D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{AF709C27-429E-478E-9AB0-B8CF25FE9941}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{AF709C27-429E-478E-9AB0-B8CF25FE9941}"/>
   </bookViews>
   <sheets>
     <sheet name="Macro" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2047" uniqueCount="720">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2054" uniqueCount="721">
   <si>
     <t>Variable</t>
   </si>
@@ -2213,6 +2213,9 @@
   </si>
   <si>
     <t>Tasas de cambio</t>
+  </si>
+  <si>
+    <t>anex-EXPORTACIONES-SerieCafeCarbonPetroleoNotradicionales-mar2025</t>
   </si>
 </sst>
 </file>
@@ -2379,7 +2382,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2511,6 +2514,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -2848,8 +2854,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CB0844A-40A1-4264-8968-9E5B325C5351}">
   <dimension ref="A1:T121"/>
   <sheetViews>
-    <sheetView topLeftCell="N88" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="O89" sqref="O89"/>
+    <sheetView tabSelected="1" topLeftCell="L98" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="O118" sqref="O118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="37.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8242,7 +8248,7 @@
         <v>412</v>
       </c>
       <c r="O96" s="3" t="str">
-        <f t="shared" ref="O96:O118" si="0">N96&amp;"/"&amp;A96&amp;".csv"</f>
+        <f t="shared" ref="O96:O116" si="0">N96&amp;"/"&amp;A96&amp;".csv"</f>
         <v>Data/Macro/raw/commodities/Iron_ore_fines_62%_Fe_CFR_Futures.csv</v>
       </c>
       <c r="P96" s="3" t="e">
@@ -9442,18 +9448,30 @@
       <c r="T118" s="3"/>
     </row>
     <row r="119" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A119"/>
-      <c r="B119"/>
-      <c r="C119"/>
-      <c r="D119"/>
-      <c r="E119"/>
-      <c r="N119" s="54" t="e">
-        <f>USDCOP!#REF!&amp;""&amp;USDCOP!B116</f>
-        <v>#REF!</v>
-      </c>
-      <c r="O119" s="54" t="e">
-        <f>N119&amp;"/"&amp;USDCOP!A116&amp;".xlsx"</f>
-        <v>#REF!</v>
+      <c r="A119" t="s">
+        <v>720</v>
+      </c>
+      <c r="B119" s="55" t="s">
+        <v>237</v>
+      </c>
+      <c r="C119" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="D119" s="35" t="s">
+        <v>322</v>
+      </c>
+      <c r="E119" s="55" t="s">
+        <v>247</v>
+      </c>
+      <c r="M119" s="55" t="s">
+        <v>237</v>
+      </c>
+      <c r="N119" s="48" t="s">
+        <v>530</v>
+      </c>
+      <c r="O119" s="3" t="str">
+        <f>N119&amp;"/"&amp;A119&amp;".xlsx"</f>
+        <v>Data/Macro/raw/exports/anex-EXPORTACIONES-SerieCafeCarbonPetroleoNotradicionales-mar2025.xlsx</v>
       </c>
       <c r="P119" s="54" t="e">
         <f>USDCOP!#REF!&amp;USDCOP!B116&amp;"\"&amp;USDCOP!A116&amp;".csv"</f>
@@ -10377,7 +10395,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4DCAF4E-6D9B-426F-A656-83ECEF1F0C9A}">
   <dimension ref="A1:T51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+    <sheetView topLeftCell="A25" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Se creo Step_0_preprocess2, lee y transforma actualmente 17 nuevos datos
</commit_message>
<xml_diff>
--- a/pipelines/Data Engineering.xlsx
+++ b/pipelines/Data Engineering.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\saule\Desktop\Pipeline\UltimoHadidMayo\SP500_INDEX_Analisis\pipelines\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E65B6CE2-42BA-41F3-B7EB-083B1106699D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68A21060-284D-42BF-A401-7E17EEC9FF0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{AF709C27-429E-478E-9AB0-B8CF25FE9941}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2054" uniqueCount="721">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2063" uniqueCount="723">
   <si>
     <t>Variable</t>
   </si>
@@ -2216,6 +2216,12 @@
   </si>
   <si>
     <t>anex-EXPORTACIONES-SerieCafeCarbonPetroleoNotradicionales-mar2025</t>
+  </si>
+  <si>
+    <t>TasasTES_Bond</t>
+  </si>
+  <si>
+    <t>Data/Macro/raw/bond/TasasTES_Bond</t>
   </si>
 </sst>
 </file>
@@ -2382,7 +2388,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2514,7 +2520,13 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2854,8 +2866,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CB0844A-40A1-4264-8968-9E5B325C5351}">
   <dimension ref="A1:T121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L98" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="O118" sqref="O118"/>
+    <sheetView tabSelected="1" topLeftCell="M98" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="O120" sqref="O120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="37.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9463,15 +9475,18 @@
       <c r="E119" s="55" t="s">
         <v>247</v>
       </c>
+      <c r="F119" s="10" t="s">
+        <v>246</v>
+      </c>
       <c r="M119" s="55" t="s">
         <v>237</v>
       </c>
       <c r="N119" s="48" t="s">
-        <v>530</v>
+        <v>327</v>
       </c>
       <c r="O119" s="3" t="str">
         <f>N119&amp;"/"&amp;A119&amp;".xlsx"</f>
-        <v>Data/Macro/raw/exports/anex-EXPORTACIONES-SerieCafeCarbonPetroleoNotradicionales-mar2025.xlsx</v>
+        <v>Data/Macro/raw/bond/anex-EXPORTACIONES-SerieCafeCarbonPetroleoNotradicionales-mar2025.xlsx</v>
       </c>
       <c r="P119" s="54" t="e">
         <f>USDCOP!#REF!&amp;USDCOP!B116&amp;"\"&amp;USDCOP!A116&amp;".csv"</f>
@@ -9486,18 +9501,30 @@
       </c>
     </row>
     <row r="120" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A120"/>
-      <c r="B120"/>
-      <c r="C120"/>
-      <c r="D120"/>
+      <c r="A120" t="s">
+        <v>721</v>
+      </c>
+      <c r="B120" s="56" t="s">
+        <v>228</v>
+      </c>
+      <c r="C120" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D120" s="57" t="s">
+        <v>322</v>
+      </c>
       <c r="E120"/>
-      <c r="N120" s="3" t="e">
-        <f>USDCOP!#REF!&amp;""&amp;USDCOP!#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="O120" s="3" t="e">
-        <f>N120&amp;"/"&amp;USDCOP!#REF!&amp;".xlsx"</f>
-        <v>#REF!</v>
+      <c r="F120" s="10" t="s">
+        <v>246</v>
+      </c>
+      <c r="M120" t="s">
+        <v>721</v>
+      </c>
+      <c r="N120" s="48" t="s">
+        <v>327</v>
+      </c>
+      <c r="O120" s="48" t="s">
+        <v>722</v>
       </c>
       <c r="P120" s="3" t="e">
         <f>USDCOP!#REF!&amp;USDCOP!#REF!&amp;"\"&amp;USDCOP!#REF!&amp;".csv"</f>

</xml_diff>